<commit_message>
[Doc]_HuyenPT_Commit file doc back-up
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -13,8 +13,8 @@
     <sheet name="TỔNG HỢP" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CODING!$H$5:$H$73</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">CODING!$A$5:$M$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CODING!$H$5:$H$74</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">CODING!$A$5:$M$72</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">DESIGN!#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621" refMode="R1C1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="195">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -620,6 +620,12 @@
   </si>
   <si>
     <t>TEST CASE:</t>
+  </si>
+  <si>
+    <t>Add new Category</t>
+  </si>
+  <si>
+    <t>Thêm thể loại sách</t>
   </si>
 </sst>
 </file>
@@ -955,152 +961,152 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1408,7 +1414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N73"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -1430,10 +1436,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="G1" s="59" t="s">
+      <c r="G1" s="44" t="s">
         <v>119</v>
       </c>
       <c r="H1" s="10"/>
@@ -1443,10 +1449,10 @@
       <c r="N1" s="20"/>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="44" t="s">
         <v>120</v>
       </c>
       <c r="H2" s="10"/>
@@ -1456,10 +1462,10 @@
       <c r="N2" s="20"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="44" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1499,12 +1505,12 @@
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -1514,12 +1520,12 @@
       <c r="N6" s="22"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
@@ -1532,8 +1538,8 @@
       <c r="B8" t="s">
         <v>118</v>
       </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="63" t="s">
+      <c r="D8" s="45"/>
+      <c r="E8" s="66" t="s">
         <v>187</v>
       </c>
       <c r="F8" s="14" t="s">
@@ -1565,8 +1571,8 @@
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D9" s="64"/>
-      <c r="E9" s="65"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="67"/>
       <c r="F9" s="14" t="s">
         <v>8</v>
       </c>
@@ -1597,7 +1603,7 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D10" s="14"/>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="65" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="14" t="s">
@@ -1633,7 +1639,7 @@
         <v>121</v>
       </c>
       <c r="D11" s="14"/>
-      <c r="E11" s="65"/>
+      <c r="E11" s="67"/>
       <c r="F11" s="14" t="s">
         <v>13</v>
       </c>
@@ -1667,10 +1673,10 @@
         <v>120</v>
       </c>
       <c r="D12" s="14"/>
-      <c r="E12" s="66" t="s">
+      <c r="E12" s="65" t="s">
         <v>188</v>
       </c>
-      <c r="F12" s="67" t="s">
+      <c r="F12" s="85" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="14" t="s">
@@ -1699,8 +1705,8 @@
     <row r="13" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="D13" s="14"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="68"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="86"/>
       <c r="G13" s="14" t="s">
         <v>160</v>
       </c>
@@ -1727,7 +1733,7 @@
         <v>119</v>
       </c>
       <c r="D14" s="14"/>
-      <c r="E14" s="65"/>
+      <c r="E14" s="67"/>
       <c r="F14" s="14" t="s">
         <v>17</v>
       </c>
@@ -1753,26 +1759,26 @@
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="71" t="s">
         <v>184</v>
       </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="51"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="73"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="3"/>
       <c r="L15" s="22"/>
       <c r="M15" s="30"/>
-      <c r="N15" s="90"/>
+      <c r="N15" s="57"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D16" s="64"/>
-      <c r="E16" s="66" t="s">
+      <c r="D16" s="46"/>
+      <c r="E16" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="60" t="s">
+      <c r="F16" s="63" t="s">
         <v>183</v>
       </c>
       <c r="G16" s="19" t="s">
@@ -1799,9 +1805,9 @@
       </c>
     </row>
     <row r="17" spans="4:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="70"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="61"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="64"/>
       <c r="G17" s="19" t="s">
         <v>185</v>
       </c>
@@ -1824,8 +1830,8 @@
       </c>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D18" s="66"/>
-      <c r="E18" s="63"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="66"/>
       <c r="F18" s="18" t="s">
         <v>20</v>
       </c>
@@ -1851,8 +1857,8 @@
       </c>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D19" s="65"/>
-      <c r="E19" s="63"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="66"/>
       <c r="F19" s="18" t="s">
         <v>22</v>
       </c>
@@ -1878,8 +1884,8 @@
       </c>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D20" s="64"/>
-      <c r="E20" s="63"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="66"/>
       <c r="F20" s="18" t="s">
         <v>24</v>
       </c>
@@ -1905,8 +1911,8 @@
       </c>
     </row>
     <row r="21" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D21" s="64"/>
-      <c r="E21" s="63"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="66"/>
       <c r="F21" s="18" t="s">
         <v>26</v>
       </c>
@@ -1932,8 +1938,8 @@
       </c>
     </row>
     <row r="22" spans="4:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="64"/>
-      <c r="E22" s="63"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="66"/>
       <c r="F22" s="18" t="s">
         <v>149</v>
       </c>
@@ -1957,8 +1963,8 @@
       </c>
     </row>
     <row r="23" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D23" s="64"/>
-      <c r="E23" s="66" t="s">
+      <c r="D23" s="46"/>
+      <c r="E23" s="65" t="s">
         <v>28</v>
       </c>
       <c r="F23" s="14" t="s">
@@ -1986,8 +1992,8 @@
       </c>
     </row>
     <row r="24" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D24" s="64"/>
-      <c r="E24" s="63"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="66"/>
       <c r="F24" s="14" t="s">
         <v>31</v>
       </c>
@@ -2013,8 +2019,8 @@
       </c>
     </row>
     <row r="25" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D25" s="64"/>
-      <c r="E25" s="63"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="66"/>
       <c r="F25" s="14" t="s">
         <v>33</v>
       </c>
@@ -2040,8 +2046,8 @@
       </c>
     </row>
     <row r="26" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D26" s="64"/>
-      <c r="E26" s="65"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="67"/>
       <c r="F26" s="14" t="s">
         <v>35</v>
       </c>
@@ -2067,8 +2073,8 @@
       </c>
     </row>
     <row r="27" spans="4:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="D27" s="64"/>
-      <c r="E27" s="64" t="s">
+      <c r="D27" s="46"/>
+      <c r="E27" s="46" t="s">
         <v>178</v>
       </c>
       <c r="F27" s="18" t="s">
@@ -2094,23 +2100,23 @@
       <c r="N27" s="23"/>
     </row>
     <row r="28" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D28" s="55" t="s">
+      <c r="D28" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="57"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="79"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="3"/>
       <c r="L28" s="22"/>
       <c r="M28" s="30"/>
-      <c r="N28" s="90"/>
+      <c r="N28" s="57"/>
     </row>
     <row r="29" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D29" s="70"/>
-      <c r="E29" s="71" t="s">
+      <c r="D29" s="48"/>
+      <c r="E29" s="80" t="s">
         <v>38</v>
       </c>
       <c r="F29" s="14" t="s">
@@ -2139,9 +2145,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="4:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="D30" s="70"/>
-      <c r="E30" s="72"/>
+    <row r="30" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D30" s="48"/>
+      <c r="E30" s="81"/>
       <c r="F30" s="19" t="s">
         <v>41</v>
       </c>
@@ -2167,12 +2173,12 @@
       </c>
     </row>
     <row r="31" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D31" s="70"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="69" t="s">
+      <c r="D31" s="48"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="G31" s="69" t="s">
+      <c r="G31" s="47" t="s">
         <v>44</v>
       </c>
       <c r="H31" s="12" t="s">
@@ -2194,14 +2200,14 @@
       </c>
     </row>
     <row r="32" spans="4:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="D32" s="70"/>
-      <c r="E32" s="66" t="s">
+      <c r="D32" s="48"/>
+      <c r="E32" s="65" t="s">
         <v>45</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G32" s="69" t="s">
+      <c r="G32" s="47" t="s">
         <v>47</v>
       </c>
       <c r="H32" s="12" t="s">
@@ -2225,8 +2231,8 @@
       </c>
     </row>
     <row r="33" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D33" s="70"/>
-      <c r="E33" s="63"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="66"/>
       <c r="F33" s="14" t="s">
         <v>48</v>
       </c>
@@ -2254,8 +2260,8 @@
       </c>
     </row>
     <row r="34" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D34" s="70"/>
-      <c r="E34" s="65"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="67"/>
       <c r="F34" s="14" t="s">
         <v>50</v>
       </c>
@@ -2281,29 +2287,29 @@
       </c>
     </row>
     <row r="35" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D35" s="52" t="s">
+      <c r="D35" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="54"/>
+      <c r="E35" s="75"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="76"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="13"/>
       <c r="L35" s="22"/>
       <c r="M35" s="30"/>
-      <c r="N35" s="90"/>
+      <c r="N35" s="57"/>
     </row>
     <row r="36" spans="4:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="D36" s="64"/>
-      <c r="E36" s="66" t="s">
+      <c r="D36" s="46"/>
+      <c r="E36" s="65" t="s">
         <v>53</v>
       </c>
       <c r="F36" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G36" s="69" t="s">
+      <c r="G36" s="47" t="s">
         <v>55</v>
       </c>
       <c r="H36" s="12" t="s">
@@ -2327,12 +2333,12 @@
       </c>
     </row>
     <row r="37" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D37" s="64"/>
-      <c r="E37" s="63"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="66"/>
       <c r="F37" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G37" s="69" t="s">
+      <c r="G37" s="47" t="s">
         <v>57</v>
       </c>
       <c r="H37" s="12" t="s">
@@ -2358,14 +2364,14 @@
       </c>
     </row>
     <row r="38" spans="4:14" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="D38" s="64"/>
-      <c r="E38" s="71" t="s">
+      <c r="D38" s="46"/>
+      <c r="E38" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="F38" s="69" t="s">
+      <c r="F38" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="G38" s="69" t="s">
+      <c r="G38" s="47" t="s">
         <v>60</v>
       </c>
       <c r="H38" s="33" t="s">
@@ -2389,12 +2395,12 @@
       </c>
     </row>
     <row r="39" spans="4:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="D39" s="64"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="69" t="s">
+      <c r="D39" s="46"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="G39" s="74" t="s">
+      <c r="G39" s="49" t="s">
         <v>62</v>
       </c>
       <c r="H39" s="12" t="s">
@@ -2418,8 +2424,8 @@
       </c>
     </row>
     <row r="40" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D40" s="64"/>
-      <c r="E40" s="72"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="81"/>
       <c r="F40" s="14" t="s">
         <v>63</v>
       </c>
@@ -2449,8 +2455,8 @@
       </c>
     </row>
     <row r="41" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D41" s="64"/>
-      <c r="E41" s="73"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="82"/>
       <c r="F41" s="14" t="s">
         <v>65</v>
       </c>
@@ -2480,14 +2486,14 @@
       </c>
     </row>
     <row r="42" spans="4:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="D42" s="64"/>
-      <c r="E42" s="66" t="s">
+      <c r="D42" s="46"/>
+      <c r="E42" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="F42" s="75" t="s">
+      <c r="F42" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="G42" s="69" t="s">
+      <c r="G42" s="47" t="s">
         <v>69</v>
       </c>
       <c r="H42" s="12" t="s">
@@ -2507,8 +2513,8 @@
       </c>
     </row>
     <row r="43" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D43" s="64"/>
-      <c r="E43" s="63"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="66"/>
       <c r="F43" s="14" t="s">
         <v>70</v>
       </c>
@@ -2532,8 +2538,8 @@
       </c>
     </row>
     <row r="44" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D44" s="64"/>
-      <c r="E44" s="65"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="67"/>
       <c r="F44" s="14" t="s">
         <v>72</v>
       </c>
@@ -2557,23 +2563,23 @@
       </c>
     </row>
     <row r="45" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D45" s="52" t="s">
+      <c r="D45" s="74" t="s">
         <v>74</v>
       </c>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="54"/>
+      <c r="E45" s="75"/>
+      <c r="F45" s="75"/>
+      <c r="G45" s="76"/>
       <c r="H45" s="12"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
       <c r="K45" s="3"/>
       <c r="L45" s="22"/>
       <c r="M45" s="30"/>
-      <c r="N45" s="90"/>
+      <c r="N45" s="57"/>
     </row>
     <row r="46" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
       <c r="F46" s="14" t="s">
         <v>75</v>
       </c>
@@ -2603,12 +2609,12 @@
       </c>
     </row>
     <row r="47" spans="4:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="D47" s="64"/>
-      <c r="E47" s="64"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
       <c r="F47" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="G47" s="69" t="s">
+      <c r="G47" s="47" t="s">
         <v>163</v>
       </c>
       <c r="H47" s="12"/>
@@ -2624,9 +2630,9 @@
       </c>
     </row>
     <row r="48" spans="4:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D48" s="70"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="58" t="s">
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="43" t="s">
         <v>77</v>
       </c>
       <c r="G48" s="18" t="s">
@@ -2651,12 +2657,12 @@
       </c>
     </row>
     <row r="49" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
       <c r="F49" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="G49" s="69" t="s">
+      <c r="G49" s="47" t="s">
         <v>154</v>
       </c>
       <c r="H49" s="12" t="s">
@@ -2678,23 +2684,23 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D50" s="47" t="s">
+      <c r="D50" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
       <c r="K50" s="3"/>
       <c r="L50" s="22"/>
       <c r="M50" s="30"/>
-      <c r="N50" s="90"/>
+      <c r="N50" s="57"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D51" s="64"/>
-      <c r="E51" s="66" t="s">
+      <c r="D51" s="46"/>
+      <c r="E51" s="65" t="s">
         <v>80</v>
       </c>
       <c r="F51" s="14" t="s">
@@ -2718,8 +2724,8 @@
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D52" s="64"/>
-      <c r="E52" s="63"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="66"/>
       <c r="F52" s="14" t="s">
         <v>82</v>
       </c>
@@ -2743,8 +2749,8 @@
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D53" s="64"/>
-      <c r="E53" s="63"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="66"/>
       <c r="F53" s="14" t="s">
         <v>84</v>
       </c>
@@ -2771,9 +2777,9 @@
       <c r="A54" t="s">
         <v>122</v>
       </c>
-      <c r="D54" s="64"/>
-      <c r="E54" s="63"/>
-      <c r="F54" s="69" t="s">
+      <c r="D54" s="46"/>
+      <c r="E54" s="66"/>
+      <c r="F54" s="47" t="s">
         <v>86</v>
       </c>
       <c r="G54" s="14" t="s">
@@ -2799,12 +2805,12 @@
       <c r="A55" t="s">
         <v>123</v>
       </c>
-      <c r="D55" s="64"/>
-      <c r="E55" s="65"/>
-      <c r="F55" s="69" t="s">
+      <c r="D55" s="46"/>
+      <c r="E55" s="67"/>
+      <c r="F55" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="G55" s="69" t="s">
+      <c r="G55" s="47" t="s">
         <v>89</v>
       </c>
       <c r="H55" s="12" t="s">
@@ -2827,8 +2833,8 @@
       <c r="A56" t="s">
         <v>118</v>
       </c>
-      <c r="D56" s="64"/>
-      <c r="E56" s="66" t="s">
+      <c r="D56" s="46"/>
+      <c r="E56" s="65" t="s">
         <v>90</v>
       </c>
       <c r="F56" s="14" t="s">
@@ -2859,24 +2865,20 @@
         <v>121</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D57" s="64"/>
-      <c r="E57" s="63"/>
+    <row r="57" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D57" s="46"/>
+      <c r="E57" s="66"/>
       <c r="F57" s="14" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
       <c r="G57" s="14" t="s">
-        <v>94</v>
+        <v>194</v>
       </c>
       <c r="H57" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="I57" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="J57" s="12" t="s">
-        <v>131</v>
-      </c>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
       <c r="K57" s="5" t="s">
         <v>119</v>
       </c>
@@ -2886,18 +2888,16 @@
       <c r="M57" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="N57" s="40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="D58" s="64"/>
-      <c r="E58" s="65"/>
-      <c r="F58" s="69" t="s">
-        <v>95</v>
+      <c r="N57" s="40"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D58" s="46"/>
+      <c r="E58" s="66"/>
+      <c r="F58" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="G58" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H58" s="12" t="s">
         <v>123</v>
@@ -2908,69 +2908,69 @@
       <c r="J58" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="K58" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="L58" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="M58" s="4" t="s">
-        <v>121</v>
+      <c r="K58" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L58" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="M58" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="N58" s="40" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D59" s="64"/>
-      <c r="E59" s="66" t="s">
+    <row r="59" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="D59" s="46"/>
+      <c r="E59" s="67"/>
+      <c r="F59" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="G59" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J59" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L59" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M59" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N59" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D60" s="46"/>
+      <c r="E60" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="F59" s="14" t="s">
+      <c r="F60" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="G59" s="14" t="s">
+      <c r="G60" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="H59" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="I59" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="J59" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="K59" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L59" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="M59" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="N59" s="40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D60" s="64"/>
-      <c r="E60" s="63"/>
-      <c r="F60" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="G60" s="14" t="s">
-        <v>101</v>
       </c>
       <c r="H60" s="12" t="s">
         <v>122</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J60" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K60" s="5" t="s">
         <v>119</v>
@@ -2986,21 +2986,25 @@
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D61" s="64"/>
-      <c r="E61" s="63"/>
+      <c r="D61" s="46"/>
+      <c r="E61" s="66"/>
       <c r="F61" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H61" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
-      <c r="K61" s="4" t="s">
-        <v>121</v>
+      <c r="I61" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="J61" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="L61" s="5" t="s">
         <v>119</v>
@@ -3012,24 +3016,26 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D62" s="64"/>
-      <c r="E62" s="63"/>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D62" s="46"/>
+      <c r="E62" s="66"/>
       <c r="F62" s="14" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="H62" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I62" s="12"/>
       <c r="J62" s="12"/>
-      <c r="K62" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L62" s="23"/>
+      <c r="K62" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L62" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="M62" s="5" t="s">
         <v>119</v>
       </c>
@@ -3038,25 +3044,23 @@
       </c>
     </row>
     <row r="63" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D63" s="64"/>
-      <c r="E63" s="65"/>
+      <c r="D63" s="46"/>
+      <c r="E63" s="66"/>
       <c r="F63" s="14" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G63" s="14" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H63" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
-      <c r="K63" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="L63" s="5" t="s">
-        <v>119</v>
-      </c>
+      <c r="K63" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L63" s="23"/>
       <c r="M63" s="5" t="s">
         <v>119</v>
       </c>
@@ -3064,28 +3068,22 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D64" s="64"/>
-      <c r="E64" s="66" t="s">
-        <v>151</v>
-      </c>
+    <row r="64" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D64" s="46"/>
+      <c r="E64" s="67"/>
       <c r="F64" s="14" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="G64" s="14" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="H64" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="I64" s="15">
-        <v>42380</v>
-      </c>
-      <c r="J64" s="15">
-        <v>42411</v>
-      </c>
-      <c r="K64" s="5" t="s">
-        <v>119</v>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="L64" s="5" t="s">
         <v>119</v>
@@ -3098,13 +3096,15 @@
       </c>
     </row>
     <row r="65" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D65" s="64"/>
-      <c r="E65" s="63"/>
+      <c r="D65" s="46"/>
+      <c r="E65" s="65" t="s">
+        <v>151</v>
+      </c>
       <c r="F65" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G65" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H65" s="12" t="s">
         <v>122</v>
@@ -3112,9 +3112,11 @@
       <c r="I65" s="15">
         <v>42380</v>
       </c>
-      <c r="J65" s="15"/>
-      <c r="K65" s="6" t="s">
-        <v>120</v>
+      <c r="J65" s="15">
+        <v>42411</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="L65" s="5" t="s">
         <v>119</v>
@@ -3127,13 +3129,13 @@
       </c>
     </row>
     <row r="66" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D66" s="64"/>
-      <c r="E66" s="65"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="66"/>
       <c r="F66" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H66" s="12" t="s">
         <v>122</v>
@@ -3141,164 +3143,166 @@
       <c r="I66" s="15">
         <v>42380</v>
       </c>
-      <c r="J66" s="15">
+      <c r="J66" s="15"/>
+      <c r="K66" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="L66" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="M66" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="N66" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="67" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D67" s="46"/>
+      <c r="E67" s="67"/>
+      <c r="F67" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G67" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="I67" s="15">
+        <v>42380</v>
+      </c>
+      <c r="J67" s="15">
         <v>42411</v>
       </c>
-      <c r="K66" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L66" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="M66" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="N66" s="40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="67" spans="4:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D67" s="70"/>
-      <c r="E67" s="76" t="s">
+      <c r="K67" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L67" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="M67" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="N67" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="68" spans="4:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D68" s="48"/>
+      <c r="E68" s="51" t="s">
         <v>150</v>
       </c>
-      <c r="F67" s="14" t="s">
+      <c r="F68" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="G67" s="14"/>
-      <c r="H67" s="31" t="s">
+      <c r="G68" s="14"/>
+      <c r="H68" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="I67" s="35"/>
-      <c r="J67" s="35"/>
-      <c r="K67" s="36" t="s">
+      <c r="I68" s="35"/>
+      <c r="J68" s="35"/>
+      <c r="K68" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="L67" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="M67" s="5"/>
-      <c r="N67" s="40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="68" spans="4:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="D68" s="66"/>
-      <c r="E68" s="66" t="s">
+      <c r="L68" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="M68" s="5"/>
+      <c r="N68" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="69" spans="4:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="D69" s="65"/>
+      <c r="E69" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="F68" s="69" t="s">
+      <c r="F69" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="G68" s="69" t="s">
+      <c r="G69" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="H68" s="45" t="s">
+      <c r="H69" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="I68" s="45"/>
-      <c r="J68" s="45"/>
-      <c r="K68" s="43" t="s">
+      <c r="I69" s="83"/>
+      <c r="J69" s="83"/>
+      <c r="K69" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="L68" s="43" t="s">
+      <c r="L69" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="M68" s="43" t="s">
+      <c r="M69" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="N68" s="91" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="69" spans="4:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="D69" s="63"/>
-      <c r="E69" s="63"/>
-      <c r="F69" s="69" t="s">
+      <c r="N69" s="60" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="4:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="D70" s="66"/>
+      <c r="E70" s="66"/>
+      <c r="F70" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="G69" s="69" t="s">
+      <c r="G70" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="H69" s="46"/>
-      <c r="I69" s="46"/>
-      <c r="J69" s="46"/>
-      <c r="K69" s="44"/>
-      <c r="L69" s="44"/>
-      <c r="M69" s="44"/>
-      <c r="N69" s="92"/>
-    </row>
-    <row r="70" spans="4:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="D70" s="63"/>
-      <c r="E70" s="63"/>
-      <c r="F70" s="69" t="s">
+      <c r="H70" s="84"/>
+      <c r="I70" s="84"/>
+      <c r="J70" s="84"/>
+      <c r="K70" s="59"/>
+      <c r="L70" s="59"/>
+      <c r="M70" s="59"/>
+      <c r="N70" s="61"/>
+    </row>
+    <row r="71" spans="4:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="D71" s="66"/>
+      <c r="E71" s="66"/>
+      <c r="F71" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="G70" s="69" t="s">
+      <c r="G71" s="47" t="s">
         <v>156</v>
       </c>
-      <c r="H70" s="46"/>
-      <c r="I70" s="46"/>
-      <c r="J70" s="46"/>
-      <c r="K70" s="44"/>
-      <c r="L70" s="44"/>
-      <c r="M70" s="44"/>
-      <c r="N70" s="92"/>
-    </row>
-    <row r="71" spans="4:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="D71" s="63"/>
-      <c r="E71" s="63"/>
-      <c r="F71" s="69" t="s">
+      <c r="H71" s="84"/>
+      <c r="I71" s="84"/>
+      <c r="J71" s="84"/>
+      <c r="K71" s="59"/>
+      <c r="L71" s="59"/>
+      <c r="M71" s="59"/>
+      <c r="N71" s="61"/>
+    </row>
+    <row r="72" spans="4:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="D72" s="66"/>
+      <c r="E72" s="66"/>
+      <c r="F72" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="G71" s="69" t="s">
+      <c r="G72" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="H71" s="46"/>
-      <c r="I71" s="46"/>
-      <c r="J71" s="46"/>
-      <c r="K71" s="44"/>
-      <c r="L71" s="44"/>
-      <c r="M71" s="44"/>
-      <c r="N71" s="93"/>
-    </row>
-    <row r="72" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D72" s="64"/>
-      <c r="E72" s="77" t="s">
+      <c r="H72" s="84"/>
+      <c r="I72" s="84"/>
+      <c r="J72" s="84"/>
+      <c r="K72" s="59"/>
+      <c r="L72" s="59"/>
+      <c r="M72" s="59"/>
+      <c r="N72" s="62"/>
+    </row>
+    <row r="73" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D73" s="46"/>
+      <c r="E73" s="68" t="s">
         <v>142</v>
       </c>
-      <c r="F72" s="69" t="s">
+      <c r="F73" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="G72" s="69" t="s">
+      <c r="G73" s="47" t="s">
         <v>140</v>
-      </c>
-      <c r="H72" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="I72" s="15"/>
-      <c r="J72" s="15">
-        <v>42562</v>
-      </c>
-      <c r="K72" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L72" s="23"/>
-      <c r="M72" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N72" s="40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="73" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D73" s="64"/>
-      <c r="E73" s="77"/>
-      <c r="F73" s="69" t="s">
-        <v>144</v>
-      </c>
-      <c r="G73" s="69" t="s">
-        <v>141</v>
       </c>
       <c r="H73" s="12" t="s">
         <v>123</v>
@@ -3318,17 +3322,40 @@
         <v>121</v>
       </c>
     </row>
+    <row r="74" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D74" s="46"/>
+      <c r="E74" s="68"/>
+      <c r="F74" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="G74" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="H74" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I74" s="15"/>
+      <c r="J74" s="15">
+        <v>42562</v>
+      </c>
+      <c r="K74" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L74" s="23"/>
+      <c r="M74" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N74" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="H5:H73"/>
+  <autoFilter ref="H5:H74"/>
   <dataConsolidate/>
   <mergeCells count="34">
-    <mergeCell ref="M68:M71"/>
-    <mergeCell ref="N68:N71"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="E59:E63"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="E73:E74"/>
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="D15:G15"/>
@@ -3342,29 +3369,33 @@
     <mergeCell ref="E23:E26"/>
     <mergeCell ref="E29:E31"/>
     <mergeCell ref="E32:E34"/>
-    <mergeCell ref="L68:L71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="H68:H71"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="E64:E66"/>
-    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="E69:E72"/>
+    <mergeCell ref="M69:M72"/>
+    <mergeCell ref="N69:N72"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="E60:E64"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="L69:L72"/>
+    <mergeCell ref="K69:K72"/>
+    <mergeCell ref="H69:H72"/>
+    <mergeCell ref="I69:I72"/>
+    <mergeCell ref="J69:J72"/>
     <mergeCell ref="D50:G50"/>
     <mergeCell ref="E51:E55"/>
-    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="D69:D72"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="E42:E44"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="E36:E37"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
       <formula1>$B$8:$B$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N72:N73 K8:M73 N8:N68">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N73:N74 N8:N69 K8:M74">
       <formula1>$G$1:$G$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H73">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H74">
       <formula1>$F$1:$F$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3439,74 +3470,74 @@
       <c r="E1" s="20"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="52" t="s">
         <v>161</v>
       </c>
-      <c r="D3" s="80" t="s">
+      <c r="D3" s="53" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="80"/>
+      <c r="E3" s="53"/>
     </row>
     <row r="4" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="81"/>
-      <c r="C4" s="79" t="s">
+      <c r="B4" s="88"/>
+      <c r="C4" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="E4" s="80"/>
+      <c r="E4" s="53"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
-      <c r="C5" s="79" t="s">
+      <c r="B5" s="89"/>
+      <c r="C5" s="52" t="s">
         <v>162</v>
       </c>
-      <c r="D5" s="79" t="s">
+      <c r="D5" s="52" t="s">
         <v>168</v>
       </c>
-      <c r="E5" s="80"/>
+      <c r="E5" s="53"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="92" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85" t="s">
+      <c r="C6" s="55"/>
+      <c r="D6" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="90" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="87"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85" t="s">
+      <c r="B7" s="93"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="88"/>
+      <c r="E7" s="91"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80" t="s">
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="53" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="56" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="89"/>
+      <c r="E9" s="56"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
@@ -3590,8 +3621,8 @@
         <v>119</v>
       </c>
       <c r="C3" s="17">
-        <f>COUNTIF(CODING!K6:K78,"Done")</f>
-        <v>30</v>
+        <f>COUNTIF(CODING!K6:K79,"Done")</f>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3599,7 +3630,7 @@
         <v>120</v>
       </c>
       <c r="C4" s="16">
-        <f>COUNTIF(CODING!K7:K81, "In Progress")</f>
+        <f>COUNTIF(CODING!K7:K82, "In Progress")</f>
         <v>20</v>
       </c>
     </row>
@@ -3608,7 +3639,7 @@
         <v>121</v>
       </c>
       <c r="C5" s="3">
-        <f>COUNTIF(CODING!K6:K79, "Not Start")</f>
+        <f>COUNTIF(CODING!K6:K80, "Not Start")</f>
         <v>7</v>
       </c>
     </row>
@@ -3618,7 +3649,7 @@
       </c>
       <c r="C6" s="3">
         <f>SUM(C3:C5)</f>
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3631,7 +3662,7 @@
         <v>119</v>
       </c>
       <c r="C9" s="17">
-        <f>COUNTIF(CODING!N7:N117,"Done")</f>
+        <f>COUNTIF(CODING!N7:N118,"Done")</f>
         <v>24</v>
       </c>
     </row>
@@ -3640,7 +3671,7 @@
         <v>120</v>
       </c>
       <c r="C10" s="16">
-        <f>COUNTIF(CODING!N6:N103,"In Progress")</f>
+        <f>COUNTIF(CODING!N6:N104,"In Progress")</f>
         <v>1</v>
       </c>
     </row>
@@ -3649,7 +3680,7 @@
         <v>121</v>
       </c>
       <c r="C11" s="3">
-        <f>COUNTIF(CODING!N7:N78, "Not Start")</f>
+        <f>COUNTIF(CODING!N7:N79, "Not Start")</f>
         <v>32</v>
       </c>
     </row>
@@ -3672,8 +3703,8 @@
         <v>119</v>
       </c>
       <c r="C16" s="17">
-        <f>COUNTIF(CODING!M5:M89,"Done")</f>
-        <v>17</v>
+        <f>COUNTIF(CODING!M5:M90,"Done")</f>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -3681,7 +3712,7 @@
         <v>120</v>
       </c>
       <c r="C17" s="16">
-        <f>COUNTIF(CODING!M6:M87,"In Progress")</f>
+        <f>COUNTIF(CODING!M6:M88,"In Progress")</f>
         <v>1</v>
       </c>
     </row>
@@ -3690,7 +3721,7 @@
         <v>121</v>
       </c>
       <c r="C18" s="3">
-        <f>COUNTIF(CODING!M6:M82, "Not Start")</f>
+        <f>COUNTIF(CODING!M6:M83, "Not Start")</f>
         <v>39</v>
       </c>
     </row>
@@ -3700,7 +3731,7 @@
       </c>
       <c r="C19" s="3">
         <f>SUM(C16:C18)</f>
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Doc]_HuyenPT_Update các file doc
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -13,8 +13,8 @@
     <sheet name="TỔNG HỢP" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CODING!$H$5:$H$74</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">CODING!$A$5:$M$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CODING!$H$5:$H$75</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">CODING!$A$5:$M$73</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">DESIGN!#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621" refMode="R1C1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="197">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -626,6 +626,12 @@
   </si>
   <si>
     <t>Thêm thể loại sách</t>
+  </si>
+  <si>
+    <t>Bỏ thích một bài đăng</t>
+  </si>
+  <si>
+    <t>Bỏ thích một bình luận</t>
   </si>
 </sst>
 </file>
@@ -1000,6 +1006,60 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1020,60 +1080,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1414,10 +1420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:N75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,12 +1511,12 @@
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D6" s="69" t="s">
+      <c r="D6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -1520,12 +1526,12 @@
       <c r="N6" s="22"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
@@ -1539,7 +1545,7 @@
         <v>118</v>
       </c>
       <c r="D8" s="45"/>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="62" t="s">
         <v>187</v>
       </c>
       <c r="F8" s="14" t="s">
@@ -1572,7 +1578,7 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D9" s="46"/>
-      <c r="E9" s="67"/>
+      <c r="E9" s="69"/>
       <c r="F9" s="14" t="s">
         <v>8</v>
       </c>
@@ -1603,7 +1609,7 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D10" s="14"/>
-      <c r="E10" s="65" t="s">
+      <c r="E10" s="61" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="14" t="s">
@@ -1639,7 +1645,7 @@
         <v>121</v>
       </c>
       <c r="D11" s="14"/>
-      <c r="E11" s="67"/>
+      <c r="E11" s="69"/>
       <c r="F11" s="14" t="s">
         <v>13</v>
       </c>
@@ -1673,7 +1679,7 @@
         <v>120</v>
       </c>
       <c r="D12" s="14"/>
-      <c r="E12" s="65" t="s">
+      <c r="E12" s="61" t="s">
         <v>188</v>
       </c>
       <c r="F12" s="85" t="s">
@@ -1705,7 +1711,7 @@
     <row r="13" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="D13" s="14"/>
-      <c r="E13" s="66"/>
+      <c r="E13" s="62"/>
       <c r="F13" s="86"/>
       <c r="G13" s="14" t="s">
         <v>160</v>
@@ -1733,7 +1739,7 @@
         <v>119</v>
       </c>
       <c r="D14" s="14"/>
-      <c r="E14" s="67"/>
+      <c r="E14" s="69"/>
       <c r="F14" s="14" t="s">
         <v>17</v>
       </c>
@@ -1759,12 +1765,12 @@
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D15" s="71" t="s">
+      <c r="D15" s="66" t="s">
         <v>184</v>
       </c>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="73"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="68"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
@@ -1775,10 +1781,10 @@
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D16" s="46"/>
-      <c r="E16" s="65" t="s">
+      <c r="E16" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="63" t="s">
+      <c r="F16" s="81" t="s">
         <v>183</v>
       </c>
       <c r="G16" s="19" t="s">
@@ -1806,8 +1812,8 @@
     </row>
     <row r="17" spans="4:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="48"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="64"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="82"/>
       <c r="G17" s="19" t="s">
         <v>185</v>
       </c>
@@ -1830,8 +1836,8 @@
       </c>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D18" s="65"/>
-      <c r="E18" s="66"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="62"/>
       <c r="F18" s="18" t="s">
         <v>20</v>
       </c>
@@ -1857,8 +1863,8 @@
       </c>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D19" s="67"/>
-      <c r="E19" s="66"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="62"/>
       <c r="F19" s="18" t="s">
         <v>22</v>
       </c>
@@ -1885,7 +1891,7 @@
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D20" s="46"/>
-      <c r="E20" s="66"/>
+      <c r="E20" s="62"/>
       <c r="F20" s="18" t="s">
         <v>24</v>
       </c>
@@ -1912,7 +1918,7 @@
     </row>
     <row r="21" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D21" s="46"/>
-      <c r="E21" s="66"/>
+      <c r="E21" s="62"/>
       <c r="F21" s="18" t="s">
         <v>26</v>
       </c>
@@ -1939,11 +1945,13 @@
     </row>
     <row r="22" spans="4:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="46"/>
-      <c r="E22" s="66"/>
+      <c r="E22" s="62"/>
       <c r="F22" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="G22" s="18"/>
+      <c r="G22" s="18" t="s">
+        <v>195</v>
+      </c>
       <c r="H22" s="12" t="s">
         <v>122</v>
       </c>
@@ -1964,7 +1972,7 @@
     </row>
     <row r="23" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D23" s="46"/>
-      <c r="E23" s="65" t="s">
+      <c r="E23" s="61" t="s">
         <v>28</v>
       </c>
       <c r="F23" s="14" t="s">
@@ -1993,7 +2001,7 @@
     </row>
     <row r="24" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D24" s="46"/>
-      <c r="E24" s="66"/>
+      <c r="E24" s="62"/>
       <c r="F24" s="14" t="s">
         <v>31</v>
       </c>
@@ -2020,7 +2028,7 @@
     </row>
     <row r="25" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D25" s="46"/>
-      <c r="E25" s="66"/>
+      <c r="E25" s="62"/>
       <c r="F25" s="14" t="s">
         <v>33</v>
       </c>
@@ -2047,7 +2055,7 @@
     </row>
     <row r="26" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D26" s="46"/>
-      <c r="E26" s="67"/>
+      <c r="E26" s="62"/>
       <c r="F26" s="14" t="s">
         <v>35</v>
       </c>
@@ -2072,98 +2080,88 @@
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="4:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="46"/>
-      <c r="E27" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>123</v>
-      </c>
+      <c r="E27" s="69"/>
+      <c r="F27" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="H27" s="12"/>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
-      <c r="K27" s="6" t="s">
+      <c r="K27" s="6"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="23"/>
+    </row>
+    <row r="28" spans="4:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="D28" s="46"/>
+      <c r="E28" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="L27" s="24" t="s">
+      <c r="L28" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="M27" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N27" s="23"/>
-    </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D28" s="77" t="s">
+      <c r="M28" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N28" s="23"/>
+    </row>
+    <row r="29" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D29" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="57"/>
-    </row>
-    <row r="29" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D29" s="48"/>
-      <c r="E29" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="H29" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="I29" s="15">
-        <v>42593</v>
-      </c>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
       <c r="J29" s="12"/>
-      <c r="K29" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N29" s="40" t="s">
-        <v>121</v>
-      </c>
+      <c r="K29" s="3"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="57"/>
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D30" s="48"/>
-      <c r="E30" s="81"/>
-      <c r="F30" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G30" s="19" t="s">
-        <v>42</v>
+      <c r="E30" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="I30" s="15"/>
+      <c r="I30" s="15">
+        <v>42593</v>
+      </c>
       <c r="J30" s="12"/>
-      <c r="K30" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L30" s="6" t="s">
-        <v>120</v>
+      <c r="K30" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="M30" s="4" t="s">
         <v>121</v>
@@ -2174,17 +2172,17 @@
     </row>
     <row r="31" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D31" s="48"/>
-      <c r="E31" s="82"/>
-      <c r="F31" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="47" t="s">
-        <v>44</v>
+      <c r="E31" s="59"/>
+      <c r="F31" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="I31" s="12"/>
+      <c r="I31" s="15"/>
       <c r="J31" s="12"/>
       <c r="K31" s="6" t="s">
         <v>120</v>
@@ -2199,29 +2197,25 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="4:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D32" s="48"/>
-      <c r="E32" s="65" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>46</v>
+      <c r="E32" s="60"/>
+      <c r="F32" s="47" t="s">
+        <v>43</v>
       </c>
       <c r="G32" s="47" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="I32" s="15">
-        <v>42593</v>
-      </c>
+      <c r="I32" s="12"/>
       <c r="J32" s="12"/>
-      <c r="K32" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L32" s="5" t="s">
-        <v>119</v>
+      <c r="K32" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>121</v>
@@ -2230,20 +2224,22 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:14" ht="45" x14ac:dyDescent="0.25">
       <c r="D33" s="48"/>
-      <c r="E33" s="66"/>
+      <c r="E33" s="61" t="s">
+        <v>45</v>
+      </c>
       <c r="F33" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="G33" s="47" t="s">
+        <v>47</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>123</v>
       </c>
       <c r="I33" s="15">
-        <v>42594</v>
+        <v>42593</v>
       </c>
       <c r="J33" s="12"/>
       <c r="K33" s="5" t="s">
@@ -2261,23 +2257,25 @@
     </row>
     <row r="34" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D34" s="48"/>
-      <c r="E34" s="67"/>
+      <c r="E34" s="62"/>
       <c r="F34" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="I34" s="12"/>
+      <c r="I34" s="15">
+        <v>42594</v>
+      </c>
       <c r="J34" s="12"/>
-      <c r="K34" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L34" s="24" t="s">
-        <v>120</v>
+      <c r="K34" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>121</v>
@@ -2287,59 +2285,57 @@
       </c>
     </row>
     <row r="35" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D35" s="74" t="s">
-        <v>52</v>
-      </c>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="12"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>123</v>
+      </c>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="57"/>
-    </row>
-    <row r="36" spans="4:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="D36" s="46"/>
-      <c r="E36" s="65" t="s">
+      <c r="K35" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="L35" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N35" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D36" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="71"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="57"/>
+    </row>
+    <row r="37" spans="4:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="D37" s="46"/>
+      <c r="E37" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F37" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G36" s="47" t="s">
+      <c r="G37" s="47" t="s">
         <v>55</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="I36" s="15">
-        <v>42411</v>
-      </c>
-      <c r="J36" s="15"/>
-      <c r="K36" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="N36" s="23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="37" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D37" s="46"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G37" s="47" t="s">
-        <v>57</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>123</v>
@@ -2347,90 +2343,90 @@
       <c r="I37" s="15">
         <v>42411</v>
       </c>
-      <c r="J37" s="15">
+      <c r="J37" s="15"/>
+      <c r="K37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="N37" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D38" s="46"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G38" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I38" s="15">
+        <v>42411</v>
+      </c>
+      <c r="J38" s="15">
         <v>42562</v>
       </c>
-      <c r="K37" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="N37" s="23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="4:14" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="D38" s="46"/>
-      <c r="E38" s="80" t="s">
+      <c r="K38" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="N38" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="4:14" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="D39" s="46"/>
+      <c r="E39" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="F38" s="47" t="s">
+      <c r="F39" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="G38" s="47" t="s">
+      <c r="G39" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="H38" s="33" t="s">
+      <c r="H39" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="I38" s="34">
+      <c r="I39" s="34">
         <v>42411</v>
       </c>
-      <c r="J38" s="33"/>
-      <c r="K38" s="25" t="s">
+      <c r="J39" s="33"/>
+      <c r="K39" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="L38" s="26" t="s">
+      <c r="L39" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="M38" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N38" s="23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="4:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="D39" s="46"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="47" t="s">
+      <c r="M39" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N39" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="4:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="D40" s="46"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="G39" s="49" t="s">
+      <c r="G40" s="49" t="s">
         <v>62</v>
-      </c>
-      <c r="H39" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="I39" s="15">
-        <v>42411</v>
-      </c>
-      <c r="J39" s="12"/>
-      <c r="K39" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L39" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="M39" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N39" s="23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D40" s="46"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>64</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>123</v>
@@ -2438,9 +2434,7 @@
       <c r="I40" s="15">
         <v>42411</v>
       </c>
-      <c r="J40" s="15">
-        <v>42562</v>
-      </c>
+      <c r="J40" s="12"/>
       <c r="K40" s="5" t="s">
         <v>119</v>
       </c>
@@ -2456,12 +2450,12 @@
     </row>
     <row r="41" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D41" s="46"/>
-      <c r="E41" s="82"/>
+      <c r="E41" s="59"/>
       <c r="F41" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H41" s="12" t="s">
         <v>123</v>
@@ -2485,41 +2479,47 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="4:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D42" s="46"/>
-      <c r="E42" s="65" t="s">
+      <c r="E42" s="60"/>
+      <c r="F42" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I42" s="15">
+        <v>42411</v>
+      </c>
+      <c r="J42" s="15">
+        <v>42562</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L42" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N42" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="4:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="D43" s="46"/>
+      <c r="E43" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="F42" s="50" t="s">
+      <c r="F43" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="G42" s="47" t="s">
+      <c r="G43" s="47" t="s">
         <v>69</v>
-      </c>
-      <c r="H42" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L42" s="24"/>
-      <c r="M42" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N42" s="23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="43" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D43" s="46"/>
-      <c r="E43" s="66"/>
-      <c r="F43" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>71</v>
       </c>
       <c r="H43" s="12" t="s">
         <v>122</v>
@@ -2539,12 +2539,12 @@
     </row>
     <row r="44" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D44" s="46"/>
-      <c r="E44" s="67"/>
+      <c r="E44" s="62"/>
       <c r="F44" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H44" s="12" t="s">
         <v>122</v>
@@ -2563,182 +2563,182 @@
       </c>
     </row>
     <row r="45" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D45" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="E45" s="75"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="76"/>
-      <c r="H45" s="12"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G45" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>122</v>
+      </c>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="22"/>
-      <c r="M45" s="30"/>
-      <c r="N45" s="57"/>
+      <c r="K45" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="L45" s="24"/>
+      <c r="M45" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N45" s="23" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="46" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="G46" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="H46" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="I46" s="15">
-        <v>42411</v>
-      </c>
-      <c r="J46" s="15">
-        <v>42562</v>
-      </c>
-      <c r="K46" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L46" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="M46" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N46" s="23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="47" spans="4:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="D46" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" s="71"/>
+      <c r="F46" s="71"/>
+      <c r="G46" s="72"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="30"/>
+      <c r="N46" s="57"/>
+    </row>
+    <row r="47" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D47" s="46"/>
       <c r="E47" s="46"/>
       <c r="F47" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I47" s="15">
+        <v>42411</v>
+      </c>
+      <c r="J47" s="15">
+        <v>42562</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L47" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N47" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="4:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="G47" s="47" t="s">
+      <c r="G48" s="47" t="s">
         <v>163</v>
       </c>
-      <c r="H47" s="12"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="23"/>
-      <c r="M47" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N47" s="40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="4:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="43" t="s">
+      <c r="H48" s="12"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N48" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="G48" s="18" t="s">
+      <c r="G49" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="H48" s="39" t="s">
+      <c r="H49" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="I48" s="39"/>
-      <c r="J48" s="39"/>
-      <c r="K48" s="41" t="s">
+      <c r="I49" s="39"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="L48" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="M48" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N48" s="40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="14" t="s">
+      <c r="L49" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N49" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="G49" s="47" t="s">
+      <c r="G50" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="H49" s="12" t="s">
+      <c r="H50" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12"/>
-      <c r="K49" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L49" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="M49" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N49" s="40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D50" s="69" t="s">
-        <v>79</v>
-      </c>
-      <c r="E50" s="69"/>
-      <c r="F50" s="69"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="12"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="22"/>
-      <c r="M50" s="30"/>
-      <c r="N50" s="57"/>
+      <c r="K50" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N50" s="40" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D51" s="46"/>
-      <c r="E51" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G51" s="14"/>
-      <c r="H51" s="12" t="s">
-        <v>118</v>
-      </c>
+      <c r="D51" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="E51" s="64"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="64"/>
+      <c r="H51" s="12"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
-      <c r="K51" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L51" s="28"/>
-      <c r="M51" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N51" s="40" t="s">
-        <v>121</v>
-      </c>
+      <c r="K51" s="3"/>
+      <c r="L51" s="22"/>
+      <c r="M51" s="30"/>
+      <c r="N51" s="57"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D52" s="46"/>
-      <c r="E52" s="66"/>
+      <c r="E52" s="61" t="s">
+        <v>80</v>
+      </c>
       <c r="F52" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="G52" s="14" t="s">
-        <v>83</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="G52" s="14"/>
       <c r="H52" s="12" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
-      <c r="K52" s="4" t="s">
-        <v>121</v>
+      <c r="K52" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="L52" s="28"/>
       <c r="M52" s="4" t="s">
@@ -2750,12 +2750,12 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D53" s="46"/>
-      <c r="E53" s="66"/>
+      <c r="E53" s="62"/>
       <c r="F53" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G53" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H53" s="12" t="s">
         <v>123</v>
@@ -2773,17 +2773,14 @@
         <v>121</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>122</v>
-      </c>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D54" s="46"/>
-      <c r="E54" s="66"/>
-      <c r="F54" s="47" t="s">
-        <v>86</v>
+      <c r="E54" s="62"/>
+      <c r="F54" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H54" s="12" t="s">
         <v>123</v>
@@ -2803,15 +2800,15 @@
     </row>
     <row r="55" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D55" s="46"/>
-      <c r="E55" s="67"/>
+      <c r="E55" s="62"/>
       <c r="F55" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="G55" s="47" t="s">
-        <v>89</v>
+        <v>86</v>
+      </c>
+      <c r="G55" s="14" t="s">
+        <v>87</v>
       </c>
       <c r="H55" s="12" t="s">
         <v>123</v>
@@ -2829,56 +2826,57 @@
         <v>121</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D56" s="46"/>
-      <c r="E56" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="G56" s="14" t="s">
-        <v>92</v>
+      <c r="E56" s="69"/>
+      <c r="F56" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="G56" s="47" t="s">
+        <v>89</v>
       </c>
       <c r="H56" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="I56" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="J56" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K56" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L56" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="M56" s="5" t="s">
-        <v>119</v>
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L56" s="28"/>
+      <c r="M56" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="N56" s="40" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="57" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>118</v>
+      </c>
       <c r="D57" s="46"/>
-      <c r="E57" s="66"/>
+      <c r="E57" s="61" t="s">
+        <v>90</v>
+      </c>
       <c r="F57" s="14" t="s">
-        <v>193</v>
+        <v>91</v>
       </c>
       <c r="G57" s="14" t="s">
-        <v>194</v>
+        <v>92</v>
       </c>
       <c r="H57" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
+      <c r="I57" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J57" s="12" t="s">
+        <v>131</v>
+      </c>
       <c r="K57" s="5" t="s">
         <v>119</v>
       </c>
@@ -2888,26 +2886,24 @@
       <c r="M57" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="N57" s="40"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N57" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D58" s="46"/>
-      <c r="E58" s="66"/>
+      <c r="E58" s="62"/>
       <c r="F58" s="14" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
       <c r="G58" s="14" t="s">
-        <v>94</v>
+        <v>194</v>
       </c>
       <c r="H58" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="I58" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="J58" s="12" t="s">
-        <v>131</v>
-      </c>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
       <c r="K58" s="5" t="s">
         <v>119</v>
       </c>
@@ -2917,18 +2913,16 @@
       <c r="M58" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="N58" s="40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="N58" s="40"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D59" s="46"/>
-      <c r="E59" s="67"/>
-      <c r="F59" s="47" t="s">
-        <v>95</v>
+      <c r="E59" s="62"/>
+      <c r="F59" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="G59" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H59" s="12" t="s">
         <v>123</v>
@@ -2939,47 +2933,45 @@
       <c r="J59" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="K59" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="L59" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="M59" s="4" t="s">
-        <v>121</v>
+      <c r="K59" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L59" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="M59" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="N59" s="40" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="D60" s="46"/>
-      <c r="E60" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>98</v>
+      <c r="E60" s="69"/>
+      <c r="F60" s="47" t="s">
+        <v>95</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J60" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="K60" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L60" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="M60" s="5" t="s">
-        <v>119</v>
+        <v>131</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L60" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M60" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="N60" s="40" t="s">
         <v>121</v>
@@ -2987,21 +2979,23 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D61" s="46"/>
-      <c r="E61" s="66"/>
+      <c r="E61" s="61" t="s">
+        <v>97</v>
+      </c>
       <c r="F61" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H61" s="12" t="s">
         <v>122</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J61" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K61" s="5" t="s">
         <v>119</v>
@@ -3018,20 +3012,24 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D62" s="46"/>
-      <c r="E62" s="66"/>
+      <c r="E62" s="62"/>
       <c r="F62" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H62" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="I62" s="12"/>
-      <c r="J62" s="12"/>
-      <c r="K62" s="4" t="s">
-        <v>121</v>
+      <c r="I62" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="J62" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="L62" s="5" t="s">
         <v>119</v>
@@ -3043,24 +3041,26 @@
         <v>121</v>
       </c>
     </row>
-    <row r="63" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D63" s="46"/>
-      <c r="E63" s="66"/>
+      <c r="E63" s="62"/>
       <c r="F63" s="14" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="G63" s="14" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="H63" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
-      <c r="K63" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L63" s="23"/>
+      <c r="K63" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L63" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="M63" s="5" t="s">
         <v>119</v>
       </c>
@@ -3070,24 +3070,22 @@
     </row>
     <row r="64" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D64" s="46"/>
-      <c r="E64" s="67"/>
+      <c r="E64" s="62"/>
       <c r="F64" s="14" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G64" s="14" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H64" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
-      <c r="K64" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="L64" s="5" t="s">
-        <v>119</v>
-      </c>
+      <c r="K64" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L64" s="23"/>
       <c r="M64" s="5" t="s">
         <v>119</v>
       </c>
@@ -3095,28 +3093,22 @@
         <v>121</v>
       </c>
     </row>
-    <row r="65" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D65" s="46"/>
-      <c r="E65" s="65" t="s">
-        <v>151</v>
-      </c>
+      <c r="E65" s="69"/>
       <c r="F65" s="14" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="G65" s="14" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="H65" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="I65" s="15">
-        <v>42380</v>
-      </c>
-      <c r="J65" s="15">
-        <v>42411</v>
-      </c>
-      <c r="K65" s="5" t="s">
-        <v>119</v>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="K65" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="L65" s="5" t="s">
         <v>119</v>
@@ -3130,12 +3122,14 @@
     </row>
     <row r="66" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D66" s="46"/>
-      <c r="E66" s="66"/>
+      <c r="E66" s="61" t="s">
+        <v>151</v>
+      </c>
       <c r="F66" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H66" s="12" t="s">
         <v>122</v>
@@ -3143,9 +3137,11 @@
       <c r="I66" s="15">
         <v>42380</v>
       </c>
-      <c r="J66" s="15"/>
-      <c r="K66" s="6" t="s">
-        <v>120</v>
+      <c r="J66" s="15">
+        <v>42411</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="L66" s="5" t="s">
         <v>119</v>
@@ -3159,12 +3155,12 @@
     </row>
     <row r="67" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D67" s="46"/>
-      <c r="E67" s="67"/>
+      <c r="E67" s="62"/>
       <c r="F67" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H67" s="12" t="s">
         <v>122</v>
@@ -3172,164 +3168,166 @@
       <c r="I67" s="15">
         <v>42380</v>
       </c>
-      <c r="J67" s="15">
+      <c r="J67" s="15"/>
+      <c r="K67" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="L67" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="M67" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="N67" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="68" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D68" s="46"/>
+      <c r="E68" s="69"/>
+      <c r="F68" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G68" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H68" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="I68" s="15">
+        <v>42380</v>
+      </c>
+      <c r="J68" s="15">
         <v>42411</v>
       </c>
-      <c r="K67" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L67" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="M67" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="N67" s="40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="68" spans="4:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D68" s="48"/>
-      <c r="E68" s="51" t="s">
+      <c r="K68" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L68" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="M68" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="N68" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="69" spans="4:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D69" s="48"/>
+      <c r="E69" s="51" t="s">
         <v>150</v>
       </c>
-      <c r="F68" s="14" t="s">
+      <c r="F69" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="G68" s="14"/>
-      <c r="H68" s="31" t="s">
+      <c r="G69" s="14"/>
+      <c r="H69" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="I68" s="35"/>
-      <c r="J68" s="35"/>
-      <c r="K68" s="36" t="s">
+      <c r="I69" s="35"/>
+      <c r="J69" s="35"/>
+      <c r="K69" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="L68" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="M68" s="5"/>
-      <c r="N68" s="40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="69" spans="4:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="D69" s="65"/>
-      <c r="E69" s="65" t="s">
+      <c r="L69" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="M69" s="5"/>
+      <c r="N69" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="4:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="D70" s="61"/>
+      <c r="E70" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="F69" s="47" t="s">
+      <c r="F70" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="G69" s="47" t="s">
+      <c r="G70" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="H69" s="83" t="s">
+      <c r="H70" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="I69" s="83"/>
-      <c r="J69" s="83"/>
-      <c r="K69" s="58" t="s">
+      <c r="I70" s="83"/>
+      <c r="J70" s="83"/>
+      <c r="K70" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="L69" s="58" t="s">
+      <c r="L70" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="M69" s="58" t="s">
+      <c r="M70" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="N69" s="60" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="70" spans="4:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="D70" s="66"/>
-      <c r="E70" s="66"/>
-      <c r="F70" s="47" t="s">
+      <c r="N70" s="78" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="71" spans="4:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="D71" s="62"/>
+      <c r="E71" s="62"/>
+      <c r="F71" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="G70" s="47" t="s">
+      <c r="G71" s="47" t="s">
         <v>155</v>
-      </c>
-      <c r="H70" s="84"/>
-      <c r="I70" s="84"/>
-      <c r="J70" s="84"/>
-      <c r="K70" s="59"/>
-      <c r="L70" s="59"/>
-      <c r="M70" s="59"/>
-      <c r="N70" s="61"/>
-    </row>
-    <row r="71" spans="4:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="D71" s="66"/>
-      <c r="E71" s="66"/>
-      <c r="F71" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="G71" s="47" t="s">
-        <v>156</v>
       </c>
       <c r="H71" s="84"/>
       <c r="I71" s="84"/>
       <c r="J71" s="84"/>
-      <c r="K71" s="59"/>
-      <c r="L71" s="59"/>
-      <c r="M71" s="59"/>
-      <c r="N71" s="61"/>
-    </row>
-    <row r="72" spans="4:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="D72" s="66"/>
-      <c r="E72" s="66"/>
+      <c r="K71" s="77"/>
+      <c r="L71" s="77"/>
+      <c r="M71" s="77"/>
+      <c r="N71" s="79"/>
+    </row>
+    <row r="72" spans="4:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="D72" s="62"/>
+      <c r="E72" s="62"/>
       <c r="F72" s="47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G72" s="47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H72" s="84"/>
       <c r="I72" s="84"/>
       <c r="J72" s="84"/>
-      <c r="K72" s="59"/>
-      <c r="L72" s="59"/>
-      <c r="M72" s="59"/>
-      <c r="N72" s="62"/>
-    </row>
-    <row r="73" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D73" s="46"/>
-      <c r="E73" s="68" t="s">
-        <v>142</v>
-      </c>
+      <c r="K72" s="77"/>
+      <c r="L72" s="77"/>
+      <c r="M72" s="77"/>
+      <c r="N72" s="79"/>
+    </row>
+    <row r="73" spans="4:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="D73" s="62"/>
+      <c r="E73" s="62"/>
       <c r="F73" s="47" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="G73" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="H73" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="I73" s="15"/>
-      <c r="J73" s="15">
-        <v>42562</v>
-      </c>
-      <c r="K73" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L73" s="23"/>
-      <c r="M73" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N73" s="40" t="s">
-        <v>121</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="H73" s="84"/>
+      <c r="I73" s="84"/>
+      <c r="J73" s="84"/>
+      <c r="K73" s="77"/>
+      <c r="L73" s="77"/>
+      <c r="M73" s="77"/>
+      <c r="N73" s="80"/>
     </row>
     <row r="74" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D74" s="46"/>
-      <c r="E74" s="68"/>
+      <c r="E74" s="63" t="s">
+        <v>142</v>
+      </c>
       <c r="F74" s="47" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G74" s="47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H74" s="12" t="s">
         <v>123</v>
@@ -3349,53 +3347,80 @@
         <v>121</v>
       </c>
     </row>
+    <row r="75" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D75" s="46"/>
+      <c r="E75" s="63"/>
+      <c r="F75" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="G75" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="H75" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15">
+        <v>42562</v>
+      </c>
+      <c r="K75" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L75" s="23"/>
+      <c r="M75" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N75" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="H5:H74"/>
+  <autoFilter ref="H5:H75"/>
   <dataConsolidate/>
   <mergeCells count="34">
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="E61:E65"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="L70:L73"/>
+    <mergeCell ref="K70:K73"/>
+    <mergeCell ref="H70:H73"/>
+    <mergeCell ref="I70:I73"/>
+    <mergeCell ref="J70:J73"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="E52:E56"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="E23:E27"/>
+    <mergeCell ref="E66:E68"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="M70:M73"/>
+    <mergeCell ref="N70:N73"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E74:E75"/>
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="D15:G15"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D36:G36"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E16:E22"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="E69:E72"/>
-    <mergeCell ref="M69:M72"/>
-    <mergeCell ref="N69:N72"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="E60:E64"/>
-    <mergeCell ref="E56:E59"/>
-    <mergeCell ref="L69:L72"/>
-    <mergeCell ref="K69:K72"/>
-    <mergeCell ref="H69:H72"/>
-    <mergeCell ref="I69:I72"/>
-    <mergeCell ref="J69:J72"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="E51:E55"/>
-    <mergeCell ref="D69:D72"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="E33:E35"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
       <formula1>$B$8:$B$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N73:N74 N8:N69 K8:M74">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N74:N75 N8:N70 K8:M75">
       <formula1>$G$1:$G$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H74">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H75">
       <formula1>$F$1:$F$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3621,7 +3646,7 @@
         <v>119</v>
       </c>
       <c r="C3" s="17">
-        <f>COUNTIF(CODING!K6:K79,"Done")</f>
+        <f>COUNTIF(CODING!K6:K80,"Done")</f>
         <v>31</v>
       </c>
     </row>
@@ -3630,7 +3655,7 @@
         <v>120</v>
       </c>
       <c r="C4" s="16">
-        <f>COUNTIF(CODING!K7:K82, "In Progress")</f>
+        <f>COUNTIF(CODING!K7:K83, "In Progress")</f>
         <v>20</v>
       </c>
     </row>
@@ -3639,7 +3664,7 @@
         <v>121</v>
       </c>
       <c r="C5" s="3">
-        <f>COUNTIF(CODING!K6:K80, "Not Start")</f>
+        <f>COUNTIF(CODING!K6:K81, "Not Start")</f>
         <v>7</v>
       </c>
     </row>
@@ -3662,7 +3687,7 @@
         <v>119</v>
       </c>
       <c r="C9" s="17">
-        <f>COUNTIF(CODING!N7:N118,"Done")</f>
+        <f>COUNTIF(CODING!N7:N119,"Done")</f>
         <v>24</v>
       </c>
     </row>
@@ -3671,7 +3696,7 @@
         <v>120</v>
       </c>
       <c r="C10" s="16">
-        <f>COUNTIF(CODING!N6:N104,"In Progress")</f>
+        <f>COUNTIF(CODING!N6:N105,"In Progress")</f>
         <v>1</v>
       </c>
     </row>
@@ -3680,7 +3705,7 @@
         <v>121</v>
       </c>
       <c r="C11" s="3">
-        <f>COUNTIF(CODING!N7:N79, "Not Start")</f>
+        <f>COUNTIF(CODING!N7:N80, "Not Start")</f>
         <v>32</v>
       </c>
     </row>
@@ -3703,7 +3728,7 @@
         <v>119</v>
       </c>
       <c r="C16" s="17">
-        <f>COUNTIF(CODING!M5:M90,"Done")</f>
+        <f>COUNTIF(CODING!M5:M91,"Done")</f>
         <v>18</v>
       </c>
     </row>
@@ -3712,7 +3737,7 @@
         <v>120</v>
       </c>
       <c r="C17" s="16">
-        <f>COUNTIF(CODING!M6:M88,"In Progress")</f>
+        <f>COUNTIF(CODING!M6:M89,"In Progress")</f>
         <v>1</v>
       </c>
     </row>
@@ -3721,7 +3746,7 @@
         <v>121</v>
       </c>
       <c r="C18" s="3">
-        <f>COUNTIF(CODING!M6:M83, "Not Start")</f>
+        <f>COUNTIF(CODING!M6:M84, "Not Start")</f>
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DangVH: Commit update tiến độ dự án
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17531"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Capstone\WIP\Users\HuyenPT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7500"/>
   </bookViews>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$5:$L$73</definedName>
   </definedNames>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -720,7 +725,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -949,10 +954,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -973,16 +988,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -992,9 +997,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FF99"/>
+      <color rgb="FF00FF99"/>
+      <color rgb="FFFFFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1043,7 +1058,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1076,9 +1091,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1111,6 +1143,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1289,7 +1338,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1352,12 +1403,12 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1370,7 +1421,7 @@
       <c r="B7" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="33" t="s">
         <v>118</v>
       </c>
       <c r="D7" s="25" t="s">
@@ -1405,7 +1456,7 @@
       <c r="B8" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="29"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="25" t="s">
         <v>8</v>
       </c>
@@ -1435,12 +1486,12 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1453,7 +1504,7 @@
       <c r="B10" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="33" t="s">
         <v>121</v>
       </c>
       <c r="D10" s="25" t="s">
@@ -1488,7 +1539,7 @@
       <c r="B11" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="29"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="25" t="s">
         <v>6</v>
       </c>
@@ -1521,7 +1572,7 @@
       <c r="B12" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="29"/>
+      <c r="C12" s="33"/>
       <c r="D12" s="25" t="s">
         <v>123</v>
       </c>
@@ -1552,7 +1603,7 @@
       <c r="B13" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="29"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="25" t="s">
         <v>125</v>
       </c>
@@ -1581,7 +1632,7 @@
       <c r="B14" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="29"/>
+      <c r="C14" s="33"/>
       <c r="D14" s="25" t="s">
         <v>126</v>
       </c>
@@ -1610,7 +1661,7 @@
       <c r="B15" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="33" t="s">
         <v>128</v>
       </c>
       <c r="D15" s="25" t="s">
@@ -1643,7 +1694,7 @@
       <c r="B16" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="29"/>
+      <c r="C16" s="33"/>
       <c r="D16" s="25" t="s">
         <v>130</v>
       </c>
@@ -1672,7 +1723,7 @@
       <c r="B17" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="29"/>
+      <c r="C17" s="33"/>
       <c r="D17" s="25" t="s">
         <v>132</v>
       </c>
@@ -1701,7 +1752,7 @@
       <c r="B18" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="29"/>
+      <c r="C18" s="33"/>
       <c r="D18" s="25" t="s">
         <v>134</v>
       </c>
@@ -1730,7 +1781,7 @@
       <c r="B19" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="29"/>
+      <c r="C19" s="33"/>
       <c r="D19" s="25" t="s">
         <v>48</v>
       </c>
@@ -1759,7 +1810,7 @@
       <c r="B20" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="29"/>
+      <c r="C20" s="33"/>
       <c r="D20" s="25" t="s">
         <v>9</v>
       </c>
@@ -1788,7 +1839,7 @@
       <c r="B21" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="29"/>
+      <c r="C21" s="33"/>
       <c r="D21" s="25" t="s">
         <v>137</v>
       </c>
@@ -1817,7 +1868,7 @@
       <c r="B22" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="33" t="s">
         <v>139</v>
       </c>
       <c r="D22" s="25" t="s">
@@ -1850,7 +1901,7 @@
       <c r="B23" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="29"/>
+      <c r="C23" s="33"/>
       <c r="D23" s="25" t="s">
         <v>142</v>
       </c>
@@ -1879,7 +1930,7 @@
       <c r="B24" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="29"/>
+      <c r="C24" s="33"/>
       <c r="D24" s="25" t="s">
         <v>144</v>
       </c>
@@ -1908,7 +1959,7 @@
       <c r="B25" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="29"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="25" t="s">
         <v>10</v>
       </c>
@@ -1939,7 +1990,7 @@
       <c r="B26" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="29"/>
+      <c r="C26" s="33"/>
       <c r="D26" s="25" t="s">
         <v>147</v>
       </c>
@@ -1970,7 +2021,7 @@
       <c r="B27" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="29"/>
+      <c r="C27" s="33"/>
       <c r="D27" s="25" t="s">
         <v>11</v>
       </c>
@@ -1999,7 +2050,7 @@
       <c r="B28" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="29"/>
+      <c r="C28" s="33"/>
       <c r="D28" s="25" t="s">
         <v>150</v>
       </c>
@@ -2028,7 +2079,7 @@
       <c r="B29" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="35" t="s">
         <v>152</v>
       </c>
       <c r="D29" s="25" t="s">
@@ -2061,7 +2112,7 @@
       <c r="B30" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="32"/>
+      <c r="C30" s="36"/>
       <c r="D30" s="25" t="s">
         <v>154</v>
       </c>
@@ -2094,7 +2145,7 @@
       <c r="B31" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="32"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="25" t="s">
         <v>155</v>
       </c>
@@ -2123,7 +2174,7 @@
       <c r="B32" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="32"/>
+      <c r="C32" s="36"/>
       <c r="D32" s="25" t="s">
         <v>156</v>
       </c>
@@ -2156,7 +2207,7 @@
       <c r="B33" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="32"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="25" t="s">
         <v>158</v>
       </c>
@@ -2187,7 +2238,7 @@
       <c r="B34" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="32"/>
+      <c r="C34" s="36"/>
       <c r="D34" s="25" t="s">
         <v>160</v>
       </c>
@@ -2220,7 +2271,7 @@
       <c r="B35" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="32"/>
+      <c r="C35" s="36"/>
       <c r="D35" s="25" t="s">
         <v>162</v>
       </c>
@@ -2253,7 +2304,7 @@
       <c r="B36" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="32"/>
+      <c r="C36" s="36"/>
       <c r="D36" s="25" t="s">
         <v>164</v>
       </c>
@@ -2282,7 +2333,7 @@
       <c r="B37" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="32"/>
+      <c r="C37" s="36"/>
       <c r="D37" s="25" t="s">
         <v>166</v>
       </c>
@@ -2309,7 +2360,7 @@
       <c r="B38" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="32"/>
+      <c r="C38" s="36"/>
       <c r="D38" s="25" t="s">
         <v>167</v>
       </c>
@@ -2338,7 +2389,7 @@
       <c r="B39" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="32"/>
+      <c r="C39" s="36"/>
       <c r="D39" s="25" t="s">
         <v>169</v>
       </c>
@@ -2367,7 +2418,7 @@
       <c r="B40" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="32"/>
+      <c r="C40" s="36"/>
       <c r="D40" s="25" t="s">
         <v>116</v>
       </c>
@@ -2394,7 +2445,7 @@
       <c r="B41" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="33"/>
+      <c r="C41" s="37"/>
       <c r="D41" s="25" t="s">
         <v>171</v>
       </c>
@@ -2421,7 +2472,7 @@
       <c r="B42" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C42" s="33" t="s">
         <v>172</v>
       </c>
       <c r="D42" s="25" t="s">
@@ -2456,7 +2507,7 @@
       <c r="B43" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="29"/>
+      <c r="C43" s="33"/>
       <c r="D43" s="25" t="s">
         <v>117</v>
       </c>
@@ -2485,7 +2536,7 @@
       <c r="B44" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="29"/>
+      <c r="C44" s="33"/>
       <c r="D44" s="25" t="s">
         <v>175</v>
       </c>
@@ -2514,7 +2565,7 @@
       <c r="B45" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="29"/>
+      <c r="C45" s="33"/>
       <c r="D45" s="25" t="s">
         <v>177</v>
       </c>
@@ -2543,7 +2594,7 @@
       <c r="B46" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="29"/>
+      <c r="C46" s="33"/>
       <c r="D46" s="25" t="s">
         <v>178</v>
       </c>
@@ -2569,12 +2620,12 @@
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2587,7 +2638,7 @@
       <c r="B48" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="29" t="s">
+      <c r="C48" s="33" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="25" t="s">
@@ -2618,7 +2669,7 @@
       <c r="B49" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="29"/>
+      <c r="C49" s="33"/>
       <c r="D49" s="25" t="s">
         <v>17</v>
       </c>
@@ -2630,11 +2681,11 @@
       </c>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
-      <c r="I49" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>28</v>
+      <c r="I49" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="K49" s="3" t="s">
         <v>28</v>
@@ -2647,7 +2698,7 @@
       <c r="B50" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="29"/>
+      <c r="C50" s="33"/>
       <c r="D50" s="25" t="s">
         <v>18</v>
       </c>
@@ -2659,11 +2710,11 @@
       </c>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
-      <c r="I50" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>28</v>
+      <c r="I50" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="K50" s="3" t="s">
         <v>28</v>
@@ -2676,7 +2727,7 @@
       <c r="B51" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="29"/>
+      <c r="C51" s="33"/>
       <c r="D51" s="25" t="s">
         <v>182</v>
       </c>
@@ -2688,11 +2739,11 @@
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
-      <c r="I51" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>28</v>
+      <c r="I51" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="K51" s="3" t="s">
         <v>28</v>
@@ -2705,7 +2756,7 @@
       <c r="B52" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="29"/>
+      <c r="C52" s="33"/>
       <c r="D52" s="25" t="s">
         <v>183</v>
       </c>
@@ -2715,11 +2766,11 @@
       </c>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
-      <c r="I52" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>28</v>
+      <c r="I52" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="K52" s="3" t="s">
         <v>28</v>
@@ -2732,7 +2783,7 @@
       <c r="B53" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="29"/>
+      <c r="C53" s="33"/>
       <c r="D53" s="25" t="s">
         <v>184</v>
       </c>
@@ -2744,11 +2795,11 @@
       </c>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
-      <c r="I53" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>28</v>
+      <c r="I53" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="K53" s="3" t="s">
         <v>28</v>
@@ -2761,7 +2812,7 @@
       <c r="B54" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="29" t="s">
+      <c r="C54" s="33" t="s">
         <v>54</v>
       </c>
       <c r="D54" s="25" t="s">
@@ -2794,7 +2845,7 @@
       <c r="B55" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="29"/>
+      <c r="C55" s="33"/>
       <c r="D55" s="25" t="s">
         <v>44</v>
       </c>
@@ -2825,7 +2876,7 @@
       <c r="B56" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="29"/>
+      <c r="C56" s="33"/>
       <c r="D56" s="25" t="s">
         <v>187</v>
       </c>
@@ -2854,7 +2905,7 @@
       <c r="B57" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="29" t="s">
+      <c r="C57" s="33" t="s">
         <v>55</v>
       </c>
       <c r="D57" s="25" t="s">
@@ -2889,7 +2940,7 @@
       <c r="B58" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="29"/>
+      <c r="C58" s="33"/>
       <c r="D58" s="25" t="s">
         <v>190</v>
       </c>
@@ -2916,7 +2967,7 @@
       <c r="B59" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="C59" s="29"/>
+      <c r="C59" s="33"/>
       <c r="D59" s="25" t="s">
         <v>192</v>
       </c>
@@ -2945,7 +2996,7 @@
       <c r="B60" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="29"/>
+      <c r="C60" s="33"/>
       <c r="D60" s="25" t="s">
         <v>19</v>
       </c>
@@ -2978,7 +3029,7 @@
       <c r="B61" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="C61" s="29"/>
+      <c r="C61" s="33"/>
       <c r="D61" s="25" t="s">
         <v>195</v>
       </c>
@@ -3009,7 +3060,7 @@
       <c r="B62" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="29"/>
+      <c r="C62" s="33"/>
       <c r="D62" s="25" t="s">
         <v>196</v>
       </c>
@@ -3042,7 +3093,7 @@
       <c r="B63" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="C63" s="29" t="s">
+      <c r="C63" s="33" t="s">
         <v>57</v>
       </c>
       <c r="D63" s="25" t="s">
@@ -3077,7 +3128,7 @@
       <c r="B64" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="C64" s="29"/>
+      <c r="C64" s="33"/>
       <c r="D64" s="25" t="s">
         <v>200</v>
       </c>
@@ -3110,7 +3161,7 @@
       <c r="B65" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="C65" s="29"/>
+      <c r="C65" s="33"/>
       <c r="D65" s="25" t="s">
         <v>203</v>
       </c>
@@ -3139,7 +3190,7 @@
       <c r="B66" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="C66" s="29"/>
+      <c r="C66" s="33"/>
       <c r="D66" s="25" t="s">
         <v>206</v>
       </c>
@@ -3166,7 +3217,7 @@
       <c r="B67" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="C67" s="29" t="s">
+      <c r="C67" s="33" t="s">
         <v>58</v>
       </c>
       <c r="D67" s="25" t="s">
@@ -3201,7 +3252,7 @@
       <c r="B68" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="C68" s="29"/>
+      <c r="C68" s="33"/>
       <c r="D68" s="25" t="s">
         <v>211</v>
       </c>
@@ -3232,7 +3283,7 @@
       <c r="B69" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="C69" s="29"/>
+      <c r="C69" s="33"/>
       <c r="D69" s="25" t="s">
         <v>214</v>
       </c>
@@ -3262,10 +3313,10 @@
       </c>
     </row>
     <row r="70" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B70" s="30" t="s">
+      <c r="B70" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="C70" s="29" t="s">
+      <c r="C70" s="33" t="s">
         <v>59</v>
       </c>
       <c r="D70" s="25" t="s">
@@ -3274,84 +3325,81 @@
       <c r="E70" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="F70" s="26" t="s">
+      <c r="F70" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G70" s="26"/>
-      <c r="H70" s="26"/>
-      <c r="I70" s="27" t="s">
+      <c r="G70" s="27"/>
+      <c r="H70" s="27"/>
+      <c r="I70" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="J70" s="27" t="s">
+      <c r="J70" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="K70" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="L70" s="28" t="s">
+      <c r="K70" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="L70" s="32" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="71" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B71" s="30"/>
-      <c r="C71" s="29"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="33"/>
       <c r="D71" s="25" t="s">
         <v>218</v>
       </c>
       <c r="E71" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="F71" s="26"/>
-      <c r="G71" s="26"/>
-      <c r="H71" s="26"/>
-      <c r="I71" s="27"/>
-      <c r="J71" s="27"/>
-      <c r="K71" s="36"/>
-      <c r="L71" s="28"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="27"/>
+      <c r="H71" s="27"/>
+      <c r="I71" s="28"/>
+      <c r="J71" s="28"/>
+      <c r="K71" s="30"/>
+      <c r="L71" s="32"/>
     </row>
     <row r="72" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B72" s="30"/>
-      <c r="C72" s="29"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="33"/>
       <c r="D72" s="25" t="s">
         <v>220</v>
       </c>
       <c r="E72" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="F72" s="26"/>
-      <c r="G72" s="26"/>
-      <c r="H72" s="26"/>
-      <c r="I72" s="27"/>
-      <c r="J72" s="27"/>
-      <c r="K72" s="36"/>
-      <c r="L72" s="28"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="27"/>
+      <c r="H72" s="27"/>
+      <c r="I72" s="28"/>
+      <c r="J72" s="28"/>
+      <c r="K72" s="30"/>
+      <c r="L72" s="32"/>
     </row>
     <row r="73" spans="2:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="B73" s="30"/>
-      <c r="C73" s="29"/>
+      <c r="B73" s="34"/>
+      <c r="C73" s="33"/>
       <c r="D73" s="25" t="s">
         <v>222</v>
       </c>
       <c r="E73" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="F73" s="26"/>
-      <c r="G73" s="26"/>
-      <c r="H73" s="26"/>
-      <c r="I73" s="27"/>
-      <c r="J73" s="27"/>
-      <c r="K73" s="37"/>
-      <c r="L73" s="28"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="27"/>
+      <c r="H73" s="27"/>
+      <c r="I73" s="28"/>
+      <c r="J73" s="28"/>
+      <c r="K73" s="31"/>
+      <c r="L73" s="32"/>
     </row>
   </sheetData>
   <autoFilter ref="F5:L73"/>
   <dataConsolidate/>
   <mergeCells count="23">
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="G70:G73"/>
-    <mergeCell ref="H70:H73"/>
-    <mergeCell ref="I70:I73"/>
-    <mergeCell ref="J70:J73"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C62"/>
     <mergeCell ref="K70:K73"/>
     <mergeCell ref="L70:L73"/>
     <mergeCell ref="C22:C28"/>
@@ -3368,8 +3416,11 @@
     <mergeCell ref="C42:C46"/>
     <mergeCell ref="B47:E47"/>
     <mergeCell ref="C48:C53"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C57:C62"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="G70:G73"/>
+    <mergeCell ref="H70:H73"/>
+    <mergeCell ref="I70:I73"/>
+    <mergeCell ref="J70:J73"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:J73 L7:L73 K7:K70">
@@ -3412,7 +3463,7 @@
       </c>
       <c r="C3" s="9">
         <f>COUNTIF(Sheet1!I7:I73, "In Progress")</f>
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3421,7 +3472,7 @@
       </c>
       <c r="C4" s="2">
         <f>COUNTIF(Sheet1!I7:I73, "Not Start")</f>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3437,8 +3488,8 @@
       <c r="A6" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
@@ -3446,7 +3497,7 @@
       </c>
       <c r="C7" s="10">
         <f>COUNTIF(Sheet1!J7:J73,"Done")</f>
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3464,7 +3515,7 @@
       </c>
       <c r="C9" s="2">
         <f>COUNTIF(Sheet1!J7:J73, "Not Start")</f>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
DangVH: Commit lại update tiến độ dự án
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -1341,7 +1341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
@@ -3438,7 +3438,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
[Doc]_Delete unecessary files and update document
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -1,29 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Capstone\WIP\Users\HuyenPT\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
-    <sheet name="TỔNG HỢP" sheetId="7" r:id="rId2"/>
+    <sheet name="CODE-TC-SRS" sheetId="8" r:id="rId1"/>
+    <sheet name="DOC" sheetId="9" r:id="rId2"/>
+    <sheet name="TỔNG HỢP" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$5:$L$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CODE-TC-SRS'!$F$5:$L$73</definedName>
   </definedNames>
-  <calcPr calcId="162913" refMode="R1C1"/>
+  <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="283">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -721,12 +717,185 @@
   <si>
     <t>DESIGN</t>
   </si>
+  <si>
+    <t>YenNTH
+HaiCM</t>
+  </si>
+  <si>
+    <t>Prototype</t>
+  </si>
+  <si>
+    <t>Architecture Design</t>
+  </si>
+  <si>
+    <t>HuyenPT
+VanTTC</t>
+  </si>
+  <si>
+    <t>Class Design</t>
+  </si>
+  <si>
+    <t>Data Design</t>
+  </si>
+  <si>
+    <t>YenNTH</t>
+  </si>
+  <si>
+    <t>Screen Design</t>
+  </si>
+  <si>
+    <t>HaiCM</t>
+  </si>
+  <si>
+    <t>Risk Management Plan</t>
+  </si>
+  <si>
+    <t>DangVH
+VanTTC</t>
+  </si>
+  <si>
+    <t>Project Schedule</t>
+  </si>
+  <si>
+    <t>CM Plan</t>
+  </si>
+  <si>
+    <t>Project Plan</t>
+  </si>
+  <si>
+    <t>Project Introduction</t>
+  </si>
+  <si>
+    <t>Test Report</t>
+  </si>
+  <si>
+    <t>Test Result</t>
+  </si>
+  <si>
+    <t>DangVH
+HuyenPT
+VanTTC</t>
+  </si>
+  <si>
+    <t>Unit Test Case</t>
+  </si>
+  <si>
+    <t>System Test Case</t>
+  </si>
+  <si>
+    <t>Test Plan</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Slides for final presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Project Result Assessment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> User guideline</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Installation guide</t>
+  </si>
+  <si>
+    <t>Final documents + source codes</t>
+  </si>
+  <si>
+    <t>Report 06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Progress Report (cho giai doan coding in Construction)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quality Report</t>
+  </si>
+  <si>
+    <t>Test Report, Test result</t>
+  </si>
+  <si>
+    <t>Report 05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UT Review Check List</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UT Cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Code review checklist</t>
+  </si>
+  <si>
+    <t>Source codes</t>
+  </si>
+  <si>
+    <t>Report 04</t>
+  </si>
+  <si>
+    <t>Progress Report cho giai doan 3 (Phan Construction co lam Test Case, Plan)</t>
+  </si>
+  <si>
+    <t>Review checklist (cho test cases, Test Plan)</t>
+  </si>
+  <si>
+    <t>Test Cases (System Test case, Integration test cases)</t>
+  </si>
+  <si>
+    <t>Report 03</t>
+  </si>
+  <si>
+    <t>Design review checklists</t>
+  </si>
+  <si>
+    <t>Progress Report cho giai doan 2 (bang tieng Nhat)</t>
+  </si>
+  <si>
+    <t>Class/Component Design</t>
+  </si>
+  <si>
+    <t>Database Design</t>
+  </si>
+  <si>
+    <t>Report 02</t>
+  </si>
+  <si>
+    <t>SRS , PP Review check list</t>
+  </si>
+  <si>
+    <t>Progress Report cho giai doan 1 (bang tieng Nhat)</t>
+  </si>
+  <si>
+    <t>Q&amp;A Sheet bang tieng Nhat</t>
+  </si>
+  <si>
+    <t>SRS =&gt; User</t>
+  </si>
+  <si>
+    <t>Project Plan in MS Word</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>Report 01</t>
+  </si>
+  <si>
+    <t>PIC</t>
+  </si>
+  <si>
+    <t>Doc</t>
+  </si>
+  <si>
+    <t>DOC:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -784,8 +953,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -815,18 +991,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -886,6 +1074,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -893,7 +1094,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -903,14 +1104,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -923,13 +1123,13 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
@@ -942,10 +1142,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -954,9 +1154,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -970,6 +1169,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -982,15 +1193,65 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1061,7 +1322,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1094,26 +1355,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1146,23 +1390,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1341,9 +1568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K63" sqref="K63"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1371,66 +1596,66 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="12"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="12"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="24" t="s">
         <v>119</v>
       </c>
       <c r="F7" s="7" t="s">
@@ -1445,25 +1670,25 @@
       <c r="I7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="L7" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="25" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>120</v>
       </c>
       <c r="F8" s="7" t="s">
@@ -1478,23 +1703,23 @@
       <c r="I8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L8" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1504,16 +1729,16 @@
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="24" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="7" t="s">
@@ -1528,25 +1753,25 @@
       <c r="I10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="25" t="s">
+      <c r="C11" s="30"/>
+      <c r="D11" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="24" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="7" t="s">
@@ -1567,19 +1792,19 @@
       <c r="K11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="25" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="24" t="s">
         <v>124</v>
       </c>
       <c r="F12" s="7" t="s">
@@ -1592,25 +1817,25 @@
       <c r="I12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="25" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="24" t="s">
         <v>125</v>
       </c>
       <c r="F13" s="7" t="s">
@@ -1621,25 +1846,25 @@
       <c r="I13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L13" s="19" t="s">
+      <c r="L13" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="25" t="s">
+      <c r="C14" s="30"/>
+      <c r="D14" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="24" t="s">
         <v>127</v>
       </c>
       <c r="F14" s="7" t="s">
@@ -1650,27 +1875,27 @@
       <c r="I14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="L14" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="24" t="s">
         <v>129</v>
       </c>
       <c r="F15" s="7" t="s">
@@ -1683,21 +1908,21 @@
       <c r="I15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="J15" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="L15" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="27"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="25" t="s">
         <v>130</v>
       </c>
@@ -1707,30 +1932,30 @@
       <c r="F16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="J16" s="18" t="s">
+      <c r="G16" s="16"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="17" t="s">
         <v>27</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="L16" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="25" t="s">
+      <c r="C17" s="30"/>
+      <c r="D17" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="24" t="s">
         <v>133</v>
       </c>
       <c r="F17" s="7" t="s">
@@ -1747,19 +1972,19 @@
       <c r="K17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="L17" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="30"/>
+      <c r="D18" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="24" t="s">
         <v>135</v>
       </c>
       <c r="F18" s="7" t="s">
@@ -1776,19 +2001,19 @@
       <c r="K18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="13" t="s">
+      <c r="L18" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="25" t="s">
+      <c r="C19" s="30"/>
+      <c r="D19" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="24" t="s">
         <v>136</v>
       </c>
       <c r="F19" s="7" t="s">
@@ -1796,7 +2021,7 @@
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="18" t="s">
+      <c r="I19" s="17" t="s">
         <v>27</v>
       </c>
       <c r="J19" s="4" t="s">
@@ -1805,26 +2030,26 @@
       <c r="K19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L19" s="13" t="s">
+      <c r="L19" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="25" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
       <c r="I20" s="4" t="s">
         <v>26</v>
       </c>
@@ -1834,26 +2059,26 @@
       <c r="K20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="13" t="s">
+      <c r="L20" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="25" t="s">
+      <c r="C21" s="30"/>
+      <c r="D21" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E21" s="24" t="s">
         <v>138</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
       <c r="I21" s="5" t="s">
         <v>27</v>
       </c>
@@ -1863,21 +2088,21 @@
       <c r="K21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L21" s="13" t="s">
+      <c r="L21" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="24" t="s">
         <v>141</v>
       </c>
       <c r="F22" s="7" t="s">
@@ -1896,15 +2121,15 @@
       <c r="K22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L22" s="19" t="s">
+      <c r="L22" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="27"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="25" t="s">
         <v>142</v>
       </c>
@@ -1925,19 +2150,19 @@
       <c r="K23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L23" s="19" t="s">
+      <c r="L23" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="25" t="s">
+      <c r="C24" s="30"/>
+      <c r="D24" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="24" t="s">
         <v>145</v>
       </c>
       <c r="F24" s="7" t="s">
@@ -1954,19 +2179,19 @@
       <c r="K24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L24" s="19" t="s">
+      <c r="L24" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="25" t="s">
+      <c r="C25" s="30"/>
+      <c r="D25" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="24" t="s">
         <v>146</v>
       </c>
       <c r="F25" s="7" t="s">
@@ -1985,19 +2210,19 @@
       <c r="K25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L25" s="19" t="s">
+      <c r="L25" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="25" t="s">
+      <c r="C26" s="30"/>
+      <c r="D26" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="24" t="s">
         <v>148</v>
       </c>
       <c r="F26" s="7" t="s">
@@ -2016,19 +2241,19 @@
       <c r="K26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L26" s="19" t="s">
+      <c r="L26" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="25" t="s">
+      <c r="C27" s="30"/>
+      <c r="D27" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="24" t="s">
         <v>149</v>
       </c>
       <c r="F27" s="7" t="s">
@@ -2045,15 +2270,15 @@
       <c r="K27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L27" s="19" t="s">
+      <c r="L27" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="28" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="27"/>
+      <c r="C28" s="30"/>
       <c r="D28" s="25" t="s">
         <v>150</v>
       </c>
@@ -2063,8 +2288,8 @@
       <c r="F28" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
       <c r="I28" s="5" t="s">
         <v>27</v>
       </c>
@@ -2079,16 +2304,16 @@
       </c>
     </row>
     <row r="29" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="24" t="s">
         <v>153</v>
       </c>
       <c r="F29" s="7" t="s">
@@ -2107,19 +2332,19 @@
       <c r="K29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L29" s="13" t="s">
+      <c r="L29" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="34"/>
-      <c r="D30" s="25" t="s">
+      <c r="C30" s="36"/>
+      <c r="D30" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="24" t="s">
         <v>13</v>
       </c>
       <c r="F30" s="7" t="s">
@@ -2140,26 +2365,26 @@
       <c r="K30" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L30" s="13" t="s">
+      <c r="L30" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="25" t="s">
+      <c r="C31" s="36"/>
+      <c r="D31" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="23" t="s">
+      <c r="E31" s="24"/>
+      <c r="F31" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G31" s="16">
+      <c r="G31" s="15">
         <v>42411</v>
       </c>
-      <c r="H31" s="23"/>
+      <c r="H31" s="22"/>
       <c r="I31" s="4" t="s">
         <v>26</v>
       </c>
@@ -2169,19 +2394,19 @@
       <c r="K31" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L31" s="13" t="s">
+      <c r="L31" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="25" t="s">
+      <c r="C32" s="36"/>
+      <c r="D32" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="24" t="s">
         <v>157</v>
       </c>
       <c r="F32" s="7" t="s">
@@ -2202,19 +2427,19 @@
       <c r="K32" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L32" s="13" t="s">
+      <c r="L32" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="25" t="s">
+      <c r="C33" s="36"/>
+      <c r="D33" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="E33" s="25" t="s">
+      <c r="E33" s="24" t="s">
         <v>159</v>
       </c>
       <c r="F33" s="7" t="s">
@@ -2227,25 +2452,25 @@
       <c r="I33" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J33" s="13" t="s">
+      <c r="J33" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L33" s="13" t="s">
+      <c r="L33" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="34"/>
-      <c r="D34" s="25" t="s">
+      <c r="C34" s="36"/>
+      <c r="D34" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E34" s="24" t="s">
         <v>161</v>
       </c>
       <c r="F34" s="7" t="s">
@@ -2260,25 +2485,25 @@
       <c r="I34" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J34" s="13" t="s">
+      <c r="J34" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L34" s="13" t="s">
+      <c r="L34" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="35" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="25" t="s">
+      <c r="C35" s="36"/>
+      <c r="D35" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E35" s="25" t="s">
+      <c r="E35" s="24" t="s">
         <v>163</v>
       </c>
       <c r="F35" s="7" t="s">
@@ -2293,21 +2518,21 @@
       <c r="I35" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J35" s="13" t="s">
+      <c r="J35" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L35" s="13" t="s">
+      <c r="L35" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="36" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="34"/>
+      <c r="C36" s="36"/>
       <c r="D36" s="25" t="s">
         <v>164</v>
       </c>
@@ -2322,21 +2547,21 @@
       <c r="I36" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J36" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="L36" s="13" t="s">
+      <c r="J36" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L36" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="34"/>
+      <c r="C37" s="36"/>
       <c r="D37" s="25" t="s">
         <v>166</v>
       </c>
@@ -2349,21 +2574,21 @@
       <c r="I37" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K37" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="L37" s="13" t="s">
+      <c r="J37" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L37" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="34"/>
+      <c r="C38" s="36"/>
       <c r="D38" s="25" t="s">
         <v>167</v>
       </c>
@@ -2378,21 +2603,21 @@
       <c r="I38" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J38" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K38" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="L38" s="13" t="s">
+      <c r="J38" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L38" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="34"/>
+      <c r="C39" s="36"/>
       <c r="D39" s="25" t="s">
         <v>169</v>
       </c>
@@ -2407,21 +2632,21 @@
       <c r="I39" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J39" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K39" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="L39" s="13" t="s">
+      <c r="J39" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L39" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="24" t="s">
+      <c r="B40" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="34"/>
+      <c r="C40" s="36"/>
       <c r="D40" s="25" t="s">
         <v>116</v>
       </c>
@@ -2434,21 +2659,21 @@
       <c r="I40" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J40" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K40" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="L40" s="13" t="s">
+      <c r="J40" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K40" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L40" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="41" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="35"/>
+      <c r="C41" s="37"/>
       <c r="D41" s="25" t="s">
         <v>171</v>
       </c>
@@ -2461,27 +2686,27 @@
       <c r="I41" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J41" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K41" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="L41" s="13" t="s">
+      <c r="J41" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K41" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L41" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="D42" s="25" t="s">
+      <c r="D42" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E42" s="25" t="s">
+      <c r="E42" s="24" t="s">
         <v>173</v>
       </c>
       <c r="F42" s="7" t="s">
@@ -2496,25 +2721,25 @@
       <c r="I42" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J42" s="13" t="s">
+      <c r="J42" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K42" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L42" s="13" t="s">
+      <c r="L42" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="25" t="s">
+      <c r="C43" s="30"/>
+      <c r="D43" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="E43" s="25" t="s">
+      <c r="E43" s="24" t="s">
         <v>174</v>
       </c>
       <c r="F43" s="7" t="s">
@@ -2525,25 +2750,25 @@
       <c r="I43" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J43" s="13" t="s">
+      <c r="J43" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K43" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L43" s="19" t="s">
+      <c r="L43" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="44" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="27"/>
-      <c r="D44" s="25" t="s">
+      <c r="C44" s="30"/>
+      <c r="D44" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="E44" s="25" t="s">
+      <c r="E44" s="24" t="s">
         <v>176</v>
       </c>
       <c r="F44" s="7" t="s">
@@ -2554,54 +2779,54 @@
       <c r="I44" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="13" t="s">
+      <c r="J44" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K44" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L44" s="19" t="s">
+      <c r="L44" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="45" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="27"/>
+      <c r="C45" s="30"/>
       <c r="D45" s="25" t="s">
         <v>177</v>
       </c>
       <c r="E45" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="F45" s="22" t="s">
+      <c r="F45" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="J45" s="20" t="s">
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J45" s="19" t="s">
         <v>26</v>
       </c>
       <c r="K45" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L45" s="19" t="s">
+      <c r="L45" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="46" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B46" s="24" t="s">
+      <c r="B46" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="27"/>
-      <c r="D46" s="25" t="s">
+      <c r="C46" s="30"/>
+      <c r="D46" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="E46" s="25" t="s">
+      <c r="E46" s="24" t="s">
         <v>179</v>
       </c>
       <c r="F46" s="7" t="s">
@@ -2618,17 +2843,17 @@
       <c r="K46" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L46" s="19" t="s">
+      <c r="L46" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="32" t="s">
+      <c r="B47" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2638,10 +2863,10 @@
       <c r="L47" s="2"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="24" t="s">
+      <c r="B48" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="27" t="s">
+      <c r="C48" s="30" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="25" t="s">
@@ -2664,19 +2889,19 @@
       <c r="K48" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L48" s="19" t="s">
+      <c r="L48" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="49" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B49" s="24" t="s">
+      <c r="B49" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="27"/>
-      <c r="D49" s="25" t="s">
+      <c r="C49" s="30"/>
+      <c r="D49" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E49" s="25" t="s">
+      <c r="E49" s="24" t="s">
         <v>181</v>
       </c>
       <c r="F49" s="7" t="s">
@@ -2693,19 +2918,19 @@
       <c r="K49" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L49" s="19" t="s">
+      <c r="L49" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="25" t="s">
+      <c r="C50" s="30"/>
+      <c r="D50" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E50" s="25" t="s">
+      <c r="E50" s="24" t="s">
         <v>18</v>
       </c>
       <c r="F50" s="7" t="s">
@@ -2722,19 +2947,19 @@
       <c r="K50" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L50" s="19" t="s">
+      <c r="L50" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="51" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B51" s="24" t="s">
+      <c r="B51" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="27"/>
-      <c r="D51" s="25" t="s">
+      <c r="C51" s="30"/>
+      <c r="D51" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="E51" s="25" t="s">
+      <c r="E51" s="24" t="s">
         <v>181</v>
       </c>
       <c r="F51" s="7" t="s">
@@ -2751,19 +2976,19 @@
       <c r="K51" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L51" s="19" t="s">
+      <c r="L51" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="52" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="27"/>
-      <c r="D52" s="25" t="s">
+      <c r="C52" s="30"/>
+      <c r="D52" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="E52" s="25"/>
+      <c r="E52" s="24"/>
       <c r="F52" s="7" t="s">
         <v>30</v>
       </c>
@@ -2778,19 +3003,19 @@
       <c r="K52" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L52" s="19" t="s">
+      <c r="L52" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="53" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="24" t="s">
+      <c r="B53" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="27"/>
-      <c r="D53" s="25" t="s">
+      <c r="C53" s="30"/>
+      <c r="D53" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="E53" s="25" t="s">
+      <c r="E53" s="24" t="s">
         <v>185</v>
       </c>
       <c r="F53" s="7" t="s">
@@ -2807,21 +3032,21 @@
       <c r="K53" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L53" s="19" t="s">
+      <c r="L53" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="54" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B54" s="24" t="s">
+      <c r="B54" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="27" t="s">
+      <c r="C54" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="25" t="s">
+      <c r="D54" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E54" s="25" t="s">
+      <c r="E54" s="24" t="s">
         <v>186</v>
       </c>
       <c r="F54" s="7" t="s">
@@ -2834,25 +3059,25 @@
       <c r="I54" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J54" s="13" t="s">
+      <c r="J54" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K54" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L54" s="19" t="s">
+      <c r="L54" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B55" s="24" t="s">
+      <c r="B55" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="27"/>
-      <c r="D55" s="25" t="s">
+      <c r="C55" s="30"/>
+      <c r="D55" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E55" s="25" t="s">
+      <c r="E55" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F55" s="7" t="s">
@@ -2865,25 +3090,25 @@
       <c r="I55" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J55" s="13" t="s">
+      <c r="J55" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K55" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L55" s="19" t="s">
+      <c r="L55" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="56" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B56" s="24" t="s">
+      <c r="B56" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="27"/>
-      <c r="D56" s="25" t="s">
+      <c r="C56" s="30"/>
+      <c r="D56" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="E56" s="25"/>
+      <c r="E56" s="24"/>
       <c r="F56" s="7" t="s">
         <v>30</v>
       </c>
@@ -2894,27 +3119,27 @@
       <c r="I56" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J56" s="13" t="s">
+      <c r="J56" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K56" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L56" s="19" t="s">
+      <c r="L56" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B57" s="24" t="s">
+      <c r="B57" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="27" t="s">
+      <c r="C57" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D57" s="25" t="s">
+      <c r="D57" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="E57" s="25" t="s">
+      <c r="E57" s="24" t="s">
         <v>189</v>
       </c>
       <c r="F57" s="7" t="s">
@@ -2935,19 +3160,19 @@
       <c r="K57" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L57" s="19" t="s">
+      <c r="L57" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="24" t="s">
+      <c r="B58" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="27"/>
-      <c r="D58" s="25" t="s">
+      <c r="C58" s="30"/>
+      <c r="D58" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="E58" s="25" t="s">
+      <c r="E58" s="24" t="s">
         <v>191</v>
       </c>
       <c r="F58" s="7" t="s">
@@ -2964,25 +3189,25 @@
       <c r="K58" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L58" s="19"/>
+      <c r="L58" s="18"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B59" s="24" t="s">
+      <c r="B59" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C59" s="27"/>
-      <c r="D59" s="25" t="s">
+      <c r="C59" s="30"/>
+      <c r="D59" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="E59" s="25" t="s">
+      <c r="E59" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="F59" s="22" t="s">
+      <c r="F59" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="18" t="s">
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="17" t="s">
         <v>27</v>
       </c>
       <c r="J59" s="3" t="s">
@@ -2991,19 +3216,19 @@
       <c r="K59" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L59" s="19" t="s">
+      <c r="L59" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B60" s="24" t="s">
+      <c r="B60" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="27"/>
-      <c r="D60" s="25" t="s">
+      <c r="C60" s="30"/>
+      <c r="D60" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E60" s="25" t="s">
+      <c r="E60" s="24" t="s">
         <v>194</v>
       </c>
       <c r="F60" s="7" t="s">
@@ -3024,19 +3249,19 @@
       <c r="K60" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L60" s="19" t="s">
+      <c r="L60" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B61" s="24" t="s">
+      <c r="B61" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C61" s="27"/>
-      <c r="D61" s="25" t="s">
+      <c r="C61" s="30"/>
+      <c r="D61" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="E61" s="25"/>
+      <c r="E61" s="24"/>
       <c r="F61" s="7" t="s">
         <v>30</v>
       </c>
@@ -3055,19 +3280,19 @@
       <c r="K61" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L61" s="19" t="s">
+      <c r="L61" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="62" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B62" s="24" t="s">
+      <c r="B62" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="27"/>
-      <c r="D62" s="25" t="s">
+      <c r="C62" s="30"/>
+      <c r="D62" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="E62" s="25" t="s">
+      <c r="E62" s="24" t="s">
         <v>20</v>
       </c>
       <c r="F62" s="7" t="s">
@@ -3088,21 +3313,21 @@
       <c r="K62" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L62" s="19" t="s">
+      <c r="L62" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B63" s="24" t="s">
+      <c r="B63" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="C63" s="27" t="s">
+      <c r="C63" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="D63" s="25" t="s">
+      <c r="D63" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="E63" s="25" t="s">
+      <c r="E63" s="24" t="s">
         <v>198</v>
       </c>
       <c r="F63" s="7" t="s">
@@ -3123,19 +3348,19 @@
       <c r="K63" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L63" s="19" t="s">
+      <c r="L63" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B64" s="24" t="s">
+      <c r="B64" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="C64" s="27"/>
-      <c r="D64" s="25" t="s">
+      <c r="C64" s="30"/>
+      <c r="D64" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="E64" s="25" t="s">
+      <c r="E64" s="24" t="s">
         <v>201</v>
       </c>
       <c r="F64" s="7" t="s">
@@ -3156,19 +3381,19 @@
       <c r="K64" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L64" s="19" t="s">
+      <c r="L64" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B65" s="24" t="s">
+      <c r="B65" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="C65" s="27"/>
-      <c r="D65" s="25" t="s">
+      <c r="C65" s="30"/>
+      <c r="D65" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="E65" s="25" t="s">
+      <c r="E65" s="24" t="s">
         <v>204</v>
       </c>
       <c r="F65" s="7" t="s">
@@ -3185,19 +3410,19 @@
       <c r="K65" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L65" s="19" t="s">
+      <c r="L65" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B66" s="24" t="s">
+      <c r="B66" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="C66" s="27"/>
-      <c r="D66" s="25" t="s">
+      <c r="C66" s="30"/>
+      <c r="D66" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="E66" s="25" t="s">
+      <c r="E66" s="24" t="s">
         <v>207</v>
       </c>
       <c r="F66" s="7" t="s">
@@ -3208,25 +3433,25 @@
       <c r="I66" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J66" s="13"/>
+      <c r="J66" s="12"/>
       <c r="K66" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L66" s="19" t="s">
+      <c r="L66" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B67" s="24" t="s">
+      <c r="B67" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="C67" s="27" t="s">
+      <c r="C67" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="D67" s="25" t="s">
+      <c r="D67" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="E67" s="25" t="s">
+      <c r="E67" s="24" t="s">
         <v>21</v>
       </c>
       <c r="F67" s="7" t="s">
@@ -3247,19 +3472,19 @@
       <c r="K67" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L67" s="19" t="s">
+      <c r="L67" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B68" s="24" t="s">
+      <c r="B68" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="C68" s="27"/>
-      <c r="D68" s="25" t="s">
+      <c r="C68" s="30"/>
+      <c r="D68" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="E68" s="25" t="s">
+      <c r="E68" s="24" t="s">
         <v>212</v>
       </c>
       <c r="F68" s="7" t="s">
@@ -3278,19 +3503,19 @@
       <c r="K68" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L68" s="19" t="s">
+      <c r="L68" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B69" s="24" t="s">
+      <c r="B69" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C69" s="27"/>
-      <c r="D69" s="25" t="s">
+      <c r="C69" s="30"/>
+      <c r="D69" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="E69" s="25" t="s">
+      <c r="E69" s="24" t="s">
         <v>22</v>
       </c>
       <c r="F69" s="7" t="s">
@@ -3311,91 +3536,91 @@
       <c r="K69" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L69" s="19" t="s">
+      <c r="L69" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="70" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B70" s="32" t="s">
+      <c r="B70" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="C70" s="27" t="s">
+      <c r="C70" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D70" s="25" t="s">
+      <c r="D70" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="E70" s="25" t="s">
+      <c r="E70" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="F70" s="36" t="s">
+      <c r="F70" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G70" s="36"/>
-      <c r="H70" s="36"/>
-      <c r="I70" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="J70" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="K70" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="L70" s="31" t="s">
+      <c r="G70" s="31"/>
+      <c r="H70" s="31"/>
+      <c r="I70" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="J70" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="K70" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="L70" s="29" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="71" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B71" s="32"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="25" t="s">
+      <c r="B71" s="34"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="E71" s="25" t="s">
+      <c r="E71" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="F71" s="36"/>
-      <c r="G71" s="36"/>
-      <c r="H71" s="36"/>
-      <c r="I71" s="37"/>
-      <c r="J71" s="38"/>
-      <c r="K71" s="29"/>
-      <c r="L71" s="31"/>
+      <c r="F71" s="31"/>
+      <c r="G71" s="31"/>
+      <c r="H71" s="31"/>
+      <c r="I71" s="32"/>
+      <c r="J71" s="33"/>
+      <c r="K71" s="27"/>
+      <c r="L71" s="29"/>
     </row>
     <row r="72" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B72" s="32"/>
-      <c r="C72" s="27"/>
-      <c r="D72" s="25" t="s">
+      <c r="B72" s="34"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="E72" s="25" t="s">
+      <c r="E72" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="F72" s="36"/>
-      <c r="G72" s="36"/>
-      <c r="H72" s="36"/>
-      <c r="I72" s="37"/>
-      <c r="J72" s="38"/>
-      <c r="K72" s="29"/>
-      <c r="L72" s="31"/>
+      <c r="F72" s="31"/>
+      <c r="G72" s="31"/>
+      <c r="H72" s="31"/>
+      <c r="I72" s="32"/>
+      <c r="J72" s="33"/>
+      <c r="K72" s="27"/>
+      <c r="L72" s="29"/>
     </row>
     <row r="73" spans="2:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="B73" s="32"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="25" t="s">
+      <c r="B73" s="34"/>
+      <c r="C73" s="30"/>
+      <c r="D73" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="E73" s="25" t="s">
+      <c r="E73" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="F73" s="36"/>
-      <c r="G73" s="36"/>
-      <c r="H73" s="36"/>
-      <c r="I73" s="37"/>
-      <c r="J73" s="38"/>
-      <c r="K73" s="30"/>
-      <c r="L73" s="31"/>
+      <c r="F73" s="31"/>
+      <c r="G73" s="31"/>
+      <c r="H73" s="31"/>
+      <c r="I73" s="32"/>
+      <c r="J73" s="33"/>
+      <c r="K73" s="28"/>
+      <c r="L73" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="F5:L73"/>
@@ -3407,13 +3632,13 @@
     <mergeCell ref="C42:C46"/>
     <mergeCell ref="B47:E47"/>
     <mergeCell ref="C48:C53"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C62"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="C10:C14"/>
     <mergeCell ref="C15:C21"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C57:C62"/>
     <mergeCell ref="K70:K73"/>
     <mergeCell ref="L70:L73"/>
     <mergeCell ref="C22:C28"/>
@@ -3426,7 +3651,7 @@
     <mergeCell ref="J70:J73"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:J73 L7:L73 K7:K70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K70 L7:L73 I7:J73">
       <formula1>$C$3:$E$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3436,186 +3661,849 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="B4:I50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="1" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="57.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="38" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="F4" s="59" t="s">
+        <v>280</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>279</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="D6" s="44"/>
+      <c r="E6" s="52" t="s">
+        <v>278</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="D7" s="44"/>
+      <c r="E7" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="44"/>
+      <c r="E8" s="52" t="s">
+        <v>239</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="44"/>
+      <c r="E9" s="52" t="s">
+        <v>276</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D10" s="44"/>
+      <c r="E10" s="52" t="s">
+        <v>275</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D11" s="44"/>
+      <c r="E11" s="52" t="s">
+        <v>274</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D12" s="41"/>
+      <c r="E12" s="52" t="s">
+        <v>273</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D13" s="56" t="s">
+        <v>272</v>
+      </c>
+      <c r="E13" s="57" t="s">
+        <v>229</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="55"/>
+      <c r="E14" s="57" t="s">
+        <v>234</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="55"/>
+      <c r="E15" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D16" s="55"/>
+      <c r="E16" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="F16" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D17" s="55"/>
+      <c r="E17" s="53" t="s">
+        <v>269</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="54"/>
+      <c r="E18" s="53" t="s">
+        <v>268</v>
+      </c>
+      <c r="F18" s="42"/>
+      <c r="G18" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="49" t="s">
+        <v>267</v>
+      </c>
+      <c r="E19" s="52" t="s">
+        <v>247</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D20" s="44"/>
+      <c r="E20" s="52" t="s">
+        <v>266</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D21" s="44"/>
+      <c r="E21" s="52" t="s">
+        <v>265</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D22" s="41"/>
+      <c r="E22" s="52" t="s">
+        <v>264</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D23" s="56" t="s">
+        <v>263</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>262</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>244</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D24" s="55"/>
+      <c r="E24" s="53" t="s">
+        <v>261</v>
+      </c>
+      <c r="F24" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="4:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D25" s="55"/>
+      <c r="E25" s="53" t="s">
+        <v>260</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>244</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="54"/>
+      <c r="E26" s="53" t="s">
+        <v>259</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D27" s="49" t="s">
+        <v>258</v>
+      </c>
+      <c r="E27" s="52" t="s">
+        <v>257</v>
+      </c>
+      <c r="F27" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D28" s="44"/>
+      <c r="E28" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="F28" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D29" s="41"/>
+      <c r="E29" s="52" t="s">
+        <v>255</v>
+      </c>
+      <c r="F29" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D30" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="E30" s="51" t="s">
+        <v>253</v>
+      </c>
+      <c r="F30" s="42"/>
+      <c r="G30" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="50"/>
+      <c r="E31" s="51" t="s">
+        <v>252</v>
+      </c>
+      <c r="F31" s="42"/>
+      <c r="G31" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D32" s="50"/>
+      <c r="E32" s="51" t="s">
+        <v>251</v>
+      </c>
+      <c r="F32" s="42"/>
+      <c r="G32" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D33" s="50"/>
+      <c r="E33" s="51" t="s">
+        <v>250</v>
+      </c>
+      <c r="F33" s="42"/>
+      <c r="G33" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="50"/>
+      <c r="E34" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F34" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D35" s="49" t="s">
+        <v>248</v>
+      </c>
+      <c r="E35" s="48" t="s">
+        <v>247</v>
+      </c>
+      <c r="F35" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D36" s="44"/>
+      <c r="E36" s="43" t="s">
+        <v>246</v>
+      </c>
+      <c r="F36" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D37" s="44"/>
+      <c r="E37" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="F37" s="39" t="s">
+        <v>244</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D38" s="44"/>
+      <c r="E38" s="45" t="s">
+        <v>243</v>
+      </c>
+      <c r="F38" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D39" s="44"/>
+      <c r="E39" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="F39" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D40" s="44"/>
+      <c r="E40" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="F40" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D41" s="44"/>
+      <c r="E41" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="F41" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D42" s="44"/>
+      <c r="E42" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="F42" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D43" s="44"/>
+      <c r="E43" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="F43" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D44" s="44"/>
+      <c r="E44" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F44" s="42"/>
+      <c r="G44" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I44" s="46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D45" s="44"/>
+      <c r="E45" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F45" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I45" s="46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D46" s="44"/>
+      <c r="E46" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="F46" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I46" s="46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D47" s="44"/>
+      <c r="E47" s="45" t="s">
+        <v>232</v>
+      </c>
+      <c r="F47" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D48" s="44"/>
+      <c r="E48" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="F48" s="39" t="s">
+        <v>230</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D49" s="44"/>
+      <c r="E49" s="43" t="s">
+        <v>229</v>
+      </c>
+      <c r="F49" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D50" s="41"/>
+      <c r="E50" s="40" t="s">
+        <v>228</v>
+      </c>
+      <c r="F50" s="39" t="s">
+        <v>227</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="D35:D50"/>
+    <mergeCell ref="D5:D12"/>
+    <mergeCell ref="D13:D18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="D30:D34"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G50">
+      <formula1>$I$44:$I$46</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F49 F24 F17:F22 F26:F35 F44:F47 F7:F15 F38:F42">
+      <formula1>$B$4:$B$8</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5">
+      <formula1>$B$4:$B$9</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:K13"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="60" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="60"/>
+    <col min="6" max="6" width="13.85546875" style="60" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="60" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="60"/>
+    <col min="10" max="10" width="12.42578125" style="60" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="60"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="10">
-        <f>COUNTIF(Sheet1!I7:I73,"Done")</f>
+      <c r="E4" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="66">
+        <f>COUNTIF('CODE-TC-SRS'!I7:I73,"Done")</f>
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="9">
-        <f>COUNTIF(Sheet1!I7:I73, "In Progress")</f>
+      <c r="F5" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="61">
+        <f>COUNTIF('CODE-TC-SRS'!K6:K78,"Done")</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="2">
-        <f>COUNTIF(Sheet1!I7:I73, "Not Start")</f>
+      <c r="J5" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="61">
+        <f>COUNTIF(DOC!G4:G49,"Done")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="9">
+        <f>COUNTIF('CODE-TC-SRS'!I7:I73, "In Progress")</f>
+        <v>24</v>
+      </c>
+      <c r="F6" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="63">
+        <f>COUNTIF('CODE-TC-SRS'!K6:K72,"In Progress")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="J6" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="63">
+        <f>COUNTIF(DOC!G4:G49,"In Progress")</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="9">
+        <f>COUNTIF('CODE-TC-SRS'!I7:I73, "Not Start")</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="63">
+        <f>COUNTIF('CODE-TC-SRS'!K6:K72, "Not Start")</f>
+        <v>38</v>
+      </c>
+      <c r="J7" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="63">
+        <f>COUNTIF(DOC!G4:G49, "Not Start")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="2">
-        <f>SUM(C2:C4)</f>
+      <c r="C8" s="9">
+        <f>SUM(C5:C7)</f>
         <v>62</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="F8" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="63">
+        <f>SUM(G5:G7)</f>
+        <v>62</v>
+      </c>
+      <c r="J8" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="63">
+        <f>SUM(K5:K7)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="s">
         <v>226</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-    </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="10">
-        <f>COUNTIF(Sheet1!J7:J73,"Done")</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="9">
-        <f>COUNTIF(Sheet1!J7:J73, "In Progress")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="2">
-        <f>COUNTIF(Sheet1!J7:J73, "Not Start")</f>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="E9" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="61">
+        <f>COUNTIF('CODE-TC-SRS'!J7:J73,"Done")</f>
+        <v>50</v>
+      </c>
+      <c r="F10" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="61">
+        <f>COUNTIF('CODE-TC-SRS'!L7:L73,"Done")</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="63">
+        <f>COUNTIF('CODE-TC-SRS'!J7:J73, "In Progress")</f>
+        <v>9</v>
+      </c>
+      <c r="F11" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="63">
+        <f>COUNTIF('CODE-TC-SRS'!L7:L73,"In Progress")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="63">
+        <f>COUNTIF('CODE-TC-SRS'!J7:J73, "Not Start")</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="F12" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="63">
+        <f>COUNTIF('CODE-TC-SRS'!L7:L73, "Not Start")</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2">
-        <f>SUM(C7:C9)</f>
+      <c r="C13" s="63">
+        <f>SUM(C10:C12)</f>
         <v>61</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="10">
-        <f>COUNTIF(Sheet1!K7:K73,"Done")</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="9">
-        <f>COUNTIF(Sheet1!K7:K73,"In Progress")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="2">
-        <f>COUNTIF(Sheet1!K7:K73, "Not Start")</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="F13" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="2">
-        <f>SUM(C12:C14)</f>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="10">
-        <f>COUNTIF(Sheet1!L7:L73,"Done")</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="9">
-        <f>COUNTIF(Sheet1!L7:L73,"In Progress")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="2">
-        <f>COUNTIF(Sheet1!L7:L73, "Not Start")</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="2">
-        <f>SUM(C17:C19)</f>
+      <c r="G13" s="63">
+        <f>SUM(G10:G12)</f>
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:C4">
+  <conditionalFormatting sqref="B5:C7">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:C12">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3627,7 +4515,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:C14">
+  <conditionalFormatting sqref="J5:K8">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3639,7 +4527,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:C19">
+  <conditionalFormatting sqref="F5:G8">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3651,7 +4539,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:C9">
+  <conditionalFormatting sqref="F10:G12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3664,5 +4552,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Doc]_Commit document for report 2
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7500"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CODE-TC-SRS" sheetId="8" r:id="rId1"/>
@@ -1157,6 +1157,59 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1169,9 +1222,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1181,77 +1231,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1568,7 +1568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1631,12 +1631,12 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1649,7 +1649,7 @@
       <c r="B7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="49" t="s">
         <v>118</v>
       </c>
       <c r="D7" s="24" t="s">
@@ -1684,7 +1684,7 @@
       <c r="B8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="49"/>
       <c r="D8" s="24" t="s">
         <v>8</v>
       </c>
@@ -1714,12 +1714,12 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1732,7 +1732,7 @@
       <c r="B10" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="49" t="s">
         <v>121</v>
       </c>
       <c r="D10" s="24" t="s">
@@ -1767,7 +1767,7 @@
       <c r="B11" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="24" t="s">
         <v>6</v>
       </c>
@@ -1800,7 +1800,7 @@
       <c r="B12" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="24" t="s">
         <v>123</v>
       </c>
@@ -1831,7 +1831,7 @@
       <c r="B13" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="30"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="24" t="s">
         <v>125</v>
       </c>
@@ -1860,7 +1860,7 @@
       <c r="B14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="24" t="s">
         <v>126</v>
       </c>
@@ -1889,7 +1889,7 @@
       <c r="B15" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="49" t="s">
         <v>128</v>
       </c>
       <c r="D15" s="24" t="s">
@@ -1922,7 +1922,7 @@
       <c r="B16" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="30"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="25" t="s">
         <v>130</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="B17" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="30"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="24" t="s">
         <v>132</v>
       </c>
@@ -1980,7 +1980,7 @@
       <c r="B18" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="30"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="24" t="s">
         <v>134</v>
       </c>
@@ -2009,7 +2009,7 @@
       <c r="B19" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="30"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="24" t="s">
         <v>48</v>
       </c>
@@ -2038,7 +2038,7 @@
       <c r="B20" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="30"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="24" t="s">
         <v>9</v>
       </c>
@@ -2067,7 +2067,7 @@
       <c r="B21" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="30"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="24" t="s">
         <v>137</v>
       </c>
@@ -2096,7 +2096,7 @@
       <c r="B22" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="49" t="s">
         <v>139</v>
       </c>
       <c r="D22" s="24" t="s">
@@ -2129,7 +2129,7 @@
       <c r="B23" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="30"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="25" t="s">
         <v>142</v>
       </c>
@@ -2158,7 +2158,7 @@
       <c r="B24" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="30"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="24" t="s">
         <v>144</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="B25" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="30"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="24" t="s">
         <v>10</v>
       </c>
@@ -2218,7 +2218,7 @@
       <c r="B26" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="30"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="24" t="s">
         <v>147</v>
       </c>
@@ -2249,7 +2249,7 @@
       <c r="B27" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="30"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="24" t="s">
         <v>11</v>
       </c>
@@ -2278,7 +2278,7 @@
       <c r="B28" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="30"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="25" t="s">
         <v>150</v>
       </c>
@@ -2307,7 +2307,7 @@
       <c r="B29" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="50" t="s">
         <v>152</v>
       </c>
       <c r="D29" s="24" t="s">
@@ -2340,7 +2340,7 @@
       <c r="B30" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="36"/>
+      <c r="C30" s="51"/>
       <c r="D30" s="24" t="s">
         <v>154</v>
       </c>
@@ -2373,7 +2373,7 @@
       <c r="B31" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="36"/>
+      <c r="C31" s="51"/>
       <c r="D31" s="24" t="s">
         <v>155</v>
       </c>
@@ -2402,7 +2402,7 @@
       <c r="B32" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="36"/>
+      <c r="C32" s="51"/>
       <c r="D32" s="24" t="s">
         <v>156</v>
       </c>
@@ -2435,7 +2435,7 @@
       <c r="B33" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="36"/>
+      <c r="C33" s="51"/>
       <c r="D33" s="24" t="s">
         <v>158</v>
       </c>
@@ -2466,7 +2466,7 @@
       <c r="B34" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="36"/>
+      <c r="C34" s="51"/>
       <c r="D34" s="24" t="s">
         <v>160</v>
       </c>
@@ -2499,7 +2499,7 @@
       <c r="B35" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="36"/>
+      <c r="C35" s="51"/>
       <c r="D35" s="24" t="s">
         <v>162</v>
       </c>
@@ -2532,7 +2532,7 @@
       <c r="B36" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="36"/>
+      <c r="C36" s="51"/>
       <c r="D36" s="25" t="s">
         <v>164</v>
       </c>
@@ -2561,7 +2561,7 @@
       <c r="B37" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="36"/>
+      <c r="C37" s="51"/>
       <c r="D37" s="25" t="s">
         <v>166</v>
       </c>
@@ -2588,7 +2588,7 @@
       <c r="B38" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="36"/>
+      <c r="C38" s="51"/>
       <c r="D38" s="25" t="s">
         <v>167</v>
       </c>
@@ -2617,7 +2617,7 @@
       <c r="B39" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="36"/>
+      <c r="C39" s="51"/>
       <c r="D39" s="25" t="s">
         <v>169</v>
       </c>
@@ -2646,7 +2646,7 @@
       <c r="B40" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="36"/>
+      <c r="C40" s="51"/>
       <c r="D40" s="25" t="s">
         <v>116</v>
       </c>
@@ -2673,7 +2673,7 @@
       <c r="B41" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="37"/>
+      <c r="C41" s="52"/>
       <c r="D41" s="25" t="s">
         <v>171</v>
       </c>
@@ -2700,7 +2700,7 @@
       <c r="B42" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="30" t="s">
+      <c r="C42" s="49" t="s">
         <v>172</v>
       </c>
       <c r="D42" s="24" t="s">
@@ -2735,7 +2735,7 @@
       <c r="B43" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="30"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="24" t="s">
         <v>117</v>
       </c>
@@ -2764,7 +2764,7 @@
       <c r="B44" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="30"/>
+      <c r="C44" s="49"/>
       <c r="D44" s="24" t="s">
         <v>175</v>
       </c>
@@ -2793,7 +2793,7 @@
       <c r="B45" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="30"/>
+      <c r="C45" s="49"/>
       <c r="D45" s="25" t="s">
         <v>177</v>
       </c>
@@ -2822,7 +2822,7 @@
       <c r="B46" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="30"/>
+      <c r="C46" s="49"/>
       <c r="D46" s="24" t="s">
         <v>178</v>
       </c>
@@ -2848,12 +2848,12 @@
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2866,7 +2866,7 @@
       <c r="B48" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="30" t="s">
+      <c r="C48" s="49" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="25" t="s">
@@ -2897,7 +2897,7 @@
       <c r="B49" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="30"/>
+      <c r="C49" s="49"/>
       <c r="D49" s="24" t="s">
         <v>17</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="B50" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="30"/>
+      <c r="C50" s="49"/>
       <c r="D50" s="24" t="s">
         <v>18</v>
       </c>
@@ -2955,7 +2955,7 @@
       <c r="B51" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="30"/>
+      <c r="C51" s="49"/>
       <c r="D51" s="24" t="s">
         <v>182</v>
       </c>
@@ -2984,7 +2984,7 @@
       <c r="B52" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="30"/>
+      <c r="C52" s="49"/>
       <c r="D52" s="24" t="s">
         <v>183</v>
       </c>
@@ -3011,7 +3011,7 @@
       <c r="B53" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="30"/>
+      <c r="C53" s="49"/>
       <c r="D53" s="24" t="s">
         <v>184</v>
       </c>
@@ -3040,7 +3040,7 @@
       <c r="B54" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="30" t="s">
+      <c r="C54" s="49" t="s">
         <v>54</v>
       </c>
       <c r="D54" s="24" t="s">
@@ -3073,7 +3073,7 @@
       <c r="B55" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="30"/>
+      <c r="C55" s="49"/>
       <c r="D55" s="24" t="s">
         <v>44</v>
       </c>
@@ -3104,7 +3104,7 @@
       <c r="B56" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="30"/>
+      <c r="C56" s="49"/>
       <c r="D56" s="24" t="s">
         <v>187</v>
       </c>
@@ -3133,7 +3133,7 @@
       <c r="B57" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="30" t="s">
+      <c r="C57" s="49" t="s">
         <v>55</v>
       </c>
       <c r="D57" s="24" t="s">
@@ -3168,7 +3168,7 @@
       <c r="B58" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="30"/>
+      <c r="C58" s="49"/>
       <c r="D58" s="24" t="s">
         <v>190</v>
       </c>
@@ -3195,7 +3195,7 @@
       <c r="B59" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C59" s="30"/>
+      <c r="C59" s="49"/>
       <c r="D59" s="24" t="s">
         <v>192</v>
       </c>
@@ -3224,7 +3224,7 @@
       <c r="B60" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="30"/>
+      <c r="C60" s="49"/>
       <c r="D60" s="24" t="s">
         <v>19</v>
       </c>
@@ -3257,7 +3257,7 @@
       <c r="B61" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C61" s="30"/>
+      <c r="C61" s="49"/>
       <c r="D61" s="24" t="s">
         <v>195</v>
       </c>
@@ -3288,7 +3288,7 @@
       <c r="B62" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="30"/>
+      <c r="C62" s="49"/>
       <c r="D62" s="24" t="s">
         <v>196</v>
       </c>
@@ -3321,7 +3321,7 @@
       <c r="B63" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="C63" s="30" t="s">
+      <c r="C63" s="49" t="s">
         <v>57</v>
       </c>
       <c r="D63" s="24" t="s">
@@ -3356,7 +3356,7 @@
       <c r="B64" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="C64" s="30"/>
+      <c r="C64" s="49"/>
       <c r="D64" s="24" t="s">
         <v>200</v>
       </c>
@@ -3389,7 +3389,7 @@
       <c r="B65" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="C65" s="30"/>
+      <c r="C65" s="49"/>
       <c r="D65" s="24" t="s">
         <v>203</v>
       </c>
@@ -3418,7 +3418,7 @@
       <c r="B66" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="C66" s="30"/>
+      <c r="C66" s="49"/>
       <c r="D66" s="24" t="s">
         <v>206</v>
       </c>
@@ -3445,7 +3445,7 @@
       <c r="B67" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="C67" s="30" t="s">
+      <c r="C67" s="49" t="s">
         <v>58</v>
       </c>
       <c r="D67" s="24" t="s">
@@ -3480,7 +3480,7 @@
       <c r="B68" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="C68" s="30"/>
+      <c r="C68" s="49"/>
       <c r="D68" s="24" t="s">
         <v>211</v>
       </c>
@@ -3511,7 +3511,7 @@
       <c r="B69" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C69" s="30"/>
+      <c r="C69" s="49"/>
       <c r="D69" s="24" t="s">
         <v>214</v>
       </c>
@@ -3541,10 +3541,10 @@
       </c>
     </row>
     <row r="70" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B70" s="34" t="s">
+      <c r="B70" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="C70" s="30" t="s">
+      <c r="C70" s="49" t="s">
         <v>59</v>
       </c>
       <c r="D70" s="24" t="s">
@@ -3553,92 +3553,79 @@
       <c r="E70" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="F70" s="31" t="s">
+      <c r="F70" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="G70" s="31"/>
-      <c r="H70" s="31"/>
-      <c r="I70" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="J70" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="K70" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="L70" s="29" t="s">
+      <c r="G70" s="57"/>
+      <c r="H70" s="57"/>
+      <c r="I70" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="J70" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="K70" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="L70" s="56" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="71" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B71" s="34"/>
-      <c r="C71" s="30"/>
+      <c r="B71" s="48"/>
+      <c r="C71" s="49"/>
       <c r="D71" s="24" t="s">
         <v>218</v>
       </c>
       <c r="E71" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="F71" s="31"/>
-      <c r="G71" s="31"/>
-      <c r="H71" s="31"/>
-      <c r="I71" s="32"/>
-      <c r="J71" s="33"/>
-      <c r="K71" s="27"/>
-      <c r="L71" s="29"/>
+      <c r="F71" s="57"/>
+      <c r="G71" s="57"/>
+      <c r="H71" s="57"/>
+      <c r="I71" s="58"/>
+      <c r="J71" s="59"/>
+      <c r="K71" s="54"/>
+      <c r="L71" s="56"/>
     </row>
     <row r="72" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B72" s="34"/>
-      <c r="C72" s="30"/>
+      <c r="B72" s="48"/>
+      <c r="C72" s="49"/>
       <c r="D72" s="24" t="s">
         <v>220</v>
       </c>
       <c r="E72" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="F72" s="31"/>
-      <c r="G72" s="31"/>
-      <c r="H72" s="31"/>
-      <c r="I72" s="32"/>
-      <c r="J72" s="33"/>
-      <c r="K72" s="27"/>
-      <c r="L72" s="29"/>
+      <c r="F72" s="57"/>
+      <c r="G72" s="57"/>
+      <c r="H72" s="57"/>
+      <c r="I72" s="58"/>
+      <c r="J72" s="59"/>
+      <c r="K72" s="54"/>
+      <c r="L72" s="56"/>
     </row>
     <row r="73" spans="2:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="B73" s="34"/>
-      <c r="C73" s="30"/>
+      <c r="B73" s="48"/>
+      <c r="C73" s="49"/>
       <c r="D73" s="24" t="s">
         <v>222</v>
       </c>
       <c r="E73" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="F73" s="31"/>
-      <c r="G73" s="31"/>
-      <c r="H73" s="31"/>
-      <c r="I73" s="32"/>
-      <c r="J73" s="33"/>
-      <c r="K73" s="28"/>
-      <c r="L73" s="29"/>
+      <c r="F73" s="57"/>
+      <c r="G73" s="57"/>
+      <c r="H73" s="57"/>
+      <c r="I73" s="58"/>
+      <c r="J73" s="59"/>
+      <c r="K73" s="55"/>
+      <c r="L73" s="56"/>
     </row>
   </sheetData>
   <autoFilter ref="F5:L73"/>
   <dataConsolidate/>
   <mergeCells count="23">
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C29:C41"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="C48:C53"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C57:C62"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="C15:C21"/>
     <mergeCell ref="K70:K73"/>
     <mergeCell ref="L70:L73"/>
     <mergeCell ref="C22:C28"/>
@@ -3649,6 +3636,19 @@
     <mergeCell ref="H70:H73"/>
     <mergeCell ref="I70:I73"/>
     <mergeCell ref="J70:J73"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="C15:C21"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C29:C41"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C62"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K70 L7:L73 I7:J73">
@@ -3663,7 +3663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -3671,38 +3671,38 @@
   <cols>
     <col min="1" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="57.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="26" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59" t="s">
+      <c r="D4" s="40"/>
+      <c r="E4" s="40" t="s">
         <v>281</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="40" t="s">
         <v>280</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="40" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="60" t="s">
         <v>279</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="39" t="s">
         <v>241</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="29" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -3710,29 +3710,29 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="52" t="s">
+      <c r="D6" s="61"/>
+      <c r="E6" s="36" t="s">
         <v>278</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>27</v>
+      <c r="G6" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="52" t="s">
+      <c r="D7" s="61"/>
+      <c r="E7" s="36" t="s">
         <v>277</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="27" t="s">
         <v>29</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -3740,14 +3740,14 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="52" t="s">
+      <c r="D8" s="61"/>
+      <c r="E8" s="36" t="s">
         <v>239</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="27" t="s">
         <v>235</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -3755,11 +3755,11 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="44"/>
-      <c r="E9" s="52" t="s">
+      <c r="D9" s="61"/>
+      <c r="E9" s="36" t="s">
         <v>276</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="29" t="s">
         <v>25</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -3767,11 +3767,11 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="44"/>
-      <c r="E10" s="52" t="s">
+      <c r="D10" s="61"/>
+      <c r="E10" s="36" t="s">
         <v>275</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -3779,11 +3779,11 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="44"/>
-      <c r="E11" s="52" t="s">
+      <c r="D11" s="61"/>
+      <c r="E11" s="36" t="s">
         <v>274</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="29" t="s">
         <v>29</v>
       </c>
       <c r="G11" s="5" t="s">
@@ -3791,11 +3791,11 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="41"/>
-      <c r="E12" s="52" t="s">
+      <c r="D12" s="62"/>
+      <c r="E12" s="36" t="s">
         <v>273</v>
       </c>
-      <c r="F12" s="42" t="s">
+      <c r="F12" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G12" s="5" t="s">
@@ -3803,25 +3803,25 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="63" t="s">
         <v>272</v>
       </c>
-      <c r="E13" s="57" t="s">
+      <c r="E13" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>27</v>
+      <c r="G13" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="55"/>
-      <c r="E14" s="57" t="s">
+      <c r="D14" s="64"/>
+      <c r="E14" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="F14" s="42" t="s">
+      <c r="F14" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G14" s="5" t="s">
@@ -3829,23 +3829,23 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="55"/>
-      <c r="E15" s="57" t="s">
+      <c r="D15" s="64"/>
+      <c r="E15" s="38" t="s">
         <v>271</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>27</v>
+      <c r="G15" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D16" s="55"/>
-      <c r="E16" s="53" t="s">
+      <c r="D16" s="64"/>
+      <c r="E16" s="37" t="s">
         <v>270</v>
       </c>
-      <c r="F16" s="47" t="s">
+      <c r="F16" s="33" t="s">
         <v>230</v>
       </c>
       <c r="G16" s="5" t="s">
@@ -3853,11 +3853,11 @@
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D17" s="55"/>
-      <c r="E17" s="53" t="s">
+      <c r="D17" s="64"/>
+      <c r="E17" s="37" t="s">
         <v>269</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="29" t="s">
         <v>29</v>
       </c>
       <c r="G17" s="5" t="s">
@@ -3865,23 +3865,23 @@
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="54"/>
-      <c r="E18" s="53" t="s">
+      <c r="D18" s="65"/>
+      <c r="E18" s="37" t="s">
         <v>268</v>
       </c>
-      <c r="F18" s="42"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="49" t="s">
+      <c r="D19" s="60" t="s">
         <v>267</v>
       </c>
-      <c r="E19" s="52" t="s">
+      <c r="E19" s="36" t="s">
         <v>247</v>
       </c>
-      <c r="F19" s="42" t="s">
+      <c r="F19" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G19" s="4" t="s">
@@ -3889,11 +3889,11 @@
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="44"/>
-      <c r="E20" s="52" t="s">
+      <c r="D20" s="61"/>
+      <c r="E20" s="36" t="s">
         <v>266</v>
       </c>
-      <c r="F20" s="42" t="s">
+      <c r="F20" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G20" s="5" t="s">
@@ -3901,11 +3901,11 @@
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="44"/>
-      <c r="E21" s="52" t="s">
+      <c r="D21" s="61"/>
+      <c r="E21" s="36" t="s">
         <v>265</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="F21" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G21" s="5" t="s">
@@ -3913,11 +3913,11 @@
       </c>
     </row>
     <row r="22" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D22" s="41"/>
-      <c r="E22" s="52" t="s">
+      <c r="D22" s="62"/>
+      <c r="E22" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="F22" s="42" t="s">
+      <c r="F22" s="29" t="s">
         <v>29</v>
       </c>
       <c r="G22" s="5" t="s">
@@ -3925,13 +3925,13 @@
       </c>
     </row>
     <row r="23" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D23" s="56" t="s">
+      <c r="D23" s="63" t="s">
         <v>263</v>
       </c>
-      <c r="E23" s="53" t="s">
+      <c r="E23" s="37" t="s">
         <v>262</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="27" t="s">
         <v>244</v>
       </c>
       <c r="G23" s="5" t="s">
@@ -3939,11 +3939,11 @@
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="55"/>
-      <c r="E24" s="53" t="s">
+      <c r="D24" s="64"/>
+      <c r="E24" s="37" t="s">
         <v>261</v>
       </c>
-      <c r="F24" s="42" t="s">
+      <c r="F24" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G24" s="5" t="s">
@@ -3951,11 +3951,11 @@
       </c>
     </row>
     <row r="25" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D25" s="55"/>
-      <c r="E25" s="53" t="s">
+      <c r="D25" s="64"/>
+      <c r="E25" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="27" t="s">
         <v>244</v>
       </c>
       <c r="G25" s="5" t="s">
@@ -3963,11 +3963,11 @@
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="54"/>
-      <c r="E26" s="53" t="s">
+      <c r="D26" s="65"/>
+      <c r="E26" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="F26" s="42" t="s">
+      <c r="F26" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G26" s="5" t="s">
@@ -3975,13 +3975,13 @@
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="49" t="s">
+      <c r="D27" s="60" t="s">
         <v>258</v>
       </c>
-      <c r="E27" s="52" t="s">
+      <c r="E27" s="36" t="s">
         <v>257</v>
       </c>
-      <c r="F27" s="42" t="s">
+      <c r="F27" s="29" t="s">
         <v>235</v>
       </c>
       <c r="G27" s="5" t="s">
@@ -3989,11 +3989,11 @@
       </c>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="44"/>
-      <c r="E28" s="52" t="s">
+      <c r="D28" s="61"/>
+      <c r="E28" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="F28" s="42" t="s">
+      <c r="F28" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G28" s="5" t="s">
@@ -4001,11 +4001,11 @@
       </c>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="41"/>
-      <c r="E29" s="52" t="s">
+      <c r="D29" s="62"/>
+      <c r="E29" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="F29" s="42" t="s">
+      <c r="F29" s="29" t="s">
         <v>29</v>
       </c>
       <c r="G29" s="5" t="s">
@@ -4013,53 +4013,53 @@
       </c>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="50" t="s">
+      <c r="D30" s="66" t="s">
         <v>254</v>
       </c>
-      <c r="E30" s="51" t="s">
+      <c r="E30" s="35" t="s">
         <v>253</v>
       </c>
-      <c r="F30" s="42"/>
+      <c r="F30" s="29"/>
       <c r="G30" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="50"/>
-      <c r="E31" s="51" t="s">
+      <c r="D31" s="66"/>
+      <c r="E31" s="35" t="s">
         <v>252</v>
       </c>
-      <c r="F31" s="42"/>
+      <c r="F31" s="29"/>
       <c r="G31" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D32" s="50"/>
-      <c r="E32" s="51" t="s">
+      <c r="D32" s="66"/>
+      <c r="E32" s="35" t="s">
         <v>251</v>
       </c>
-      <c r="F32" s="42"/>
+      <c r="F32" s="29"/>
       <c r="G32" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D33" s="50"/>
-      <c r="E33" s="51" t="s">
+      <c r="D33" s="66"/>
+      <c r="E33" s="35" t="s">
         <v>250</v>
       </c>
-      <c r="F33" s="42"/>
+      <c r="F33" s="29"/>
       <c r="G33" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="50"/>
+      <c r="D34" s="66"/>
       <c r="E34" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="F34" s="42" t="s">
+      <c r="F34" s="29" t="s">
         <v>235</v>
       </c>
       <c r="G34" s="5" t="s">
@@ -4067,13 +4067,13 @@
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D35" s="49" t="s">
+      <c r="D35" s="60" t="s">
         <v>248</v>
       </c>
-      <c r="E35" s="48" t="s">
+      <c r="E35" s="34" t="s">
         <v>247</v>
       </c>
-      <c r="F35" s="42" t="s">
+      <c r="F35" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G35" s="4" t="s">
@@ -4081,11 +4081,11 @@
       </c>
     </row>
     <row r="36" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D36" s="44"/>
-      <c r="E36" s="43" t="s">
+      <c r="D36" s="61"/>
+      <c r="E36" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="F36" s="47" t="s">
+      <c r="F36" s="33" t="s">
         <v>227</v>
       </c>
       <c r="G36" s="5" t="s">
@@ -4093,11 +4093,11 @@
       </c>
     </row>
     <row r="37" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D37" s="44"/>
-      <c r="E37" s="45" t="s">
+      <c r="D37" s="61"/>
+      <c r="E37" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="F37" s="39" t="s">
+      <c r="F37" s="27" t="s">
         <v>244</v>
       </c>
       <c r="G37" s="5" t="s">
@@ -4105,11 +4105,11 @@
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D38" s="44"/>
-      <c r="E38" s="45" t="s">
+      <c r="D38" s="61"/>
+      <c r="E38" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="F38" s="42" t="s">
+      <c r="F38" s="29" t="s">
         <v>235</v>
       </c>
       <c r="G38" s="5" t="s">
@@ -4117,11 +4117,11 @@
       </c>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D39" s="44"/>
-      <c r="E39" s="45" t="s">
+      <c r="D39" s="61"/>
+      <c r="E39" s="31" t="s">
         <v>242</v>
       </c>
-      <c r="F39" s="42" t="s">
+      <c r="F39" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G39" s="5" t="s">
@@ -4129,11 +4129,11 @@
       </c>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D40" s="44"/>
-      <c r="E40" s="40" t="s">
+      <c r="D40" s="61"/>
+      <c r="E40" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="F40" s="42" t="s">
+      <c r="F40" s="29" t="s">
         <v>29</v>
       </c>
       <c r="G40" s="4" t="s">
@@ -4141,11 +4141,11 @@
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D41" s="44"/>
-      <c r="E41" s="40" t="s">
+      <c r="D41" s="61"/>
+      <c r="E41" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="F41" s="42" t="s">
+      <c r="F41" s="29" t="s">
         <v>29</v>
       </c>
       <c r="G41" s="4" t="s">
@@ -4153,11 +4153,11 @@
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D42" s="44"/>
-      <c r="E42" s="40" t="s">
+      <c r="D42" s="61"/>
+      <c r="E42" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="F42" s="42" t="s">
+      <c r="F42" s="29" t="s">
         <v>235</v>
       </c>
       <c r="G42" s="4" t="s">
@@ -4165,11 +4165,11 @@
       </c>
     </row>
     <row r="43" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D43" s="44"/>
-      <c r="E43" s="40" t="s">
+      <c r="D43" s="61"/>
+      <c r="E43" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="F43" s="39" t="s">
+      <c r="F43" s="27" t="s">
         <v>237</v>
       </c>
       <c r="G43" s="5" t="s">
@@ -4177,54 +4177,54 @@
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D44" s="44"/>
-      <c r="E44" s="40" t="s">
+      <c r="D44" s="61"/>
+      <c r="E44" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="F44" s="42"/>
+      <c r="F44" s="29"/>
       <c r="G44" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I44" s="46" t="s">
+      <c r="I44" s="32" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D45" s="44"/>
-      <c r="E45" s="43" t="s">
+      <c r="D45" s="61"/>
+      <c r="E45" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F45" s="42" t="s">
+      <c r="F45" s="29" t="s">
         <v>235</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I45" s="46" t="s">
+      <c r="I45" s="32" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D46" s="44"/>
-      <c r="E46" s="45" t="s">
+      <c r="D46" s="61"/>
+      <c r="E46" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="F46" s="42" t="s">
+      <c r="F46" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I46" s="46" t="s">
+      <c r="I46" s="32" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D47" s="44"/>
-      <c r="E47" s="45" t="s">
+      <c r="D47" s="61"/>
+      <c r="E47" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="F47" s="42" t="s">
+      <c r="F47" s="29" t="s">
         <v>25</v>
       </c>
       <c r="G47" s="5" t="s">
@@ -4232,11 +4232,11 @@
       </c>
     </row>
     <row r="48" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D48" s="44"/>
-      <c r="E48" s="43" t="s">
+      <c r="D48" s="61"/>
+      <c r="E48" s="30" t="s">
         <v>231</v>
       </c>
-      <c r="F48" s="39" t="s">
+      <c r="F48" s="27" t="s">
         <v>230</v>
       </c>
       <c r="G48" s="5" t="s">
@@ -4244,11 +4244,11 @@
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" s="44"/>
-      <c r="E49" s="43" t="s">
+      <c r="D49" s="61"/>
+      <c r="E49" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="F49" s="42" t="s">
+      <c r="F49" s="29" t="s">
         <v>25</v>
       </c>
       <c r="G49" s="5" t="s">
@@ -4256,11 +4256,11 @@
       </c>
     </row>
     <row r="50" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D50" s="41"/>
-      <c r="E50" s="40" t="s">
+      <c r="D50" s="62"/>
+      <c r="E50" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="F50" s="39" t="s">
+      <c r="F50" s="27" t="s">
         <v>227</v>
       </c>
       <c r="G50" s="4" t="s">
@@ -4301,191 +4301,191 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="60" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="60"/>
-    <col min="6" max="6" width="13.85546875" style="60" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="60" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="60"/>
-    <col min="10" max="10" width="12.42578125" style="60" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="60"/>
+    <col min="1" max="1" width="10.42578125" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="41" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="41"/>
+    <col min="6" max="6" width="13.85546875" style="41" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="41" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="41"/>
+    <col min="10" max="10" width="12.42578125" style="41" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="41"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="60" t="s">
+      <c r="I4" s="41" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="66">
+      <c r="B5" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="47">
         <f>COUNTIF('CODE-TC-SRS'!I7:I73,"Done")</f>
         <v>38</v>
       </c>
-      <c r="F5" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="61">
+      <c r="F5" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="42">
         <f>COUNTIF('CODE-TC-SRS'!K6:K78,"Done")</f>
         <v>24</v>
       </c>
-      <c r="J5" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="61">
+      <c r="J5" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="42">
         <f>COUNTIF(DOC!G4:G49,"Done")</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="43" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="9">
         <f>COUNTIF('CODE-TC-SRS'!I7:I73, "In Progress")</f>
         <v>24</v>
       </c>
-      <c r="F6" s="62" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="63">
+      <c r="F6" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="44">
         <f>COUNTIF('CODE-TC-SRS'!K6:K72,"In Progress")</f>
         <v>0</v>
       </c>
-      <c r="J6" s="62" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="63">
+      <c r="J6" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="44">
         <f>COUNTIF(DOC!G4:G49,"In Progress")</f>
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="45" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="9">
         <f>COUNTIF('CODE-TC-SRS'!I7:I73, "Not Start")</f>
         <v>0</v>
       </c>
-      <c r="F7" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="63">
+      <c r="F7" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="44">
         <f>COUNTIF('CODE-TC-SRS'!K6:K72, "Not Start")</f>
         <v>38</v>
       </c>
-      <c r="J7" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="63">
+      <c r="J7" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="44">
         <f>COUNTIF(DOC!G4:G49, "Not Start")</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="44" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="9">
         <f>SUM(C5:C7)</f>
         <v>62</v>
       </c>
-      <c r="F8" s="63" t="s">
+      <c r="F8" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="63">
+      <c r="G8" s="44">
         <f>SUM(G5:G7)</f>
         <v>62</v>
       </c>
-      <c r="J8" s="63" t="s">
+      <c r="J8" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="63">
+      <c r="K8" s="44">
         <f>SUM(K5:K7)</f>
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
-      <c r="E9" s="60" t="s">
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="E9" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="61">
+      <c r="B10" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="42">
         <f>COUNTIF('CODE-TC-SRS'!J7:J73,"Done")</f>
         <v>50</v>
       </c>
-      <c r="F10" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="61">
+      <c r="F10" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="42">
         <f>COUNTIF('CODE-TC-SRS'!L7:L73,"Done")</f>
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="62" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="63">
+      <c r="B11" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="44">
         <f>COUNTIF('CODE-TC-SRS'!J7:J73, "In Progress")</f>
         <v>9</v>
       </c>
-      <c r="F11" s="62" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="63">
+      <c r="F11" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="44">
         <f>COUNTIF('CODE-TC-SRS'!L7:L73,"In Progress")</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="63">
+      <c r="B12" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="44">
         <f>COUNTIF('CODE-TC-SRS'!J7:J73, "Not Start")</f>
         <v>2</v>
       </c>
-      <c r="F12" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="63">
+      <c r="F12" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="44">
         <f>COUNTIF('CODE-TC-SRS'!L7:L73, "Not Start")</f>
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="63">
+      <c r="C13" s="44">
         <f>SUM(C10:C12)</f>
         <v>61</v>
       </c>
-      <c r="F13" s="63" t="s">
+      <c r="F13" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="63">
+      <c r="G13" s="44">
         <f>SUM(G10:G12)</f>
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
[Doc]_Commit document cho các report
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -1195,21 +1195,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1222,6 +1207,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1230,6 +1218,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1631,12 +1631,12 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1649,7 +1649,7 @@
       <c r="B7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="52" t="s">
         <v>118</v>
       </c>
       <c r="D7" s="24" t="s">
@@ -1684,7 +1684,7 @@
       <c r="B8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="49"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="24" t="s">
         <v>8</v>
       </c>
@@ -1714,12 +1714,12 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1732,7 +1732,7 @@
       <c r="B10" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="52" t="s">
         <v>121</v>
       </c>
       <c r="D10" s="24" t="s">
@@ -1767,7 +1767,7 @@
       <c r="B11" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="49"/>
+      <c r="C11" s="52"/>
       <c r="D11" s="24" t="s">
         <v>6</v>
       </c>
@@ -1800,7 +1800,7 @@
       <c r="B12" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="49"/>
+      <c r="C12" s="52"/>
       <c r="D12" s="24" t="s">
         <v>123</v>
       </c>
@@ -1831,7 +1831,7 @@
       <c r="B13" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="49"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="24" t="s">
         <v>125</v>
       </c>
@@ -1860,7 +1860,7 @@
       <c r="B14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="49"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="24" t="s">
         <v>126</v>
       </c>
@@ -1889,7 +1889,7 @@
       <c r="B15" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="52" t="s">
         <v>128</v>
       </c>
       <c r="D15" s="24" t="s">
@@ -1922,7 +1922,7 @@
       <c r="B16" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="49"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="25" t="s">
         <v>130</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="B17" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="49"/>
+      <c r="C17" s="52"/>
       <c r="D17" s="24" t="s">
         <v>132</v>
       </c>
@@ -1980,7 +1980,7 @@
       <c r="B18" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="49"/>
+      <c r="C18" s="52"/>
       <c r="D18" s="24" t="s">
         <v>134</v>
       </c>
@@ -2009,7 +2009,7 @@
       <c r="B19" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="49"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="24" t="s">
         <v>48</v>
       </c>
@@ -2038,7 +2038,7 @@
       <c r="B20" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="49"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="24" t="s">
         <v>9</v>
       </c>
@@ -2067,7 +2067,7 @@
       <c r="B21" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="49"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="24" t="s">
         <v>137</v>
       </c>
@@ -2096,7 +2096,7 @@
       <c r="B22" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="52" t="s">
         <v>139</v>
       </c>
       <c r="D22" s="24" t="s">
@@ -2129,7 +2129,7 @@
       <c r="B23" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="49"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="25" t="s">
         <v>142</v>
       </c>
@@ -2158,7 +2158,7 @@
       <c r="B24" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="49"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="24" t="s">
         <v>144</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="B25" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="49"/>
+      <c r="C25" s="52"/>
       <c r="D25" s="24" t="s">
         <v>10</v>
       </c>
@@ -2218,7 +2218,7 @@
       <c r="B26" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="49"/>
+      <c r="C26" s="52"/>
       <c r="D26" s="24" t="s">
         <v>147</v>
       </c>
@@ -2249,7 +2249,7 @@
       <c r="B27" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="49"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="24" t="s">
         <v>11</v>
       </c>
@@ -2278,7 +2278,7 @@
       <c r="B28" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="49"/>
+      <c r="C28" s="52"/>
       <c r="D28" s="25" t="s">
         <v>150</v>
       </c>
@@ -2307,7 +2307,7 @@
       <c r="B29" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="50" t="s">
+      <c r="C29" s="57" t="s">
         <v>152</v>
       </c>
       <c r="D29" s="24" t="s">
@@ -2340,7 +2340,7 @@
       <c r="B30" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="51"/>
+      <c r="C30" s="58"/>
       <c r="D30" s="24" t="s">
         <v>154</v>
       </c>
@@ -2373,7 +2373,7 @@
       <c r="B31" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="51"/>
+      <c r="C31" s="58"/>
       <c r="D31" s="24" t="s">
         <v>155</v>
       </c>
@@ -2402,7 +2402,7 @@
       <c r="B32" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="51"/>
+      <c r="C32" s="58"/>
       <c r="D32" s="24" t="s">
         <v>156</v>
       </c>
@@ -2435,7 +2435,7 @@
       <c r="B33" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="51"/>
+      <c r="C33" s="58"/>
       <c r="D33" s="24" t="s">
         <v>158</v>
       </c>
@@ -2466,7 +2466,7 @@
       <c r="B34" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="51"/>
+      <c r="C34" s="58"/>
       <c r="D34" s="24" t="s">
         <v>160</v>
       </c>
@@ -2499,7 +2499,7 @@
       <c r="B35" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="51"/>
+      <c r="C35" s="58"/>
       <c r="D35" s="24" t="s">
         <v>162</v>
       </c>
@@ -2532,7 +2532,7 @@
       <c r="B36" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="51"/>
+      <c r="C36" s="58"/>
       <c r="D36" s="25" t="s">
         <v>164</v>
       </c>
@@ -2561,7 +2561,7 @@
       <c r="B37" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="51"/>
+      <c r="C37" s="58"/>
       <c r="D37" s="25" t="s">
         <v>166</v>
       </c>
@@ -2588,7 +2588,7 @@
       <c r="B38" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="51"/>
+      <c r="C38" s="58"/>
       <c r="D38" s="25" t="s">
         <v>167</v>
       </c>
@@ -2617,7 +2617,7 @@
       <c r="B39" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="51"/>
+      <c r="C39" s="58"/>
       <c r="D39" s="25" t="s">
         <v>169</v>
       </c>
@@ -2646,7 +2646,7 @@
       <c r="B40" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="51"/>
+      <c r="C40" s="58"/>
       <c r="D40" s="25" t="s">
         <v>116</v>
       </c>
@@ -2673,7 +2673,7 @@
       <c r="B41" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="52"/>
+      <c r="C41" s="59"/>
       <c r="D41" s="25" t="s">
         <v>171</v>
       </c>
@@ -2700,7 +2700,7 @@
       <c r="B42" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="52" t="s">
         <v>172</v>
       </c>
       <c r="D42" s="24" t="s">
@@ -2735,7 +2735,7 @@
       <c r="B43" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="49"/>
+      <c r="C43" s="52"/>
       <c r="D43" s="24" t="s">
         <v>117</v>
       </c>
@@ -2764,7 +2764,7 @@
       <c r="B44" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="49"/>
+      <c r="C44" s="52"/>
       <c r="D44" s="24" t="s">
         <v>175</v>
       </c>
@@ -2793,7 +2793,7 @@
       <c r="B45" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="49"/>
+      <c r="C45" s="52"/>
       <c r="D45" s="25" t="s">
         <v>177</v>
       </c>
@@ -2822,7 +2822,7 @@
       <c r="B46" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="49"/>
+      <c r="C46" s="52"/>
       <c r="D46" s="24" t="s">
         <v>178</v>
       </c>
@@ -2848,12 +2848,12 @@
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="48" t="s">
+      <c r="B47" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2866,7 +2866,7 @@
       <c r="B48" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="49" t="s">
+      <c r="C48" s="52" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="25" t="s">
@@ -2897,7 +2897,7 @@
       <c r="B49" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="49"/>
+      <c r="C49" s="52"/>
       <c r="D49" s="24" t="s">
         <v>17</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="B50" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="49"/>
+      <c r="C50" s="52"/>
       <c r="D50" s="24" t="s">
         <v>18</v>
       </c>
@@ -2955,7 +2955,7 @@
       <c r="B51" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="49"/>
+      <c r="C51" s="52"/>
       <c r="D51" s="24" t="s">
         <v>182</v>
       </c>
@@ -2984,7 +2984,7 @@
       <c r="B52" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="49"/>
+      <c r="C52" s="52"/>
       <c r="D52" s="24" t="s">
         <v>183</v>
       </c>
@@ -3011,7 +3011,7 @@
       <c r="B53" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="49"/>
+      <c r="C53" s="52"/>
       <c r="D53" s="24" t="s">
         <v>184</v>
       </c>
@@ -3040,7 +3040,7 @@
       <c r="B54" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="49" t="s">
+      <c r="C54" s="52" t="s">
         <v>54</v>
       </c>
       <c r="D54" s="24" t="s">
@@ -3073,7 +3073,7 @@
       <c r="B55" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="49"/>
+      <c r="C55" s="52"/>
       <c r="D55" s="24" t="s">
         <v>44</v>
       </c>
@@ -3104,7 +3104,7 @@
       <c r="B56" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="49"/>
+      <c r="C56" s="52"/>
       <c r="D56" s="24" t="s">
         <v>187</v>
       </c>
@@ -3133,7 +3133,7 @@
       <c r="B57" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="49" t="s">
+      <c r="C57" s="52" t="s">
         <v>55</v>
       </c>
       <c r="D57" s="24" t="s">
@@ -3168,7 +3168,7 @@
       <c r="B58" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="49"/>
+      <c r="C58" s="52"/>
       <c r="D58" s="24" t="s">
         <v>190</v>
       </c>
@@ -3195,7 +3195,7 @@
       <c r="B59" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C59" s="49"/>
+      <c r="C59" s="52"/>
       <c r="D59" s="24" t="s">
         <v>192</v>
       </c>
@@ -3224,7 +3224,7 @@
       <c r="B60" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="49"/>
+      <c r="C60" s="52"/>
       <c r="D60" s="24" t="s">
         <v>19</v>
       </c>
@@ -3257,7 +3257,7 @@
       <c r="B61" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C61" s="49"/>
+      <c r="C61" s="52"/>
       <c r="D61" s="24" t="s">
         <v>195</v>
       </c>
@@ -3288,7 +3288,7 @@
       <c r="B62" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="49"/>
+      <c r="C62" s="52"/>
       <c r="D62" s="24" t="s">
         <v>196</v>
       </c>
@@ -3321,7 +3321,7 @@
       <c r="B63" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="C63" s="49" t="s">
+      <c r="C63" s="52" t="s">
         <v>57</v>
       </c>
       <c r="D63" s="24" t="s">
@@ -3356,7 +3356,7 @@
       <c r="B64" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="C64" s="49"/>
+      <c r="C64" s="52"/>
       <c r="D64" s="24" t="s">
         <v>200</v>
       </c>
@@ -3389,7 +3389,7 @@
       <c r="B65" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="C65" s="49"/>
+      <c r="C65" s="52"/>
       <c r="D65" s="24" t="s">
         <v>203</v>
       </c>
@@ -3418,7 +3418,7 @@
       <c r="B66" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="C66" s="49"/>
+      <c r="C66" s="52"/>
       <c r="D66" s="24" t="s">
         <v>206</v>
       </c>
@@ -3445,7 +3445,7 @@
       <c r="B67" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="C67" s="49" t="s">
+      <c r="C67" s="52" t="s">
         <v>58</v>
       </c>
       <c r="D67" s="24" t="s">
@@ -3480,7 +3480,7 @@
       <c r="B68" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="C68" s="49"/>
+      <c r="C68" s="52"/>
       <c r="D68" s="24" t="s">
         <v>211</v>
       </c>
@@ -3511,7 +3511,7 @@
       <c r="B69" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C69" s="49"/>
+      <c r="C69" s="52"/>
       <c r="D69" s="24" t="s">
         <v>214</v>
       </c>
@@ -3541,10 +3541,10 @@
       </c>
     </row>
     <row r="70" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B70" s="48" t="s">
+      <c r="B70" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="C70" s="49" t="s">
+      <c r="C70" s="52" t="s">
         <v>59</v>
       </c>
       <c r="D70" s="24" t="s">
@@ -3553,79 +3553,92 @@
       <c r="E70" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="F70" s="57" t="s">
+      <c r="F70" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="G70" s="57"/>
-      <c r="H70" s="57"/>
-      <c r="I70" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="J70" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="K70" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="L70" s="56" t="s">
+      <c r="G70" s="53"/>
+      <c r="H70" s="53"/>
+      <c r="I70" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="J70" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="K70" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="L70" s="51" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="71" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B71" s="48"/>
-      <c r="C71" s="49"/>
+      <c r="B71" s="56"/>
+      <c r="C71" s="52"/>
       <c r="D71" s="24" t="s">
         <v>218</v>
       </c>
       <c r="E71" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="F71" s="57"/>
-      <c r="G71" s="57"/>
-      <c r="H71" s="57"/>
-      <c r="I71" s="58"/>
-      <c r="J71" s="59"/>
-      <c r="K71" s="54"/>
-      <c r="L71" s="56"/>
+      <c r="F71" s="53"/>
+      <c r="G71" s="53"/>
+      <c r="H71" s="53"/>
+      <c r="I71" s="54"/>
+      <c r="J71" s="55"/>
+      <c r="K71" s="49"/>
+      <c r="L71" s="51"/>
     </row>
     <row r="72" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B72" s="48"/>
-      <c r="C72" s="49"/>
+      <c r="B72" s="56"/>
+      <c r="C72" s="52"/>
       <c r="D72" s="24" t="s">
         <v>220</v>
       </c>
       <c r="E72" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="F72" s="57"/>
-      <c r="G72" s="57"/>
-      <c r="H72" s="57"/>
-      <c r="I72" s="58"/>
-      <c r="J72" s="59"/>
-      <c r="K72" s="54"/>
-      <c r="L72" s="56"/>
+      <c r="F72" s="53"/>
+      <c r="G72" s="53"/>
+      <c r="H72" s="53"/>
+      <c r="I72" s="54"/>
+      <c r="J72" s="55"/>
+      <c r="K72" s="49"/>
+      <c r="L72" s="51"/>
     </row>
     <row r="73" spans="2:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="B73" s="48"/>
-      <c r="C73" s="49"/>
+      <c r="B73" s="56"/>
+      <c r="C73" s="52"/>
       <c r="D73" s="24" t="s">
         <v>222</v>
       </c>
       <c r="E73" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="F73" s="57"/>
-      <c r="G73" s="57"/>
-      <c r="H73" s="57"/>
-      <c r="I73" s="58"/>
-      <c r="J73" s="59"/>
-      <c r="K73" s="55"/>
-      <c r="L73" s="56"/>
+      <c r="F73" s="53"/>
+      <c r="G73" s="53"/>
+      <c r="H73" s="53"/>
+      <c r="I73" s="54"/>
+      <c r="J73" s="55"/>
+      <c r="K73" s="50"/>
+      <c r="L73" s="51"/>
     </row>
   </sheetData>
   <autoFilter ref="F5:L73"/>
   <dataConsolidate/>
   <mergeCells count="23">
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C29:C41"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C62"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="C15:C21"/>
     <mergeCell ref="K70:K73"/>
     <mergeCell ref="L70:L73"/>
     <mergeCell ref="C22:C28"/>
@@ -3636,19 +3649,6 @@
     <mergeCell ref="H70:H73"/>
     <mergeCell ref="I70:I73"/>
     <mergeCell ref="J70:J73"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="C15:C21"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C29:C41"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="C48:C53"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C57:C62"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K70 L7:L73 I7:J73">
@@ -3663,9 +3663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4172,8 +4170,8 @@
       <c r="F43" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="G43" s="5" t="s">
-        <v>27</v>
+      <c r="G43" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.25">
@@ -4227,8 +4225,8 @@
       <c r="F47" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G47" s="5" t="s">
-        <v>27</v>
+      <c r="G47" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="4:9" ht="30" x14ac:dyDescent="0.25">
@@ -4251,8 +4249,8 @@
       <c r="F49" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G49" s="5" t="s">
-        <v>27</v>
+      <c r="G49" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="4:7" ht="30" x14ac:dyDescent="0.25">
@@ -4342,7 +4340,7 @@
       </c>
       <c r="K5" s="42">
         <f>COUNTIF(DOC!G4:G49,"Done")</f>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -4365,7 +4363,7 @@
       </c>
       <c r="K6" s="44">
         <f>COUNTIF(DOC!G4:G49,"In Progress")</f>
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update phần test case
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\201609JS02\WIP\Users\HuyenPT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="CODE-TC-SRS" sheetId="8" r:id="rId1"/>
@@ -14,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CODE-TC-SRS'!$F$5:$L$73</definedName>
   </definedNames>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -894,7 +899,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1195,6 +1200,21 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1207,9 +1227,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1218,18 +1235,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1322,7 +1327,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1355,9 +1360,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1390,6 +1412,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1568,7 +1607,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L73"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1631,12 +1672,12 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1649,7 +1690,7 @@
       <c r="B7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="49" t="s">
         <v>118</v>
       </c>
       <c r="D7" s="24" t="s">
@@ -1684,7 +1725,7 @@
       <c r="B8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="52"/>
+      <c r="C8" s="49"/>
       <c r="D8" s="24" t="s">
         <v>8</v>
       </c>
@@ -1714,12 +1755,12 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1732,7 +1773,7 @@
       <c r="B10" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="49" t="s">
         <v>121</v>
       </c>
       <c r="D10" s="24" t="s">
@@ -1767,7 +1808,7 @@
       <c r="B11" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="52"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="24" t="s">
         <v>6</v>
       </c>
@@ -1800,7 +1841,7 @@
       <c r="B12" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="52"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="24" t="s">
         <v>123</v>
       </c>
@@ -1831,7 +1872,7 @@
       <c r="B13" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="52"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="24" t="s">
         <v>125</v>
       </c>
@@ -1860,7 +1901,7 @@
       <c r="B14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="52"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="24" t="s">
         <v>126</v>
       </c>
@@ -1889,7 +1930,7 @@
       <c r="B15" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="49" t="s">
         <v>128</v>
       </c>
       <c r="D15" s="24" t="s">
@@ -1922,7 +1963,7 @@
       <c r="B16" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="52"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="25" t="s">
         <v>130</v>
       </c>
@@ -1951,7 +1992,7 @@
       <c r="B17" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="52"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="24" t="s">
         <v>132</v>
       </c>
@@ -1980,7 +2021,7 @@
       <c r="B18" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="52"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="24" t="s">
         <v>134</v>
       </c>
@@ -2009,7 +2050,7 @@
       <c r="B19" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="52"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="24" t="s">
         <v>48</v>
       </c>
@@ -2038,7 +2079,7 @@
       <c r="B20" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="52"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="24" t="s">
         <v>9</v>
       </c>
@@ -2067,7 +2108,7 @@
       <c r="B21" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="52"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="24" t="s">
         <v>137</v>
       </c>
@@ -2096,7 +2137,7 @@
       <c r="B22" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="49" t="s">
         <v>139</v>
       </c>
       <c r="D22" s="24" t="s">
@@ -2118,8 +2159,8 @@
       <c r="J22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>28</v>
+      <c r="K22" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="L22" s="18" t="s">
         <v>28</v>
@@ -2129,7 +2170,7 @@
       <c r="B23" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="52"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="25" t="s">
         <v>142</v>
       </c>
@@ -2147,8 +2188,8 @@
       <c r="J23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>28</v>
+      <c r="K23" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="L23" s="18" t="s">
         <v>28</v>
@@ -2158,7 +2199,7 @@
       <c r="B24" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="52"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="24" t="s">
         <v>144</v>
       </c>
@@ -2176,8 +2217,8 @@
       <c r="J24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K24" s="3" t="s">
-        <v>28</v>
+      <c r="K24" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="L24" s="18" t="s">
         <v>28</v>
@@ -2187,7 +2228,7 @@
       <c r="B25" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="52"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="24" t="s">
         <v>10</v>
       </c>
@@ -2207,8 +2248,8 @@
       <c r="J25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>28</v>
+      <c r="K25" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="L25" s="18" t="s">
         <v>28</v>
@@ -2218,7 +2259,7 @@
       <c r="B26" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="52"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="24" t="s">
         <v>147</v>
       </c>
@@ -2238,8 +2279,8 @@
       <c r="J26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K26" s="3" t="s">
-        <v>28</v>
+      <c r="K26" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="L26" s="18" t="s">
         <v>28</v>
@@ -2249,7 +2290,7 @@
       <c r="B27" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="52"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="24" t="s">
         <v>11</v>
       </c>
@@ -2267,8 +2308,8 @@
       <c r="J27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K27" s="3" t="s">
-        <v>28</v>
+      <c r="K27" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="L27" s="18" t="s">
         <v>28</v>
@@ -2278,7 +2319,7 @@
       <c r="B28" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="52"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="25" t="s">
         <v>150</v>
       </c>
@@ -2296,8 +2337,8 @@
       <c r="J28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K28" s="3" t="s">
-        <v>28</v>
+      <c r="K28" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>28</v>
@@ -2307,7 +2348,7 @@
       <c r="B29" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="57" t="s">
+      <c r="C29" s="50" t="s">
         <v>152</v>
       </c>
       <c r="D29" s="24" t="s">
@@ -2340,7 +2381,7 @@
       <c r="B30" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="58"/>
+      <c r="C30" s="51"/>
       <c r="D30" s="24" t="s">
         <v>154</v>
       </c>
@@ -2373,7 +2414,7 @@
       <c r="B31" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="58"/>
+      <c r="C31" s="51"/>
       <c r="D31" s="24" t="s">
         <v>155</v>
       </c>
@@ -2402,7 +2443,7 @@
       <c r="B32" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="58"/>
+      <c r="C32" s="51"/>
       <c r="D32" s="24" t="s">
         <v>156</v>
       </c>
@@ -2435,7 +2476,7 @@
       <c r="B33" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="58"/>
+      <c r="C33" s="51"/>
       <c r="D33" s="24" t="s">
         <v>158</v>
       </c>
@@ -2466,7 +2507,7 @@
       <c r="B34" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="58"/>
+      <c r="C34" s="51"/>
       <c r="D34" s="24" t="s">
         <v>160</v>
       </c>
@@ -2499,7 +2540,7 @@
       <c r="B35" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="58"/>
+      <c r="C35" s="51"/>
       <c r="D35" s="24" t="s">
         <v>162</v>
       </c>
@@ -2532,7 +2573,7 @@
       <c r="B36" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="58"/>
+      <c r="C36" s="51"/>
       <c r="D36" s="25" t="s">
         <v>164</v>
       </c>
@@ -2561,7 +2602,7 @@
       <c r="B37" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="58"/>
+      <c r="C37" s="51"/>
       <c r="D37" s="25" t="s">
         <v>166</v>
       </c>
@@ -2588,7 +2629,7 @@
       <c r="B38" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="58"/>
+      <c r="C38" s="51"/>
       <c r="D38" s="25" t="s">
         <v>167</v>
       </c>
@@ -2617,7 +2658,7 @@
       <c r="B39" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="58"/>
+      <c r="C39" s="51"/>
       <c r="D39" s="25" t="s">
         <v>169</v>
       </c>
@@ -2646,7 +2687,7 @@
       <c r="B40" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="58"/>
+      <c r="C40" s="51"/>
       <c r="D40" s="25" t="s">
         <v>116</v>
       </c>
@@ -2673,7 +2714,7 @@
       <c r="B41" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="59"/>
+      <c r="C41" s="52"/>
       <c r="D41" s="25" t="s">
         <v>171</v>
       </c>
@@ -2700,7 +2741,7 @@
       <c r="B42" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="52" t="s">
+      <c r="C42" s="49" t="s">
         <v>172</v>
       </c>
       <c r="D42" s="24" t="s">
@@ -2724,8 +2765,8 @@
       <c r="J42" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K42" s="3" t="s">
-        <v>28</v>
+      <c r="K42" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="L42" s="12" t="s">
         <v>26</v>
@@ -2735,7 +2776,7 @@
       <c r="B43" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="52"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="24" t="s">
         <v>117</v>
       </c>
@@ -2753,8 +2794,8 @@
       <c r="J43" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K43" s="3" t="s">
-        <v>28</v>
+      <c r="K43" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="L43" s="18" t="s">
         <v>28</v>
@@ -2764,7 +2805,7 @@
       <c r="B44" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="52"/>
+      <c r="C44" s="49"/>
       <c r="D44" s="24" t="s">
         <v>175</v>
       </c>
@@ -2782,8 +2823,8 @@
       <c r="J44" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K44" s="3" t="s">
-        <v>28</v>
+      <c r="K44" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="L44" s="18" t="s">
         <v>28</v>
@@ -2793,7 +2834,7 @@
       <c r="B45" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="52"/>
+      <c r="C45" s="49"/>
       <c r="D45" s="25" t="s">
         <v>177</v>
       </c>
@@ -2811,8 +2852,8 @@
       <c r="J45" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="K45" s="3" t="s">
-        <v>28</v>
+      <c r="K45" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="L45" s="18" t="s">
         <v>28</v>
@@ -2822,7 +2863,7 @@
       <c r="B46" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="52"/>
+      <c r="C46" s="49"/>
       <c r="D46" s="24" t="s">
         <v>178</v>
       </c>
@@ -2840,20 +2881,20 @@
       <c r="J46" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K46" s="3" t="s">
-        <v>28</v>
+      <c r="K46" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="L46" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2866,7 +2907,7 @@
       <c r="B48" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="52" t="s">
+      <c r="C48" s="49" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="25" t="s">
@@ -2897,7 +2938,7 @@
       <c r="B49" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="52"/>
+      <c r="C49" s="49"/>
       <c r="D49" s="24" t="s">
         <v>17</v>
       </c>
@@ -2926,7 +2967,7 @@
       <c r="B50" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="52"/>
+      <c r="C50" s="49"/>
       <c r="D50" s="24" t="s">
         <v>18</v>
       </c>
@@ -2955,7 +2996,7 @@
       <c r="B51" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="52"/>
+      <c r="C51" s="49"/>
       <c r="D51" s="24" t="s">
         <v>182</v>
       </c>
@@ -2984,7 +3025,7 @@
       <c r="B52" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="52"/>
+      <c r="C52" s="49"/>
       <c r="D52" s="24" t="s">
         <v>183</v>
       </c>
@@ -3011,7 +3052,7 @@
       <c r="B53" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="52"/>
+      <c r="C53" s="49"/>
       <c r="D53" s="24" t="s">
         <v>184</v>
       </c>
@@ -3040,7 +3081,7 @@
       <c r="B54" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="52" t="s">
+      <c r="C54" s="49" t="s">
         <v>54</v>
       </c>
       <c r="D54" s="24" t="s">
@@ -3073,7 +3114,7 @@
       <c r="B55" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="52"/>
+      <c r="C55" s="49"/>
       <c r="D55" s="24" t="s">
         <v>44</v>
       </c>
@@ -3104,7 +3145,7 @@
       <c r="B56" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="52"/>
+      <c r="C56" s="49"/>
       <c r="D56" s="24" t="s">
         <v>187</v>
       </c>
@@ -3133,7 +3174,7 @@
       <c r="B57" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="52" t="s">
+      <c r="C57" s="49" t="s">
         <v>55</v>
       </c>
       <c r="D57" s="24" t="s">
@@ -3168,7 +3209,7 @@
       <c r="B58" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="52"/>
+      <c r="C58" s="49"/>
       <c r="D58" s="24" t="s">
         <v>190</v>
       </c>
@@ -3195,7 +3236,7 @@
       <c r="B59" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C59" s="52"/>
+      <c r="C59" s="49"/>
       <c r="D59" s="24" t="s">
         <v>192</v>
       </c>
@@ -3224,7 +3265,7 @@
       <c r="B60" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="52"/>
+      <c r="C60" s="49"/>
       <c r="D60" s="24" t="s">
         <v>19</v>
       </c>
@@ -3257,7 +3298,7 @@
       <c r="B61" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C61" s="52"/>
+      <c r="C61" s="49"/>
       <c r="D61" s="24" t="s">
         <v>195</v>
       </c>
@@ -3288,7 +3329,7 @@
       <c r="B62" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="52"/>
+      <c r="C62" s="49"/>
       <c r="D62" s="24" t="s">
         <v>196</v>
       </c>
@@ -3321,7 +3362,7 @@
       <c r="B63" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="C63" s="52" t="s">
+      <c r="C63" s="49" t="s">
         <v>57</v>
       </c>
       <c r="D63" s="24" t="s">
@@ -3356,7 +3397,7 @@
       <c r="B64" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="C64" s="52"/>
+      <c r="C64" s="49"/>
       <c r="D64" s="24" t="s">
         <v>200</v>
       </c>
@@ -3389,7 +3430,7 @@
       <c r="B65" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="C65" s="52"/>
+      <c r="C65" s="49"/>
       <c r="D65" s="24" t="s">
         <v>203</v>
       </c>
@@ -3418,7 +3459,7 @@
       <c r="B66" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="C66" s="52"/>
+      <c r="C66" s="49"/>
       <c r="D66" s="24" t="s">
         <v>206</v>
       </c>
@@ -3445,7 +3486,7 @@
       <c r="B67" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="C67" s="52" t="s">
+      <c r="C67" s="49" t="s">
         <v>58</v>
       </c>
       <c r="D67" s="24" t="s">
@@ -3480,7 +3521,7 @@
       <c r="B68" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="C68" s="52"/>
+      <c r="C68" s="49"/>
       <c r="D68" s="24" t="s">
         <v>211</v>
       </c>
@@ -3511,7 +3552,7 @@
       <c r="B69" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C69" s="52"/>
+      <c r="C69" s="49"/>
       <c r="D69" s="24" t="s">
         <v>214</v>
       </c>
@@ -3541,10 +3582,10 @@
       </c>
     </row>
     <row r="70" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B70" s="56" t="s">
+      <c r="B70" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="C70" s="52" t="s">
+      <c r="C70" s="49" t="s">
         <v>59</v>
       </c>
       <c r="D70" s="24" t="s">
@@ -3553,92 +3594,79 @@
       <c r="E70" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="F70" s="53" t="s">
+      <c r="F70" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="G70" s="53"/>
-      <c r="H70" s="53"/>
-      <c r="I70" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="J70" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="K70" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="L70" s="51" t="s">
+      <c r="G70" s="57"/>
+      <c r="H70" s="57"/>
+      <c r="I70" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="J70" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="K70" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="L70" s="56" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="71" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B71" s="56"/>
-      <c r="C71" s="52"/>
+      <c r="B71" s="48"/>
+      <c r="C71" s="49"/>
       <c r="D71" s="24" t="s">
         <v>218</v>
       </c>
       <c r="E71" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="F71" s="53"/>
-      <c r="G71" s="53"/>
-      <c r="H71" s="53"/>
-      <c r="I71" s="54"/>
-      <c r="J71" s="55"/>
-      <c r="K71" s="49"/>
-      <c r="L71" s="51"/>
+      <c r="F71" s="57"/>
+      <c r="G71" s="57"/>
+      <c r="H71" s="57"/>
+      <c r="I71" s="58"/>
+      <c r="J71" s="59"/>
+      <c r="K71" s="54"/>
+      <c r="L71" s="56"/>
     </row>
     <row r="72" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B72" s="56"/>
-      <c r="C72" s="52"/>
+      <c r="B72" s="48"/>
+      <c r="C72" s="49"/>
       <c r="D72" s="24" t="s">
         <v>220</v>
       </c>
       <c r="E72" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="F72" s="53"/>
-      <c r="G72" s="53"/>
-      <c r="H72" s="53"/>
-      <c r="I72" s="54"/>
-      <c r="J72" s="55"/>
-      <c r="K72" s="49"/>
-      <c r="L72" s="51"/>
+      <c r="F72" s="57"/>
+      <c r="G72" s="57"/>
+      <c r="H72" s="57"/>
+      <c r="I72" s="58"/>
+      <c r="J72" s="59"/>
+      <c r="K72" s="54"/>
+      <c r="L72" s="56"/>
     </row>
     <row r="73" spans="2:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="B73" s="56"/>
-      <c r="C73" s="52"/>
+      <c r="B73" s="48"/>
+      <c r="C73" s="49"/>
       <c r="D73" s="24" t="s">
         <v>222</v>
       </c>
       <c r="E73" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="F73" s="53"/>
-      <c r="G73" s="53"/>
-      <c r="H73" s="53"/>
-      <c r="I73" s="54"/>
-      <c r="J73" s="55"/>
-      <c r="K73" s="50"/>
-      <c r="L73" s="51"/>
+      <c r="F73" s="57"/>
+      <c r="G73" s="57"/>
+      <c r="H73" s="57"/>
+      <c r="I73" s="58"/>
+      <c r="J73" s="59"/>
+      <c r="K73" s="55"/>
+      <c r="L73" s="56"/>
     </row>
   </sheetData>
   <autoFilter ref="F5:L73"/>
   <dataConsolidate/>
   <mergeCells count="23">
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C29:C41"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="C48:C53"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C57:C62"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="C15:C21"/>
     <mergeCell ref="K70:K73"/>
     <mergeCell ref="L70:L73"/>
     <mergeCell ref="C22:C28"/>
@@ -3649,9 +3677,22 @@
     <mergeCell ref="H70:H73"/>
     <mergeCell ref="I70:I73"/>
     <mergeCell ref="J70:J73"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="C15:C21"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C29:C41"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C62"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K70 L7:L73 I7:J73">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:J73 L7:L73 K7:K70">
       <formula1>$C$3:$E$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3663,7 +3704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4295,7 +4336,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:K13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4333,7 +4376,7 @@
       </c>
       <c r="G5" s="42">
         <f>COUNTIF('CODE-TC-SRS'!K6:K78,"Done")</f>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J5" s="42" t="s">
         <v>26</v>
@@ -4356,7 +4399,7 @@
       </c>
       <c r="G6" s="44">
         <f>COUNTIF('CODE-TC-SRS'!K6:K72,"In Progress")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J6" s="43" t="s">
         <v>27</v>
@@ -4379,7 +4422,7 @@
       </c>
       <c r="G7" s="44">
         <f>COUNTIF('CODE-TC-SRS'!K6:K72, "Not Start")</f>
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J7" s="45" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
[Doc]_Commit ảnh cho các UC, Update các file doc đã làm
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -1934,11 +1934,11 @@
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="21"/>
-      <c r="I16" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>27</v>
+      <c r="I16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>26</v>
@@ -2021,8 +2021,8 @@
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="17" t="s">
-        <v>27</v>
+      <c r="I19" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>26</v>
@@ -2170,8 +2170,8 @@
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
-      <c r="I24" s="5" t="s">
-        <v>27</v>
+      <c r="I24" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>26</v>
@@ -2574,8 +2574,8 @@
       <c r="I37" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="5" t="s">
-        <v>27</v>
+      <c r="J37" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="K37" s="12" t="s">
         <v>26</v>
@@ -2603,8 +2603,8 @@
       <c r="I38" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J38" s="5" t="s">
-        <v>27</v>
+      <c r="J38" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>26</v>
@@ -2632,8 +2632,8 @@
       <c r="I39" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J39" s="5" t="s">
-        <v>27</v>
+      <c r="J39" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="K39" s="12" t="s">
         <v>26</v>
@@ -2659,8 +2659,8 @@
       <c r="I40" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J40" s="5" t="s">
-        <v>27</v>
+      <c r="J40" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>26</v>
@@ -2686,8 +2686,8 @@
       <c r="I41" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J41" s="5" t="s">
-        <v>27</v>
+      <c r="J41" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="K41" s="12" t="s">
         <v>26</v>
@@ -2883,8 +2883,8 @@
       <c r="I48" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J48" s="3" t="s">
-        <v>28</v>
+      <c r="J48" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>28</v>
@@ -2967,8 +2967,8 @@
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
-      <c r="I51" s="5" t="s">
-        <v>27</v>
+      <c r="I51" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>26</v>
@@ -3210,8 +3210,8 @@
       <c r="I59" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="J59" s="3" t="s">
-        <v>28</v>
+      <c r="J59" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="K59" s="3" t="s">
         <v>28</v>
@@ -3401,8 +3401,8 @@
       </c>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
-      <c r="I65" s="5" t="s">
-        <v>27</v>
+      <c r="I65" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>26</v>
@@ -3494,8 +3494,8 @@
         <v>42380</v>
       </c>
       <c r="H68" s="8"/>
-      <c r="I68" s="5" t="s">
-        <v>27</v>
+      <c r="I68" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>26</v>
@@ -3558,8 +3558,8 @@
       </c>
       <c r="G70" s="53"/>
       <c r="H70" s="53"/>
-      <c r="I70" s="54" t="s">
-        <v>27</v>
+      <c r="I70" s="55" t="s">
+        <v>26</v>
       </c>
       <c r="J70" s="55" t="s">
         <v>26</v>
@@ -3796,8 +3796,8 @@
       <c r="F12" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>27</v>
+      <c r="G12" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -4193,7 +4193,7 @@
         <v>46</v>
       </c>
       <c r="F45" s="29" t="s">
-        <v>235</v>
+        <v>29</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>27</v>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="C5" s="47">
         <f>COUNTIF('CODE-TC-SRS'!I7:I73,"Done")</f>
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F5" s="42" t="s">
         <v>26</v>
@@ -4340,7 +4340,7 @@
       </c>
       <c r="K5" s="42">
         <f>COUNTIF(DOC!G4:G49,"Done")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -4349,7 +4349,7 @@
       </c>
       <c r="C6" s="9">
         <f>COUNTIF('CODE-TC-SRS'!I7:I73, "In Progress")</f>
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F6" s="43" t="s">
         <v>27</v>
@@ -4363,7 +4363,7 @@
       </c>
       <c r="K6" s="44">
         <f>COUNTIF(DOC!G4:G49,"In Progress")</f>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -4430,7 +4430,7 @@
       </c>
       <c r="C10" s="42">
         <f>COUNTIF('CODE-TC-SRS'!J7:J73,"Done")</f>
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F10" s="42" t="s">
         <v>26</v>
@@ -4446,7 +4446,7 @@
       </c>
       <c r="C11" s="44">
         <f>COUNTIF('CODE-TC-SRS'!J7:J73, "In Progress")</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F11" s="43" t="s">
         <v>27</v>
@@ -4462,7 +4462,7 @@
       </c>
       <c r="C12" s="44">
         <f>COUNTIF('CODE-TC-SRS'!J7:J73, "Not Start")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12" s="45" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
[Doc]_Commit update tiến độ dự án và update file SRS
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CODE-TC-SRS" sheetId="8" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="TỔNG HỢP" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CODE-TC-SRS'!$F$5:$L$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CODE-TC-SRS'!$F$5:$M$73</definedName>
   </definedNames>
   <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="287">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -889,6 +889,18 @@
   </si>
   <si>
     <t>DOC:</t>
+  </si>
+  <si>
+    <t>Yen</t>
+  </si>
+  <si>
+    <t>Tested</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>TEST ROUND 1:</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1106,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1204,22 +1216,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1230,6 +1230,27 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1566,9 +1587,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L73"/>
+  <dimension ref="B3:M73"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K70" sqref="K70:K73"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1581,10 +1604,11 @@
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>26</v>
       </c>
@@ -1595,7 +1619,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>0</v>
       </c>
@@ -1626,26 +1650,30 @@
       <c r="K5" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="M5" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="56" t="s">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="2"/>
       <c r="J6" s="11"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="11"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="2"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>60</v>
       </c>
@@ -1676,11 +1704,12 @@
       <c r="K7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="L7" s="4"/>
+      <c r="M7" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>61</v>
       </c>
@@ -1709,17 +1738,18 @@
       <c r="K8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="56" t="s">
+      <c r="L8" s="4"/>
+      <c r="M8" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1727,8 +1757,9 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>62</v>
       </c>
@@ -1759,11 +1790,14 @@
       <c r="K10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>63</v>
       </c>
@@ -1792,11 +1826,14 @@
       <c r="K11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L11" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>64</v>
       </c>
@@ -1823,11 +1860,14 @@
       <c r="K12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="18" t="s">
+      <c r="L12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
         <v>65</v>
       </c>
@@ -1852,11 +1892,14 @@
       <c r="K13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L13" s="18" t="s">
+      <c r="L13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
         <v>66</v>
       </c>
@@ -1881,11 +1924,14 @@
       <c r="K14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="L14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="23" t="s">
         <v>67</v>
       </c>
@@ -1914,11 +1960,14 @@
       <c r="K15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>68</v>
       </c>
@@ -1943,11 +1992,14 @@
       <c r="K16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>69</v>
       </c>
@@ -1972,11 +2024,14 @@
       <c r="K17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="23" t="s">
         <v>70</v>
       </c>
@@ -2001,11 +2056,14 @@
       <c r="K18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="23" t="s">
         <v>71</v>
       </c>
@@ -2030,11 +2088,14 @@
       <c r="K19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L19" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="23" t="s">
         <v>72</v>
       </c>
@@ -2059,11 +2120,14 @@
       <c r="K20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="s">
         <v>73</v>
       </c>
@@ -2088,11 +2152,14 @@
       <c r="K21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L21" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
         <v>74</v>
       </c>
@@ -2119,13 +2186,16 @@
         <v>26</v>
       </c>
       <c r="K22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L22" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
         <v>75</v>
       </c>
@@ -2148,13 +2218,16 @@
         <v>27</v>
       </c>
       <c r="K23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L23" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="23" t="s">
         <v>76</v>
       </c>
@@ -2177,13 +2250,16 @@
         <v>26</v>
       </c>
       <c r="K24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M24" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L24" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="23" t="s">
         <v>77</v>
       </c>
@@ -2208,13 +2284,16 @@
         <v>26</v>
       </c>
       <c r="K25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M25" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L25" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="23" t="s">
         <v>78</v>
       </c>
@@ -2239,13 +2318,16 @@
         <v>26</v>
       </c>
       <c r="K26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M26" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L26" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="23" t="s">
         <v>79</v>
       </c>
@@ -2261,20 +2343,23 @@
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
-      <c r="I27" s="5" t="s">
-        <v>27</v>
+      <c r="I27" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>26</v>
       </c>
       <c r="K27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M27" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L27" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="B28" s="23" t="s">
         <v>80</v>
       </c>
@@ -2297,17 +2382,20 @@
         <v>26</v>
       </c>
       <c r="K28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M28" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L28" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="57" t="s">
+      <c r="C29" s="53" t="s">
         <v>152</v>
       </c>
       <c r="D29" s="24" t="s">
@@ -2332,15 +2420,18 @@
       <c r="K29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L29" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L29" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="58"/>
+      <c r="C30" s="54"/>
       <c r="D30" s="24" t="s">
         <v>154</v>
       </c>
@@ -2365,15 +2456,18 @@
       <c r="K30" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L30" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="58"/>
+      <c r="C31" s="54"/>
       <c r="D31" s="24" t="s">
         <v>155</v>
       </c>
@@ -2394,15 +2488,18 @@
       <c r="K31" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L31" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="58"/>
+      <c r="C32" s="54"/>
       <c r="D32" s="24" t="s">
         <v>156</v>
       </c>
@@ -2427,15 +2524,18 @@
       <c r="K32" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L32" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="58"/>
+      <c r="C33" s="54"/>
       <c r="D33" s="24" t="s">
         <v>158</v>
       </c>
@@ -2458,15 +2558,18 @@
       <c r="K33" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L33" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="58"/>
+      <c r="C34" s="54"/>
       <c r="D34" s="24" t="s">
         <v>160</v>
       </c>
@@ -2491,15 +2594,18 @@
       <c r="K34" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L34" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="58"/>
+      <c r="C35" s="54"/>
       <c r="D35" s="24" t="s">
         <v>162</v>
       </c>
@@ -2524,15 +2630,18 @@
       <c r="K35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L35" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="58"/>
+      <c r="C36" s="54"/>
       <c r="D36" s="25" t="s">
         <v>164</v>
       </c>
@@ -2553,15 +2662,18 @@
       <c r="K36" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L36" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L36" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M36" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="58"/>
+      <c r="C37" s="54"/>
       <c r="D37" s="25" t="s">
         <v>166</v>
       </c>
@@ -2580,15 +2692,18 @@
       <c r="K37" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L37" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L37" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M37" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="58"/>
+      <c r="C38" s="54"/>
       <c r="D38" s="25" t="s">
         <v>167</v>
       </c>
@@ -2609,15 +2724,18 @@
       <c r="K38" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L38" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L38" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M38" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="58"/>
+      <c r="C39" s="54"/>
       <c r="D39" s="25" t="s">
         <v>169</v>
       </c>
@@ -2638,15 +2756,18 @@
       <c r="K39" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L39" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L39" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M39" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="58"/>
+      <c r="C40" s="54"/>
       <c r="D40" s="25" t="s">
         <v>116</v>
       </c>
@@ -2665,15 +2786,18 @@
       <c r="K40" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L40" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M40" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="59"/>
+      <c r="C41" s="55"/>
       <c r="D41" s="25" t="s">
         <v>171</v>
       </c>
@@ -2692,11 +2816,14 @@
       <c r="K41" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L41" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L41" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M41" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="23" t="s">
         <v>94</v>
       </c>
@@ -2724,14 +2851,17 @@
       <c r="J42" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K42" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L42" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K42" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="L42" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M42" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="23" t="s">
         <v>95</v>
       </c>
@@ -2753,14 +2883,17 @@
       <c r="J43" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K43" s="3" t="s">
+      <c r="K43" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M43" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L43" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="23" t="s">
         <v>96</v>
       </c>
@@ -2782,14 +2915,17 @@
       <c r="J44" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K44" s="3" t="s">
+      <c r="K44" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M44" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L44" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="23" t="s">
         <v>97</v>
       </c>
@@ -2811,14 +2947,17 @@
       <c r="J45" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="K45" s="3" t="s">
+      <c r="K45" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="L45" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M45" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L45" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="B46" s="23" t="s">
         <v>98</v>
       </c>
@@ -2840,20 +2979,23 @@
       <c r="J46" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K46" s="3" t="s">
+      <c r="K46" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="L46" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M46" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L46" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="56" t="s">
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2861,8 +3003,9 @@
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M47" s="2"/>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="23" t="s">
         <v>99</v>
       </c>
@@ -2880,20 +3023,21 @@
       </c>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
-      <c r="I48" s="5" t="s">
-        <v>27</v>
+      <c r="I48" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>26</v>
       </c>
       <c r="K48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L48" s="3"/>
+      <c r="M48" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L48" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B49" s="23" t="s">
         <v>100</v>
       </c>
@@ -2916,13 +3060,14 @@
         <v>26</v>
       </c>
       <c r="K49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L49" s="3"/>
+      <c r="M49" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L49" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50" s="23" t="s">
         <v>101</v>
       </c>
@@ -2945,13 +3090,14 @@
         <v>26</v>
       </c>
       <c r="K50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L50" s="3"/>
+      <c r="M50" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L50" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B51" s="23" t="s">
         <v>102</v>
       </c>
@@ -2974,13 +3120,16 @@
         <v>26</v>
       </c>
       <c r="K51" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M51" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L51" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B52" s="23" t="s">
         <v>103</v>
       </c>
@@ -2994,20 +3143,23 @@
       </c>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
-      <c r="I52" s="5" t="s">
-        <v>27</v>
+      <c r="I52" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>26</v>
       </c>
       <c r="K52" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M52" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L52" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="23" t="s">
         <v>104</v>
       </c>
@@ -3023,20 +3175,23 @@
       </c>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
-      <c r="I53" s="5" t="s">
-        <v>27</v>
+      <c r="I53" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>26</v>
       </c>
       <c r="K53" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M53" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L53" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="23" t="s">
         <v>105</v>
       </c>
@@ -3063,13 +3218,16 @@
         <v>26</v>
       </c>
       <c r="K54" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M54" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L54" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B55" s="23" t="s">
         <v>106</v>
       </c>
@@ -3094,13 +3252,16 @@
         <v>26</v>
       </c>
       <c r="K55" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L55" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M55" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L55" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="56" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B56" s="23" t="s">
         <v>107</v>
       </c>
@@ -3123,13 +3284,16 @@
         <v>26</v>
       </c>
       <c r="K56" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M56" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L56" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B57" s="23" t="s">
         <v>108</v>
       </c>
@@ -3158,13 +3322,16 @@
         <v>26</v>
       </c>
       <c r="K57" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M57" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L57" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B58" s="23" t="s">
         <v>109</v>
       </c>
@@ -3187,11 +3354,14 @@
         <v>26</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L58" s="18"/>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M58" s="18"/>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B59" s="23" t="s">
         <v>110</v>
       </c>
@@ -3214,13 +3384,16 @@
         <v>27</v>
       </c>
       <c r="K59" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M59" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L59" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B60" s="23" t="s">
         <v>111</v>
       </c>
@@ -3247,13 +3420,16 @@
         <v>26</v>
       </c>
       <c r="K60" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M60" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L60" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B61" s="23" t="s">
         <v>115</v>
       </c>
@@ -3271,20 +3447,23 @@
       <c r="H61" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I61" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J61" s="5" t="s">
-        <v>27</v>
+      <c r="I61" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="K61" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L61" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M61" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L61" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="62" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B62" s="23" t="s">
         <v>112</v>
       </c>
@@ -3304,20 +3483,23 @@
       <c r="H62" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="I62" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J62" s="5" t="s">
-        <v>27</v>
+      <c r="I62" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="K62" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L62" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M62" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L62" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B63" s="23" t="s">
         <v>113</v>
       </c>
@@ -3346,13 +3528,16 @@
         <v>26</v>
       </c>
       <c r="K63" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L63" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M63" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L63" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B64" s="23" t="s">
         <v>199</v>
       </c>
@@ -3379,13 +3564,16 @@
         <v>26</v>
       </c>
       <c r="K64" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L64" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M64" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L64" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B65" s="23" t="s">
         <v>202</v>
       </c>
@@ -3408,13 +3596,16 @@
         <v>26</v>
       </c>
       <c r="K65" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L65" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M65" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L65" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B66" s="23" t="s">
         <v>205</v>
       </c>
@@ -3435,13 +3626,16 @@
       </c>
       <c r="J66" s="12"/>
       <c r="K66" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L66" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M66" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L66" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B67" s="23" t="s">
         <v>208</v>
       </c>
@@ -3467,16 +3661,19 @@
         <v>26</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>26</v>
+        <v>285</v>
       </c>
       <c r="K67" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L67" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M67" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L67" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B68" s="23" t="s">
         <v>210</v>
       </c>
@@ -3501,13 +3698,16 @@
         <v>26</v>
       </c>
       <c r="K68" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L68" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M68" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L68" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B69" s="23" t="s">
         <v>213</v>
       </c>
@@ -3534,14 +3734,17 @@
         <v>26</v>
       </c>
       <c r="K69" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L69" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M69" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L69" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="70" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B70" s="56" t="s">
+    </row>
+    <row r="70" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B70" s="51" t="s">
         <v>215</v>
       </c>
       <c r="C70" s="52" t="s">
@@ -3553,26 +3756,27 @@
       <c r="E70" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="F70" s="53" t="s">
+      <c r="F70" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="G70" s="53"/>
-      <c r="H70" s="53"/>
-      <c r="I70" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="J70" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="K70" s="48" t="s">
+      <c r="G70" s="60"/>
+      <c r="H70" s="60"/>
+      <c r="I70" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="J70" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="K70" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="L70" s="51" t="s">
+      <c r="L70" s="48"/>
+      <c r="M70" s="59" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B71" s="56"/>
+    <row r="71" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B71" s="51"/>
       <c r="C71" s="52"/>
       <c r="D71" s="24" t="s">
         <v>218</v>
@@ -3580,16 +3784,17 @@
       <c r="E71" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="F71" s="53"/>
-      <c r="G71" s="53"/>
-      <c r="H71" s="53"/>
-      <c r="I71" s="54"/>
-      <c r="J71" s="55"/>
-      <c r="K71" s="49"/>
-      <c r="L71" s="51"/>
-    </row>
-    <row r="72" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B72" s="56"/>
+      <c r="F71" s="60"/>
+      <c r="G71" s="60"/>
+      <c r="H71" s="60"/>
+      <c r="I71" s="62"/>
+      <c r="J71" s="61"/>
+      <c r="K71" s="57"/>
+      <c r="L71" s="49"/>
+      <c r="M71" s="59"/>
+    </row>
+    <row r="72" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B72" s="51"/>
       <c r="C72" s="52"/>
       <c r="D72" s="24" t="s">
         <v>220</v>
@@ -3597,16 +3802,17 @@
       <c r="E72" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="F72" s="53"/>
-      <c r="G72" s="53"/>
-      <c r="H72" s="53"/>
-      <c r="I72" s="54"/>
-      <c r="J72" s="55"/>
-      <c r="K72" s="49"/>
-      <c r="L72" s="51"/>
-    </row>
-    <row r="73" spans="2:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="B73" s="56"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
+      <c r="H72" s="60"/>
+      <c r="I72" s="62"/>
+      <c r="J72" s="61"/>
+      <c r="K72" s="57"/>
+      <c r="L72" s="49"/>
+      <c r="M72" s="59"/>
+    </row>
+    <row r="73" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="B73" s="51"/>
       <c r="C73" s="52"/>
       <c r="D73" s="24" t="s">
         <v>222</v>
@@ -3614,18 +3820,34 @@
       <c r="E73" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="F73" s="53"/>
-      <c r="G73" s="53"/>
-      <c r="H73" s="53"/>
-      <c r="I73" s="54"/>
-      <c r="J73" s="55"/>
-      <c r="K73" s="50"/>
-      <c r="L73" s="51"/>
+      <c r="F73" s="60"/>
+      <c r="G73" s="60"/>
+      <c r="H73" s="60"/>
+      <c r="I73" s="62"/>
+      <c r="J73" s="61"/>
+      <c r="K73" s="58"/>
+      <c r="L73" s="50"/>
+      <c r="M73" s="59"/>
     </row>
   </sheetData>
-  <autoFilter ref="F5:L73"/>
+  <autoFilter ref="F5:M73"/>
   <dataConsolidate/>
   <mergeCells count="23">
+    <mergeCell ref="K70:K73"/>
+    <mergeCell ref="M70:M73"/>
+    <mergeCell ref="C22:C28"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C67:C69"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="G70:G73"/>
+    <mergeCell ref="H70:H73"/>
+    <mergeCell ref="I70:I73"/>
+    <mergeCell ref="J70:J73"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="C15:C21"/>
     <mergeCell ref="B70:B73"/>
     <mergeCell ref="C70:C73"/>
     <mergeCell ref="C29:C41"/>
@@ -3634,24 +3856,9 @@
     <mergeCell ref="C48:C53"/>
     <mergeCell ref="C54:C56"/>
     <mergeCell ref="C57:C62"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="C15:C21"/>
-    <mergeCell ref="K70:K73"/>
-    <mergeCell ref="L70:L73"/>
-    <mergeCell ref="C22:C28"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="C67:C69"/>
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="G70:G73"/>
-    <mergeCell ref="H70:H73"/>
-    <mergeCell ref="I70:I73"/>
-    <mergeCell ref="J70:J73"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K70 L7:L73 I7:J73">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:J73 M7:M73 K7:L70">
       <formula1>$C$3:$E$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3663,7 +3870,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3694,7 +3903,7 @@
       <c r="B5" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="63" t="s">
         <v>279</v>
       </c>
       <c r="E5" s="39" t="s">
@@ -3711,7 +3920,7 @@
       <c r="B6" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="D6" s="61"/>
+      <c r="D6" s="64"/>
       <c r="E6" s="36" t="s">
         <v>278</v>
       </c>
@@ -3726,7 +3935,7 @@
       <c r="B7" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="D7" s="61"/>
+      <c r="D7" s="64"/>
       <c r="E7" s="36" t="s">
         <v>277</v>
       </c>
@@ -3741,7 +3950,7 @@
       <c r="B8" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="61"/>
+      <c r="D8" s="64"/>
       <c r="E8" s="36" t="s">
         <v>239</v>
       </c>
@@ -3753,7 +3962,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="61"/>
+      <c r="D9" s="64"/>
       <c r="E9" s="36" t="s">
         <v>276</v>
       </c>
@@ -3765,7 +3974,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="61"/>
+      <c r="D10" s="64"/>
       <c r="E10" s="36" t="s">
         <v>275</v>
       </c>
@@ -3777,7 +3986,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="61"/>
+      <c r="D11" s="64"/>
       <c r="E11" s="36" t="s">
         <v>274</v>
       </c>
@@ -3789,7 +3998,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="62"/>
+      <c r="D12" s="65"/>
       <c r="E12" s="36" t="s">
         <v>273</v>
       </c>
@@ -3801,7 +4010,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="66" t="s">
         <v>272</v>
       </c>
       <c r="E13" s="38" t="s">
@@ -3815,7 +4024,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="64"/>
+      <c r="D14" s="67"/>
       <c r="E14" s="38" t="s">
         <v>234</v>
       </c>
@@ -3827,7 +4036,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="64"/>
+      <c r="D15" s="67"/>
       <c r="E15" s="38" t="s">
         <v>271</v>
       </c>
@@ -3839,7 +4048,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D16" s="64"/>
+      <c r="D16" s="67"/>
       <c r="E16" s="37" t="s">
         <v>270</v>
       </c>
@@ -3851,7 +4060,7 @@
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D17" s="64"/>
+      <c r="D17" s="67"/>
       <c r="E17" s="37" t="s">
         <v>269</v>
       </c>
@@ -3863,7 +4072,7 @@
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="65"/>
+      <c r="D18" s="68"/>
       <c r="E18" s="37" t="s">
         <v>268</v>
       </c>
@@ -3873,7 +4082,7 @@
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="63" t="s">
         <v>267</v>
       </c>
       <c r="E19" s="36" t="s">
@@ -3887,7 +4096,7 @@
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="61"/>
+      <c r="D20" s="64"/>
       <c r="E20" s="36" t="s">
         <v>266</v>
       </c>
@@ -3899,7 +4108,7 @@
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="61"/>
+      <c r="D21" s="64"/>
       <c r="E21" s="36" t="s">
         <v>265</v>
       </c>
@@ -3911,7 +4120,7 @@
       </c>
     </row>
     <row r="22" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D22" s="62"/>
+      <c r="D22" s="65"/>
       <c r="E22" s="36" t="s">
         <v>264</v>
       </c>
@@ -3923,7 +4132,7 @@
       </c>
     </row>
     <row r="23" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D23" s="63" t="s">
+      <c r="D23" s="66" t="s">
         <v>263</v>
       </c>
       <c r="E23" s="37" t="s">
@@ -3937,7 +4146,7 @@
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="64"/>
+      <c r="D24" s="67"/>
       <c r="E24" s="37" t="s">
         <v>261</v>
       </c>
@@ -3949,7 +4158,7 @@
       </c>
     </row>
     <row r="25" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D25" s="64"/>
+      <c r="D25" s="67"/>
       <c r="E25" s="37" t="s">
         <v>260</v>
       </c>
@@ -3961,7 +4170,7 @@
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="65"/>
+      <c r="D26" s="68"/>
       <c r="E26" s="37" t="s">
         <v>259</v>
       </c>
@@ -3973,7 +4182,7 @@
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="60" t="s">
+      <c r="D27" s="63" t="s">
         <v>258</v>
       </c>
       <c r="E27" s="36" t="s">
@@ -3987,7 +4196,7 @@
       </c>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="61"/>
+      <c r="D28" s="64"/>
       <c r="E28" s="36" t="s">
         <v>256</v>
       </c>
@@ -3999,7 +4208,7 @@
       </c>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="62"/>
+      <c r="D29" s="65"/>
       <c r="E29" s="36" t="s">
         <v>255</v>
       </c>
@@ -4011,7 +4220,7 @@
       </c>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="66" t="s">
+      <c r="D30" s="69" t="s">
         <v>254</v>
       </c>
       <c r="E30" s="35" t="s">
@@ -4023,7 +4232,7 @@
       </c>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="66"/>
+      <c r="D31" s="69"/>
       <c r="E31" s="35" t="s">
         <v>252</v>
       </c>
@@ -4033,7 +4242,7 @@
       </c>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D32" s="66"/>
+      <c r="D32" s="69"/>
       <c r="E32" s="35" t="s">
         <v>251</v>
       </c>
@@ -4043,7 +4252,7 @@
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D33" s="66"/>
+      <c r="D33" s="69"/>
       <c r="E33" s="35" t="s">
         <v>250</v>
       </c>
@@ -4053,7 +4262,7 @@
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="66"/>
+      <c r="D34" s="69"/>
       <c r="E34" s="2" t="s">
         <v>249</v>
       </c>
@@ -4065,7 +4274,7 @@
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D35" s="60" t="s">
+      <c r="D35" s="63" t="s">
         <v>248</v>
       </c>
       <c r="E35" s="34" t="s">
@@ -4079,7 +4288,7 @@
       </c>
     </row>
     <row r="36" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D36" s="61"/>
+      <c r="D36" s="64"/>
       <c r="E36" s="30" t="s">
         <v>246</v>
       </c>
@@ -4091,7 +4300,7 @@
       </c>
     </row>
     <row r="37" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D37" s="61"/>
+      <c r="D37" s="64"/>
       <c r="E37" s="31" t="s">
         <v>245</v>
       </c>
@@ -4103,7 +4312,7 @@
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D38" s="61"/>
+      <c r="D38" s="64"/>
       <c r="E38" s="31" t="s">
         <v>243</v>
       </c>
@@ -4115,7 +4324,7 @@
       </c>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D39" s="61"/>
+      <c r="D39" s="64"/>
       <c r="E39" s="31" t="s">
         <v>242</v>
       </c>
@@ -4127,7 +4336,7 @@
       </c>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D40" s="61"/>
+      <c r="D40" s="64"/>
       <c r="E40" s="28" t="s">
         <v>241</v>
       </c>
@@ -4139,7 +4348,7 @@
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D41" s="61"/>
+      <c r="D41" s="64"/>
       <c r="E41" s="28" t="s">
         <v>240</v>
       </c>
@@ -4151,7 +4360,7 @@
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D42" s="61"/>
+      <c r="D42" s="64"/>
       <c r="E42" s="28" t="s">
         <v>239</v>
       </c>
@@ -4163,7 +4372,7 @@
       </c>
     </row>
     <row r="43" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D43" s="61"/>
+      <c r="D43" s="64"/>
       <c r="E43" s="28" t="s">
         <v>238</v>
       </c>
@@ -4175,7 +4384,7 @@
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D44" s="61"/>
+      <c r="D44" s="64"/>
       <c r="E44" s="28" t="s">
         <v>236</v>
       </c>
@@ -4188,7 +4397,7 @@
       </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D45" s="61"/>
+      <c r="D45" s="64"/>
       <c r="E45" s="30" t="s">
         <v>46</v>
       </c>
@@ -4198,12 +4407,15 @@
       <c r="G45" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="H45" s="1" t="s">
+        <v>283</v>
+      </c>
       <c r="I45" s="32" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D46" s="61"/>
+      <c r="D46" s="64"/>
       <c r="E46" s="31" t="s">
         <v>234</v>
       </c>
@@ -4218,7 +4430,7 @@
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D47" s="61"/>
+      <c r="D47" s="64"/>
       <c r="E47" s="31" t="s">
         <v>232</v>
       </c>
@@ -4230,7 +4442,7 @@
       </c>
     </row>
     <row r="48" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D48" s="61"/>
+      <c r="D48" s="64"/>
       <c r="E48" s="30" t="s">
         <v>231</v>
       </c>
@@ -4242,7 +4454,7 @@
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" s="61"/>
+      <c r="D49" s="64"/>
       <c r="E49" s="30" t="s">
         <v>229</v>
       </c>
@@ -4254,7 +4466,7 @@
       </c>
     </row>
     <row r="50" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D50" s="62"/>
+      <c r="D50" s="65"/>
       <c r="E50" s="28" t="s">
         <v>228</v>
       </c>
@@ -4295,7 +4507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:K13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4326,14 +4538,14 @@
       </c>
       <c r="C5" s="47">
         <f>COUNTIF('CODE-TC-SRS'!I7:I73,"Done")</f>
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F5" s="42" t="s">
         <v>26</v>
       </c>
       <c r="G5" s="42">
         <f>COUNTIF('CODE-TC-SRS'!K6:K78,"Done")</f>
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="J5" s="42" t="s">
         <v>26</v>
@@ -4349,14 +4561,14 @@
       </c>
       <c r="C6" s="9">
         <f>COUNTIF('CODE-TC-SRS'!I7:I73, "In Progress")</f>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F6" s="43" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="44">
         <f>COUNTIF('CODE-TC-SRS'!K6:K72,"In Progress")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J6" s="43" t="s">
         <v>27</v>
@@ -4379,7 +4591,7 @@
       </c>
       <c r="G7" s="44">
         <f>COUNTIF('CODE-TC-SRS'!K6:K72, "Not Start")</f>
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="J7" s="45" t="s">
         <v>28</v>
@@ -4421,6 +4633,9 @@
       <c r="E9" s="41" t="s">
         <v>52</v>
       </c>
+      <c r="I9" s="41" t="s">
+        <v>286</v>
+      </c>
       <c r="J9" s="46"/>
       <c r="K9" s="46"/>
     </row>
@@ -4430,14 +4645,21 @@
       </c>
       <c r="C10" s="42">
         <f>COUNTIF('CODE-TC-SRS'!J7:J73,"Done")</f>
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F10" s="42" t="s">
         <v>26</v>
       </c>
       <c r="G10" s="42">
+        <f>COUNTIF('CODE-TC-SRS'!M7:M73,"Done")</f>
+        <v>26</v>
+      </c>
+      <c r="J10" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="42">
         <f>COUNTIF('CODE-TC-SRS'!L7:L73,"Done")</f>
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -4446,14 +4668,21 @@
       </c>
       <c r="C11" s="44">
         <f>COUNTIF('CODE-TC-SRS'!J7:J73, "In Progress")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" s="43" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="44">
+        <f>COUNTIF('CODE-TC-SRS'!M7:M73,"In Progress")</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="44">
         <f>COUNTIF('CODE-TC-SRS'!L7:L73,"In Progress")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -4468,8 +4697,15 @@
         <v>28</v>
       </c>
       <c r="G12" s="44">
+        <f>COUNTIF('CODE-TC-SRS'!M7:M73, "Not Start")</f>
+        <v>35</v>
+      </c>
+      <c r="J12" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="44">
         <f>COUNTIF('CODE-TC-SRS'!L7:L73, "Not Start")</f>
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -4487,10 +4723,17 @@
         <f>SUM(G10:G12)</f>
         <v>61</v>
       </c>
+      <c r="J13" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="44">
+        <f>SUM(K10:K12)</f>
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5:C7">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4502,6 +4745,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C12">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:K8">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -4513,7 +4768,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5:K8">
+  <conditionalFormatting sqref="F5:G8">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -4525,7 +4780,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5:G8">
+  <conditionalFormatting sqref="F10:G12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4537,7 +4792,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:G12">
+  <conditionalFormatting sqref="J10:K13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
[Doc]_Commit doc cho các file report
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7500" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CODE-TC-SRS" sheetId="8" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="291">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -901,6 +901,18 @@
   </si>
   <si>
     <t>TEST ROUND 1:</t>
+  </si>
+  <si>
+    <t>Hai</t>
+  </si>
+  <si>
+    <t>chưa thấy Yến commit</t>
+  </si>
+  <si>
+    <t>còn integration TC</t>
+  </si>
+  <si>
+    <t>test result đang bị lỗi công thức</t>
   </si>
 </sst>
 </file>
@@ -973,7 +985,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1022,6 +1034,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1106,7 +1124,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1215,6 +1233,22 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1589,9 +1623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:M73"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K70" sqref="K70:K73"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1658,12 +1690,12 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1677,7 +1709,7 @@
       <c r="B7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="58" t="s">
         <v>118</v>
       </c>
       <c r="D7" s="24" t="s">
@@ -1713,7 +1745,7 @@
       <c r="B8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="52"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="24" t="s">
         <v>8</v>
       </c>
@@ -1744,12 +1776,12 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1763,7 +1795,7 @@
       <c r="B10" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="58" t="s">
         <v>121</v>
       </c>
       <c r="D10" s="24" t="s">
@@ -1801,7 +1833,7 @@
       <c r="B11" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="52"/>
+      <c r="C11" s="58"/>
       <c r="D11" s="24" t="s">
         <v>6</v>
       </c>
@@ -1837,7 +1869,7 @@
       <c r="B12" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="52"/>
+      <c r="C12" s="58"/>
       <c r="D12" s="24" t="s">
         <v>123</v>
       </c>
@@ -1871,7 +1903,7 @@
       <c r="B13" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="52"/>
+      <c r="C13" s="58"/>
       <c r="D13" s="24" t="s">
         <v>125</v>
       </c>
@@ -1903,7 +1935,7 @@
       <c r="B14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="52"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="24" t="s">
         <v>126</v>
       </c>
@@ -1935,7 +1967,7 @@
       <c r="B15" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="58" t="s">
         <v>128</v>
       </c>
       <c r="D15" s="24" t="s">
@@ -1971,7 +2003,7 @@
       <c r="B16" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="52"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="25" t="s">
         <v>130</v>
       </c>
@@ -2003,7 +2035,7 @@
       <c r="B17" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="52"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="24" t="s">
         <v>132</v>
       </c>
@@ -2035,7 +2067,7 @@
       <c r="B18" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="52"/>
+      <c r="C18" s="58"/>
       <c r="D18" s="24" t="s">
         <v>134</v>
       </c>
@@ -2067,7 +2099,7 @@
       <c r="B19" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="52"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="24" t="s">
         <v>48</v>
       </c>
@@ -2099,7 +2131,7 @@
       <c r="B20" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="52"/>
+      <c r="C20" s="58"/>
       <c r="D20" s="24" t="s">
         <v>9</v>
       </c>
@@ -2131,7 +2163,7 @@
       <c r="B21" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="52"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="24" t="s">
         <v>137</v>
       </c>
@@ -2163,7 +2195,7 @@
       <c r="B22" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="58" t="s">
         <v>139</v>
       </c>
       <c r="D22" s="24" t="s">
@@ -2185,7 +2217,7 @@
       <c r="J22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K22" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L22" s="4" t="s">
@@ -2199,31 +2231,31 @@
       <c r="B23" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="25" t="s">
+      <c r="C23" s="58"/>
+      <c r="D23" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M23" s="18" t="s">
+      <c r="G23" s="54"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="L23" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" s="56" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2231,7 +2263,7 @@
       <c r="B24" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="52"/>
+      <c r="C24" s="58"/>
       <c r="D24" s="24" t="s">
         <v>144</v>
       </c>
@@ -2249,7 +2281,7 @@
       <c r="J24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K24" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L24" s="4" t="s">
@@ -2263,7 +2295,7 @@
       <c r="B25" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="52"/>
+      <c r="C25" s="58"/>
       <c r="D25" s="24" t="s">
         <v>10</v>
       </c>
@@ -2283,7 +2315,7 @@
       <c r="J25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="K25" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L25" s="4" t="s">
@@ -2297,7 +2329,7 @@
       <c r="B26" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="52"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="24" t="s">
         <v>147</v>
       </c>
@@ -2317,7 +2349,7 @@
       <c r="J26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="K26" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L26" s="4" t="s">
@@ -2331,7 +2363,7 @@
       <c r="B27" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="52"/>
+      <c r="C27" s="58"/>
       <c r="D27" s="24" t="s">
         <v>11</v>
       </c>
@@ -2349,7 +2381,7 @@
       <c r="J27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="K27" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L27" s="4" t="s">
@@ -2363,7 +2395,7 @@
       <c r="B28" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="52"/>
+      <c r="C28" s="58"/>
       <c r="D28" s="25" t="s">
         <v>150</v>
       </c>
@@ -2381,7 +2413,7 @@
       <c r="J28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="K28" s="5" t="s">
         <v>27</v>
       </c>
       <c r="L28" s="4" t="s">
@@ -2395,7 +2427,7 @@
       <c r="B29" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="53" t="s">
+      <c r="C29" s="59" t="s">
         <v>152</v>
       </c>
       <c r="D29" s="24" t="s">
@@ -2431,7 +2463,7 @@
       <c r="B30" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="54"/>
+      <c r="C30" s="60"/>
       <c r="D30" s="24" t="s">
         <v>154</v>
       </c>
@@ -2467,7 +2499,7 @@
       <c r="B31" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="54"/>
+      <c r="C31" s="60"/>
       <c r="D31" s="24" t="s">
         <v>155</v>
       </c>
@@ -2499,7 +2531,7 @@
       <c r="B32" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="54"/>
+      <c r="C32" s="60"/>
       <c r="D32" s="24" t="s">
         <v>156</v>
       </c>
@@ -2535,7 +2567,7 @@
       <c r="B33" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="54"/>
+      <c r="C33" s="60"/>
       <c r="D33" s="24" t="s">
         <v>158</v>
       </c>
@@ -2569,7 +2601,7 @@
       <c r="B34" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="54"/>
+      <c r="C34" s="60"/>
       <c r="D34" s="24" t="s">
         <v>160</v>
       </c>
@@ -2605,7 +2637,7 @@
       <c r="B35" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="54"/>
+      <c r="C35" s="60"/>
       <c r="D35" s="24" t="s">
         <v>162</v>
       </c>
@@ -2641,7 +2673,7 @@
       <c r="B36" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="54"/>
+      <c r="C36" s="60"/>
       <c r="D36" s="25" t="s">
         <v>164</v>
       </c>
@@ -2673,7 +2705,7 @@
       <c r="B37" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="54"/>
+      <c r="C37" s="60"/>
       <c r="D37" s="25" t="s">
         <v>166</v>
       </c>
@@ -2703,7 +2735,7 @@
       <c r="B38" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="54"/>
+      <c r="C38" s="60"/>
       <c r="D38" s="25" t="s">
         <v>167</v>
       </c>
@@ -2735,7 +2767,7 @@
       <c r="B39" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="54"/>
+      <c r="C39" s="60"/>
       <c r="D39" s="25" t="s">
         <v>169</v>
       </c>
@@ -2767,7 +2799,7 @@
       <c r="B40" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="54"/>
+      <c r="C40" s="60"/>
       <c r="D40" s="25" t="s">
         <v>116</v>
       </c>
@@ -2797,7 +2829,7 @@
       <c r="B41" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="55"/>
+      <c r="C41" s="61"/>
       <c r="D41" s="25" t="s">
         <v>171</v>
       </c>
@@ -2827,7 +2859,7 @@
       <c r="B42" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="52" t="s">
+      <c r="C42" s="58" t="s">
         <v>172</v>
       </c>
       <c r="D42" s="24" t="s">
@@ -2851,7 +2883,7 @@
       <c r="J42" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K42" s="20" t="s">
+      <c r="K42" s="51" t="s">
         <v>26</v>
       </c>
       <c r="L42" s="4" t="s">
@@ -2865,7 +2897,7 @@
       <c r="B43" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="52"/>
+      <c r="C43" s="58"/>
       <c r="D43" s="24" t="s">
         <v>117</v>
       </c>
@@ -2883,7 +2915,7 @@
       <c r="J43" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K43" s="20" t="s">
+      <c r="K43" s="51" t="s">
         <v>26</v>
       </c>
       <c r="L43" s="4" t="s">
@@ -2897,7 +2929,7 @@
       <c r="B44" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="52"/>
+      <c r="C44" s="58"/>
       <c r="D44" s="24" t="s">
         <v>175</v>
       </c>
@@ -2915,7 +2947,7 @@
       <c r="J44" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K44" s="20" t="s">
+      <c r="K44" s="51" t="s">
         <v>26</v>
       </c>
       <c r="L44" s="4" t="s">
@@ -2929,7 +2961,7 @@
       <c r="B45" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="52"/>
+      <c r="C45" s="58"/>
       <c r="D45" s="25" t="s">
         <v>177</v>
       </c>
@@ -2961,7 +2993,7 @@
       <c r="B46" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="52"/>
+      <c r="C46" s="58"/>
       <c r="D46" s="24" t="s">
         <v>178</v>
       </c>
@@ -2990,12 +3022,12 @@
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="51" t="s">
+      <c r="B47" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
-      <c r="E47" s="51"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -3009,7 +3041,7 @@
       <c r="B48" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="52" t="s">
+      <c r="C48" s="58" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="25" t="s">
@@ -3029,7 +3061,7 @@
       <c r="J48" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K48" s="3" t="s">
+      <c r="K48" s="5" t="s">
         <v>27</v>
       </c>
       <c r="L48" s="3"/>
@@ -3041,7 +3073,7 @@
       <c r="B49" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="52"/>
+      <c r="C49" s="58"/>
       <c r="D49" s="24" t="s">
         <v>17</v>
       </c>
@@ -3059,7 +3091,7 @@
       <c r="J49" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K49" s="3" t="s">
+      <c r="K49" s="5" t="s">
         <v>27</v>
       </c>
       <c r="L49" s="3"/>
@@ -3071,7 +3103,7 @@
       <c r="B50" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="52"/>
+      <c r="C50" s="58"/>
       <c r="D50" s="24" t="s">
         <v>18</v>
       </c>
@@ -3089,7 +3121,7 @@
       <c r="J50" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K50" s="3" t="s">
+      <c r="K50" s="5" t="s">
         <v>27</v>
       </c>
       <c r="L50" s="3"/>
@@ -3101,7 +3133,7 @@
       <c r="B51" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="52"/>
+      <c r="C51" s="58"/>
       <c r="D51" s="24" t="s">
         <v>182</v>
       </c>
@@ -3119,7 +3151,7 @@
       <c r="J51" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K51" s="3" t="s">
+      <c r="K51" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L51" s="3" t="s">
@@ -3133,7 +3165,7 @@
       <c r="B52" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="52"/>
+      <c r="C52" s="58"/>
       <c r="D52" s="24" t="s">
         <v>183</v>
       </c>
@@ -3149,7 +3181,7 @@
       <c r="J52" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K52" s="3" t="s">
+      <c r="K52" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L52" s="3" t="s">
@@ -3163,7 +3195,7 @@
       <c r="B53" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="52"/>
+      <c r="C53" s="58"/>
       <c r="D53" s="24" t="s">
         <v>184</v>
       </c>
@@ -3181,7 +3213,7 @@
       <c r="J53" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K53" s="3" t="s">
+      <c r="K53" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L53" s="3" t="s">
@@ -3195,7 +3227,7 @@
       <c r="B54" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="52" t="s">
+      <c r="C54" s="58" t="s">
         <v>54</v>
       </c>
       <c r="D54" s="24" t="s">
@@ -3217,7 +3249,7 @@
       <c r="J54" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K54" s="3" t="s">
+      <c r="K54" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L54" s="3" t="s">
@@ -3231,7 +3263,7 @@
       <c r="B55" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="52"/>
+      <c r="C55" s="58"/>
       <c r="D55" s="24" t="s">
         <v>44</v>
       </c>
@@ -3251,7 +3283,7 @@
       <c r="J55" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K55" s="3" t="s">
+      <c r="K55" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L55" s="3" t="s">
@@ -3265,7 +3297,7 @@
       <c r="B56" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="52"/>
+      <c r="C56" s="58"/>
       <c r="D56" s="24" t="s">
         <v>187</v>
       </c>
@@ -3283,7 +3315,7 @@
       <c r="J56" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K56" s="3" t="s">
+      <c r="K56" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L56" s="3" t="s">
@@ -3297,7 +3329,7 @@
       <c r="B57" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="52" t="s">
+      <c r="C57" s="58" t="s">
         <v>55</v>
       </c>
       <c r="D57" s="24" t="s">
@@ -3321,7 +3353,7 @@
       <c r="J57" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K57" s="3" t="s">
+      <c r="K57" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L57" s="3" t="s">
@@ -3335,7 +3367,7 @@
       <c r="B58" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="52"/>
+      <c r="C58" s="58"/>
       <c r="D58" s="24" t="s">
         <v>190</v>
       </c>
@@ -3353,7 +3385,7 @@
       <c r="J58" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K58" s="3" t="s">
+      <c r="K58" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L58" s="3" t="s">
@@ -3365,7 +3397,7 @@
       <c r="B59" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C59" s="52"/>
+      <c r="C59" s="58"/>
       <c r="D59" s="24" t="s">
         <v>192</v>
       </c>
@@ -3383,7 +3415,7 @@
       <c r="J59" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="K59" s="3" t="s">
+      <c r="K59" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L59" s="3" t="s">
@@ -3397,7 +3429,7 @@
       <c r="B60" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="52"/>
+      <c r="C60" s="58"/>
       <c r="D60" s="24" t="s">
         <v>19</v>
       </c>
@@ -3419,7 +3451,7 @@
       <c r="J60" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K60" s="3" t="s">
+      <c r="K60" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L60" s="3" t="s">
@@ -3433,7 +3465,7 @@
       <c r="B61" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C61" s="52"/>
+      <c r="C61" s="58"/>
       <c r="D61" s="24" t="s">
         <v>195</v>
       </c>
@@ -3453,7 +3485,7 @@
       <c r="J61" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K61" s="3" t="s">
+      <c r="K61" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L61" s="3" t="s">
@@ -3467,7 +3499,7 @@
       <c r="B62" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="52"/>
+      <c r="C62" s="58"/>
       <c r="D62" s="24" t="s">
         <v>196</v>
       </c>
@@ -3489,7 +3521,7 @@
       <c r="J62" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K62" s="3" t="s">
+      <c r="K62" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L62" s="3" t="s">
@@ -3503,7 +3535,7 @@
       <c r="B63" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="C63" s="52" t="s">
+      <c r="C63" s="58" t="s">
         <v>57</v>
       </c>
       <c r="D63" s="24" t="s">
@@ -3527,7 +3559,7 @@
       <c r="J63" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K63" s="3" t="s">
+      <c r="K63" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L63" s="3" t="s">
@@ -3541,7 +3573,7 @@
       <c r="B64" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="C64" s="52"/>
+      <c r="C64" s="58"/>
       <c r="D64" s="24" t="s">
         <v>200</v>
       </c>
@@ -3563,7 +3595,7 @@
       <c r="J64" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K64" s="3" t="s">
+      <c r="K64" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L64" s="3" t="s">
@@ -3577,7 +3609,7 @@
       <c r="B65" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="C65" s="52"/>
+      <c r="C65" s="58"/>
       <c r="D65" s="24" t="s">
         <v>203</v>
       </c>
@@ -3595,7 +3627,7 @@
       <c r="J65" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K65" s="3" t="s">
+      <c r="K65" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L65" s="3" t="s">
@@ -3609,7 +3641,7 @@
       <c r="B66" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="C66" s="52"/>
+      <c r="C66" s="58"/>
       <c r="D66" s="24" t="s">
         <v>206</v>
       </c>
@@ -3625,7 +3657,7 @@
         <v>26</v>
       </c>
       <c r="J66" s="12"/>
-      <c r="K66" s="3" t="s">
+      <c r="K66" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L66" s="3" t="s">
@@ -3639,7 +3671,7 @@
       <c r="B67" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="C67" s="52" t="s">
+      <c r="C67" s="58" t="s">
         <v>58</v>
       </c>
       <c r="D67" s="24" t="s">
@@ -3663,7 +3695,7 @@
       <c r="J67" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="K67" s="3" t="s">
+      <c r="K67" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L67" s="3" t="s">
@@ -3677,7 +3709,7 @@
       <c r="B68" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="C68" s="52"/>
+      <c r="C68" s="58"/>
       <c r="D68" s="24" t="s">
         <v>211</v>
       </c>
@@ -3697,7 +3729,7 @@
       <c r="J68" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K68" s="3" t="s">
+      <c r="K68" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L68" s="3" t="s">
@@ -3711,7 +3743,7 @@
       <c r="B69" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C69" s="52"/>
+      <c r="C69" s="58"/>
       <c r="D69" s="24" t="s">
         <v>214</v>
       </c>
@@ -3733,7 +3765,7 @@
       <c r="J69" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K69" s="3" t="s">
+      <c r="K69" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L69" s="3" t="s">
@@ -3744,10 +3776,10 @@
       </c>
     </row>
     <row r="70" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B70" s="51" t="s">
+      <c r="B70" s="57" t="s">
         <v>215</v>
       </c>
-      <c r="C70" s="52" t="s">
+      <c r="C70" s="58" t="s">
         <v>59</v>
       </c>
       <c r="D70" s="24" t="s">
@@ -3756,78 +3788,78 @@
       <c r="E70" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="F70" s="60" t="s">
+      <c r="F70" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="G70" s="60"/>
-      <c r="H70" s="60"/>
-      <c r="I70" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="J70" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="K70" s="56" t="s">
+      <c r="G70" s="66"/>
+      <c r="H70" s="66"/>
+      <c r="I70" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="J70" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="K70" s="62" t="s">
         <v>28</v>
       </c>
       <c r="L70" s="48"/>
-      <c r="M70" s="59" t="s">
+      <c r="M70" s="65" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="71" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B71" s="51"/>
-      <c r="C71" s="52"/>
+      <c r="B71" s="57"/>
+      <c r="C71" s="58"/>
       <c r="D71" s="24" t="s">
         <v>218</v>
       </c>
       <c r="E71" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="F71" s="60"/>
-      <c r="G71" s="60"/>
-      <c r="H71" s="60"/>
-      <c r="I71" s="62"/>
-      <c r="J71" s="61"/>
-      <c r="K71" s="57"/>
+      <c r="F71" s="66"/>
+      <c r="G71" s="66"/>
+      <c r="H71" s="66"/>
+      <c r="I71" s="68"/>
+      <c r="J71" s="67"/>
+      <c r="K71" s="63"/>
       <c r="L71" s="49"/>
-      <c r="M71" s="59"/>
+      <c r="M71" s="65"/>
     </row>
     <row r="72" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B72" s="51"/>
-      <c r="C72" s="52"/>
+      <c r="B72" s="57"/>
+      <c r="C72" s="58"/>
       <c r="D72" s="24" t="s">
         <v>220</v>
       </c>
       <c r="E72" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="F72" s="60"/>
-      <c r="G72" s="60"/>
-      <c r="H72" s="60"/>
-      <c r="I72" s="62"/>
-      <c r="J72" s="61"/>
-      <c r="K72" s="57"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
+      <c r="H72" s="66"/>
+      <c r="I72" s="68"/>
+      <c r="J72" s="67"/>
+      <c r="K72" s="63"/>
       <c r="L72" s="49"/>
-      <c r="M72" s="59"/>
+      <c r="M72" s="65"/>
     </row>
     <row r="73" spans="2:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="B73" s="51"/>
-      <c r="C73" s="52"/>
+      <c r="B73" s="57"/>
+      <c r="C73" s="58"/>
       <c r="D73" s="24" t="s">
         <v>222</v>
       </c>
       <c r="E73" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="F73" s="60"/>
-      <c r="G73" s="60"/>
-      <c r="H73" s="60"/>
-      <c r="I73" s="62"/>
-      <c r="J73" s="61"/>
-      <c r="K73" s="58"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
+      <c r="H73" s="66"/>
+      <c r="I73" s="68"/>
+      <c r="J73" s="67"/>
+      <c r="K73" s="64"/>
       <c r="L73" s="50"/>
-      <c r="M73" s="59"/>
+      <c r="M73" s="65"/>
     </row>
   </sheetData>
   <autoFilter ref="F5:M73"/>
@@ -3870,9 +3902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3884,7 +3914,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="32" t="s">
         <v>29</v>
       </c>
@@ -3899,11 +3929,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="69" t="s">
         <v>279</v>
       </c>
       <c r="E5" s="39" t="s">
@@ -3916,11 +3946,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="D6" s="64"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="36" t="s">
         <v>278</v>
       </c>
@@ -3931,11 +3961,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="D7" s="64"/>
+      <c r="D7" s="70"/>
       <c r="E7" s="36" t="s">
         <v>277</v>
       </c>
@@ -3946,11 +3976,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="64"/>
+      <c r="D8" s="70"/>
       <c r="E8" s="36" t="s">
         <v>239</v>
       </c>
@@ -3961,8 +3991,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="64"/>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="70"/>
       <c r="E9" s="36" t="s">
         <v>276</v>
       </c>
@@ -3973,8 +4003,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="64"/>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="70"/>
       <c r="E10" s="36" t="s">
         <v>275</v>
       </c>
@@ -3984,21 +4014,24 @@
       <c r="G10" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="64"/>
+      <c r="H10" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="70"/>
       <c r="E11" s="36" t="s">
         <v>274</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>29</v>
+        <v>233</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="65"/>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="71"/>
       <c r="E12" s="36" t="s">
         <v>273</v>
       </c>
@@ -4009,8 +4042,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="66" t="s">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="72" t="s">
         <v>272</v>
       </c>
       <c r="E13" s="38" t="s">
@@ -4023,20 +4056,20 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="67"/>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="73"/>
       <c r="E14" s="38" t="s">
         <v>234</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="67"/>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="73"/>
       <c r="E15" s="38" t="s">
         <v>271</v>
       </c>
@@ -4047,8 +4080,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D16" s="67"/>
+    <row r="16" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D16" s="73"/>
       <c r="E16" s="37" t="s">
         <v>270</v>
       </c>
@@ -4059,30 +4092,32 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D17" s="67"/>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D17" s="73"/>
       <c r="E17" s="37" t="s">
         <v>269</v>
       </c>
       <c r="F17" s="29" t="s">
-        <v>29</v>
+        <v>233</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="68"/>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D18" s="74"/>
       <c r="E18" s="37" t="s">
         <v>268</v>
       </c>
-      <c r="F18" s="29"/>
+      <c r="F18" s="29" t="s">
+        <v>233</v>
+      </c>
       <c r="G18" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="63" t="s">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D19" s="69" t="s">
         <v>267</v>
       </c>
       <c r="E19" s="36" t="s">
@@ -4095,20 +4130,23 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="64"/>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D20" s="70"/>
       <c r="E20" s="36" t="s">
         <v>266</v>
       </c>
       <c r="F20" s="29" t="s">
-        <v>233</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="64"/>
+        <v>235</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D21" s="70"/>
       <c r="E21" s="36" t="s">
         <v>265</v>
       </c>
@@ -4119,20 +4157,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D22" s="65"/>
+    <row r="22" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D22" s="71"/>
       <c r="E22" s="36" t="s">
         <v>264</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>29</v>
+        <v>233</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D23" s="66" t="s">
+    <row r="23" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D23" s="72" t="s">
         <v>263</v>
       </c>
       <c r="E23" s="37" t="s">
@@ -4145,44 +4183,44 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="67"/>
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="73"/>
       <c r="E24" s="37" t="s">
         <v>261</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>233</v>
+        <v>30</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D25" s="67"/>
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="73"/>
       <c r="E25" s="37" t="s">
         <v>260</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>244</v>
+        <v>30</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="68"/>
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="74"/>
       <c r="E26" s="37" t="s">
         <v>259</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>233</v>
+        <v>29</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="63" t="s">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="69" t="s">
         <v>258</v>
       </c>
       <c r="E27" s="36" t="s">
@@ -4191,24 +4229,27 @@
       <c r="F27" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="64"/>
+      <c r="G27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="70"/>
       <c r="E28" s="36" t="s">
         <v>256</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="65"/>
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="71"/>
       <c r="E29" s="36" t="s">
         <v>255</v>
       </c>
@@ -4219,62 +4260,68 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="69" t="s">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="75" t="s">
         <v>254</v>
       </c>
       <c r="E30" s="35" t="s">
         <v>253</v>
       </c>
-      <c r="F30" s="29"/>
+      <c r="F30" s="29" t="s">
+        <v>29</v>
+      </c>
       <c r="G30" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="69"/>
+    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D31" s="75"/>
       <c r="E31" s="35" t="s">
         <v>252</v>
       </c>
-      <c r="F31" s="29"/>
+      <c r="F31" s="29" t="s">
+        <v>30</v>
+      </c>
       <c r="G31" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D32" s="69"/>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D32" s="75"/>
       <c r="E32" s="35" t="s">
         <v>251</v>
       </c>
-      <c r="F32" s="29"/>
+      <c r="F32" s="29" t="s">
+        <v>30</v>
+      </c>
       <c r="G32" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D33" s="69"/>
+      <c r="D33" s="75"/>
       <c r="E33" s="35" t="s">
         <v>250</v>
       </c>
-      <c r="F33" s="29"/>
+      <c r="F33" s="29" t="s">
+        <v>29</v>
+      </c>
       <c r="G33" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="69"/>
+      <c r="D34" s="75"/>
       <c r="E34" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="F34" s="29" t="s">
-        <v>235</v>
-      </c>
+      <c r="F34" s="29"/>
       <c r="G34" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D35" s="63" t="s">
+      <c r="D35" s="69" t="s">
         <v>248</v>
       </c>
       <c r="E35" s="34" t="s">
@@ -4288,19 +4335,19 @@
       </c>
     </row>
     <row r="36" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D36" s="64"/>
+      <c r="D36" s="70"/>
       <c r="E36" s="30" t="s">
         <v>246</v>
       </c>
       <c r="F36" s="33" t="s">
         <v>227</v>
       </c>
-      <c r="G36" s="5" t="s">
-        <v>27</v>
+      <c r="G36" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D37" s="64"/>
+      <c r="D37" s="70"/>
       <c r="E37" s="31" t="s">
         <v>245</v>
       </c>
@@ -4312,31 +4359,31 @@
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D38" s="64"/>
+      <c r="D38" s="70"/>
       <c r="E38" s="31" t="s">
         <v>243</v>
       </c>
       <c r="F38" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="G38" s="5" t="s">
-        <v>27</v>
+      <c r="G38" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D39" s="64"/>
+      <c r="D39" s="70"/>
       <c r="E39" s="31" t="s">
         <v>242</v>
       </c>
       <c r="F39" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="G39" s="5" t="s">
-        <v>27</v>
+      <c r="G39" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D40" s="64"/>
+      <c r="D40" s="70"/>
       <c r="E40" s="28" t="s">
         <v>241</v>
       </c>
@@ -4348,7 +4395,7 @@
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D41" s="64"/>
+      <c r="D41" s="70"/>
       <c r="E41" s="28" t="s">
         <v>240</v>
       </c>
@@ -4360,7 +4407,7 @@
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D42" s="64"/>
+      <c r="D42" s="70"/>
       <c r="E42" s="28" t="s">
         <v>239</v>
       </c>
@@ -4372,7 +4419,7 @@
       </c>
     </row>
     <row r="43" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D43" s="64"/>
+      <c r="D43" s="70"/>
       <c r="E43" s="28" t="s">
         <v>238</v>
       </c>
@@ -4384,7 +4431,7 @@
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D44" s="64"/>
+      <c r="D44" s="70"/>
       <c r="E44" s="28" t="s">
         <v>236</v>
       </c>
@@ -4397,7 +4444,7 @@
       </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D45" s="64"/>
+      <c r="D45" s="70"/>
       <c r="E45" s="30" t="s">
         <v>46</v>
       </c>
@@ -4415,22 +4462,25 @@
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D46" s="64"/>
+      <c r="D46" s="70"/>
       <c r="E46" s="31" t="s">
         <v>234</v>
       </c>
       <c r="F46" s="29" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>27</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="I46" s="32" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D47" s="64"/>
+      <c r="D47" s="70"/>
       <c r="E47" s="31" t="s">
         <v>232</v>
       </c>
@@ -4441,20 +4491,20 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D48" s="64"/>
+    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D48" s="70"/>
       <c r="E48" s="30" t="s">
         <v>231</v>
       </c>
       <c r="F48" s="27" t="s">
-        <v>230</v>
+        <v>29</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" s="64"/>
+      <c r="D49" s="70"/>
       <c r="E49" s="30" t="s">
         <v>229</v>
       </c>
@@ -4466,7 +4516,7 @@
       </c>
     </row>
     <row r="50" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D50" s="65"/>
+      <c r="D50" s="71"/>
       <c r="E50" s="28" t="s">
         <v>228</v>
       </c>
@@ -4507,7 +4557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4552,7 +4602,7 @@
       </c>
       <c r="K5" s="42">
         <f>COUNTIF(DOC!G4:G49,"Done")</f>
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -4575,7 +4625,7 @@
       </c>
       <c r="K6" s="44">
         <f>COUNTIF(DOC!G4:G49,"In Progress")</f>
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Doc]_Commit update class design
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -1241,6 +1241,21 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1253,9 +1268,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1264,18 +1276,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1681,12 +1681,12 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1700,7 +1700,7 @@
       <c r="B7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="58" t="s">
         <v>118</v>
       </c>
       <c r="D7" s="24" t="s">
@@ -1736,7 +1736,7 @@
       <c r="B8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="61"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="24" t="s">
         <v>8</v>
       </c>
@@ -1767,12 +1767,12 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1786,7 +1786,7 @@
       <c r="B10" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="58" t="s">
         <v>121</v>
       </c>
       <c r="D10" s="24" t="s">
@@ -1824,7 +1824,7 @@
       <c r="B11" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="61"/>
+      <c r="C11" s="58"/>
       <c r="D11" s="24" t="s">
         <v>6</v>
       </c>
@@ -1860,7 +1860,7 @@
       <c r="B12" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="61"/>
+      <c r="C12" s="58"/>
       <c r="D12" s="24" t="s">
         <v>123</v>
       </c>
@@ -1894,7 +1894,7 @@
       <c r="B13" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="61"/>
+      <c r="C13" s="58"/>
       <c r="D13" s="24" t="s">
         <v>125</v>
       </c>
@@ -1926,7 +1926,7 @@
       <c r="B14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="61"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="24" t="s">
         <v>126</v>
       </c>
@@ -1958,7 +1958,7 @@
       <c r="B15" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="58" t="s">
         <v>128</v>
       </c>
       <c r="D15" s="24" t="s">
@@ -1994,7 +1994,7 @@
       <c r="B16" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="61"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="25" t="s">
         <v>130</v>
       </c>
@@ -2026,7 +2026,7 @@
       <c r="B17" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="61"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="24" t="s">
         <v>132</v>
       </c>
@@ -2058,7 +2058,7 @@
       <c r="B18" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="61"/>
+      <c r="C18" s="58"/>
       <c r="D18" s="24" t="s">
         <v>134</v>
       </c>
@@ -2090,7 +2090,7 @@
       <c r="B19" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="61"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="24" t="s">
         <v>48</v>
       </c>
@@ -2122,7 +2122,7 @@
       <c r="B20" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="61"/>
+      <c r="C20" s="58"/>
       <c r="D20" s="24" t="s">
         <v>9</v>
       </c>
@@ -2154,7 +2154,7 @@
       <c r="B21" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="61"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="24" t="s">
         <v>137</v>
       </c>
@@ -2186,7 +2186,7 @@
       <c r="B22" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="61" t="s">
+      <c r="C22" s="58" t="s">
         <v>139</v>
       </c>
       <c r="D22" s="24" t="s">
@@ -2222,7 +2222,7 @@
       <c r="B23" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="61"/>
+      <c r="C23" s="58"/>
       <c r="D23" s="52" t="s">
         <v>142</v>
       </c>
@@ -2254,7 +2254,7 @@
       <c r="B24" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="61"/>
+      <c r="C24" s="58"/>
       <c r="D24" s="24" t="s">
         <v>144</v>
       </c>
@@ -2286,7 +2286,7 @@
       <c r="B25" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="61"/>
+      <c r="C25" s="58"/>
       <c r="D25" s="24" t="s">
         <v>10</v>
       </c>
@@ -2320,7 +2320,7 @@
       <c r="B26" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="61"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="24" t="s">
         <v>147</v>
       </c>
@@ -2354,7 +2354,7 @@
       <c r="B27" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="61"/>
+      <c r="C27" s="58"/>
       <c r="D27" s="24" t="s">
         <v>11</v>
       </c>
@@ -2386,7 +2386,7 @@
       <c r="B28" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="61"/>
+      <c r="C28" s="58"/>
       <c r="D28" s="25" t="s">
         <v>150</v>
       </c>
@@ -2418,7 +2418,7 @@
       <c r="B29" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="59" t="s">
         <v>152</v>
       </c>
       <c r="D29" s="24" t="s">
@@ -2454,7 +2454,7 @@
       <c r="B30" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="67"/>
+      <c r="C30" s="60"/>
       <c r="D30" s="24" t="s">
         <v>154</v>
       </c>
@@ -2490,7 +2490,7 @@
       <c r="B31" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="67"/>
+      <c r="C31" s="60"/>
       <c r="D31" s="24" t="s">
         <v>155</v>
       </c>
@@ -2522,7 +2522,7 @@
       <c r="B32" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="67"/>
+      <c r="C32" s="60"/>
       <c r="D32" s="24" t="s">
         <v>156</v>
       </c>
@@ -2558,7 +2558,7 @@
       <c r="B33" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="67"/>
+      <c r="C33" s="60"/>
       <c r="D33" s="24" t="s">
         <v>158</v>
       </c>
@@ -2592,7 +2592,7 @@
       <c r="B34" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="67"/>
+      <c r="C34" s="60"/>
       <c r="D34" s="24" t="s">
         <v>160</v>
       </c>
@@ -2628,7 +2628,7 @@
       <c r="B35" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="67"/>
+      <c r="C35" s="60"/>
       <c r="D35" s="24" t="s">
         <v>162</v>
       </c>
@@ -2664,7 +2664,7 @@
       <c r="B36" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="67"/>
+      <c r="C36" s="60"/>
       <c r="D36" s="25" t="s">
         <v>164</v>
       </c>
@@ -2696,7 +2696,7 @@
       <c r="B37" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="67"/>
+      <c r="C37" s="60"/>
       <c r="D37" s="25" t="s">
         <v>166</v>
       </c>
@@ -2726,7 +2726,7 @@
       <c r="B38" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="67"/>
+      <c r="C38" s="60"/>
       <c r="D38" s="25" t="s">
         <v>167</v>
       </c>
@@ -2758,7 +2758,7 @@
       <c r="B39" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="67"/>
+      <c r="C39" s="60"/>
       <c r="D39" s="25" t="s">
         <v>169</v>
       </c>
@@ -2790,7 +2790,7 @@
       <c r="B40" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="67"/>
+      <c r="C40" s="60"/>
       <c r="D40" s="25" t="s">
         <v>116</v>
       </c>
@@ -2820,7 +2820,7 @@
       <c r="B41" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="68"/>
+      <c r="C41" s="61"/>
       <c r="D41" s="25" t="s">
         <v>171</v>
       </c>
@@ -2850,7 +2850,7 @@
       <c r="B42" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="61" t="s">
+      <c r="C42" s="58" t="s">
         <v>172</v>
       </c>
       <c r="D42" s="24" t="s">
@@ -2888,7 +2888,7 @@
       <c r="B43" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="61"/>
+      <c r="C43" s="58"/>
       <c r="D43" s="24" t="s">
         <v>117</v>
       </c>
@@ -2920,7 +2920,7 @@
       <c r="B44" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="61"/>
+      <c r="C44" s="58"/>
       <c r="D44" s="24" t="s">
         <v>175</v>
       </c>
@@ -2952,7 +2952,7 @@
       <c r="B45" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="61"/>
+      <c r="C45" s="58"/>
       <c r="D45" s="25" t="s">
         <v>177</v>
       </c>
@@ -2984,7 +2984,7 @@
       <c r="B46" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="61"/>
+      <c r="C46" s="58"/>
       <c r="D46" s="24" t="s">
         <v>178</v>
       </c>
@@ -3013,12 +3013,12 @@
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="65" t="s">
+      <c r="B47" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="65"/>
-      <c r="D47" s="65"/>
-      <c r="E47" s="65"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -3032,7 +3032,7 @@
       <c r="B48" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="61" t="s">
+      <c r="C48" s="58" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="25" t="s">
@@ -3064,7 +3064,7 @@
       <c r="B49" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="61"/>
+      <c r="C49" s="58"/>
       <c r="D49" s="24" t="s">
         <v>17</v>
       </c>
@@ -3094,7 +3094,7 @@
       <c r="B50" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="61"/>
+      <c r="C50" s="58"/>
       <c r="D50" s="24" t="s">
         <v>18</v>
       </c>
@@ -3124,7 +3124,7 @@
       <c r="B51" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="61"/>
+      <c r="C51" s="58"/>
       <c r="D51" s="24" t="s">
         <v>182</v>
       </c>
@@ -3156,7 +3156,7 @@
       <c r="B52" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="61"/>
+      <c r="C52" s="58"/>
       <c r="D52" s="24" t="s">
         <v>183</v>
       </c>
@@ -3186,7 +3186,7 @@
       <c r="B53" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="61"/>
+      <c r="C53" s="58"/>
       <c r="D53" s="24" t="s">
         <v>184</v>
       </c>
@@ -3218,7 +3218,7 @@
       <c r="B54" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="61" t="s">
+      <c r="C54" s="58" t="s">
         <v>54</v>
       </c>
       <c r="D54" s="24" t="s">
@@ -3254,7 +3254,7 @@
       <c r="B55" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="61"/>
+      <c r="C55" s="58"/>
       <c r="D55" s="24" t="s">
         <v>44</v>
       </c>
@@ -3288,7 +3288,7 @@
       <c r="B56" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="61"/>
+      <c r="C56" s="58"/>
       <c r="D56" s="24" t="s">
         <v>187</v>
       </c>
@@ -3320,7 +3320,7 @@
       <c r="B57" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="61" t="s">
+      <c r="C57" s="58" t="s">
         <v>55</v>
       </c>
       <c r="D57" s="24" t="s">
@@ -3358,7 +3358,7 @@
       <c r="B58" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="61"/>
+      <c r="C58" s="58"/>
       <c r="D58" s="24" t="s">
         <v>190</v>
       </c>
@@ -3388,7 +3388,7 @@
       <c r="B59" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C59" s="61"/>
+      <c r="C59" s="58"/>
       <c r="D59" s="24" t="s">
         <v>192</v>
       </c>
@@ -3420,7 +3420,7 @@
       <c r="B60" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="61"/>
+      <c r="C60" s="58"/>
       <c r="D60" s="24" t="s">
         <v>19</v>
       </c>
@@ -3456,7 +3456,7 @@
       <c r="B61" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C61" s="61"/>
+      <c r="C61" s="58"/>
       <c r="D61" s="24" t="s">
         <v>195</v>
       </c>
@@ -3490,7 +3490,7 @@
       <c r="B62" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="61"/>
+      <c r="C62" s="58"/>
       <c r="D62" s="24" t="s">
         <v>196</v>
       </c>
@@ -3526,7 +3526,7 @@
       <c r="B63" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="C63" s="61" t="s">
+      <c r="C63" s="58" t="s">
         <v>57</v>
       </c>
       <c r="D63" s="24" t="s">
@@ -3564,7 +3564,7 @@
       <c r="B64" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="C64" s="61"/>
+      <c r="C64" s="58"/>
       <c r="D64" s="24" t="s">
         <v>200</v>
       </c>
@@ -3600,7 +3600,7 @@
       <c r="B65" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="C65" s="61"/>
+      <c r="C65" s="58"/>
       <c r="D65" s="24" t="s">
         <v>203</v>
       </c>
@@ -3632,7 +3632,7 @@
       <c r="B66" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="C66" s="61"/>
+      <c r="C66" s="58"/>
       <c r="D66" s="24" t="s">
         <v>206</v>
       </c>
@@ -3662,7 +3662,7 @@
       <c r="B67" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="C67" s="61" t="s">
+      <c r="C67" s="58" t="s">
         <v>58</v>
       </c>
       <c r="D67" s="24" t="s">
@@ -3700,7 +3700,7 @@
       <c r="B68" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="C68" s="61"/>
+      <c r="C68" s="58"/>
       <c r="D68" s="24" t="s">
         <v>211</v>
       </c>
@@ -3734,7 +3734,7 @@
       <c r="B69" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C69" s="61"/>
+      <c r="C69" s="58"/>
       <c r="D69" s="24" t="s">
         <v>214</v>
       </c>
@@ -3767,10 +3767,10 @@
       </c>
     </row>
     <row r="70" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B70" s="65" t="s">
+      <c r="B70" s="57" t="s">
         <v>215</v>
       </c>
-      <c r="C70" s="61" t="s">
+      <c r="C70" s="58" t="s">
         <v>59</v>
       </c>
       <c r="D70" s="24" t="s">
@@ -3779,96 +3779,83 @@
       <c r="E70" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="F70" s="62" t="s">
+      <c r="F70" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="G70" s="62"/>
-      <c r="H70" s="62"/>
-      <c r="I70" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="J70" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="K70" s="57" t="s">
+      <c r="G70" s="66"/>
+      <c r="H70" s="66"/>
+      <c r="I70" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="J70" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="K70" s="62" t="s">
         <v>28</v>
       </c>
       <c r="L70" s="48"/>
-      <c r="M70" s="60" t="s">
+      <c r="M70" s="65" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="71" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B71" s="65"/>
-      <c r="C71" s="61"/>
+      <c r="B71" s="57"/>
+      <c r="C71" s="58"/>
       <c r="D71" s="24" t="s">
         <v>218</v>
       </c>
       <c r="E71" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="F71" s="62"/>
-      <c r="G71" s="62"/>
-      <c r="H71" s="62"/>
-      <c r="I71" s="64"/>
-      <c r="J71" s="63"/>
-      <c r="K71" s="58"/>
+      <c r="F71" s="66"/>
+      <c r="G71" s="66"/>
+      <c r="H71" s="66"/>
+      <c r="I71" s="68"/>
+      <c r="J71" s="67"/>
+      <c r="K71" s="63"/>
       <c r="L71" s="49"/>
-      <c r="M71" s="60"/>
+      <c r="M71" s="65"/>
     </row>
     <row r="72" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B72" s="65"/>
-      <c r="C72" s="61"/>
+      <c r="B72" s="57"/>
+      <c r="C72" s="58"/>
       <c r="D72" s="24" t="s">
         <v>220</v>
       </c>
       <c r="E72" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="F72" s="62"/>
-      <c r="G72" s="62"/>
-      <c r="H72" s="62"/>
-      <c r="I72" s="64"/>
-      <c r="J72" s="63"/>
-      <c r="K72" s="58"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
+      <c r="H72" s="66"/>
+      <c r="I72" s="68"/>
+      <c r="J72" s="67"/>
+      <c r="K72" s="63"/>
       <c r="L72" s="49"/>
-      <c r="M72" s="60"/>
+      <c r="M72" s="65"/>
     </row>
     <row r="73" spans="2:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="B73" s="65"/>
-      <c r="C73" s="61"/>
+      <c r="B73" s="57"/>
+      <c r="C73" s="58"/>
       <c r="D73" s="24" t="s">
         <v>222</v>
       </c>
       <c r="E73" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="F73" s="62"/>
-      <c r="G73" s="62"/>
-      <c r="H73" s="62"/>
-      <c r="I73" s="64"/>
-      <c r="J73" s="63"/>
-      <c r="K73" s="59"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
+      <c r="H73" s="66"/>
+      <c r="I73" s="68"/>
+      <c r="J73" s="67"/>
+      <c r="K73" s="64"/>
       <c r="L73" s="50"/>
-      <c r="M73" s="60"/>
+      <c r="M73" s="65"/>
     </row>
   </sheetData>
   <autoFilter ref="F5:M73"/>
   <dataConsolidate/>
   <mergeCells count="23">
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C29:C41"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="C48:C53"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C57:C62"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="C15:C21"/>
     <mergeCell ref="K70:K73"/>
     <mergeCell ref="M70:M73"/>
     <mergeCell ref="C22:C28"/>
@@ -3879,6 +3866,19 @@
     <mergeCell ref="H70:H73"/>
     <mergeCell ref="I70:I73"/>
     <mergeCell ref="J70:J73"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="C15:C21"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C29:C41"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C62"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:J73 M7:M73 K7:L70">
@@ -3990,8 +3990,8 @@
       <c r="F9" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>27</v>
+      <c r="G9" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -4584,7 +4584,7 @@
       </c>
       <c r="K5" s="42">
         <f>COUNTIF(DOC!G4:G49,"Done")</f>
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -4607,7 +4607,7 @@
       </c>
       <c r="K6" s="44">
         <f>COUNTIF(DOC!G4:G49,"In Progress")</f>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Doc]_Update file trong report
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -13,13 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CODE-TC-SRS'!$F$5:$M$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DOC!$D$4:$I$50</definedName>
   </definedNames>
   <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="288">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -4334,13 +4335,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D37" s="70"/>
       <c r="E37" s="31" t="s">
         <v>245</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>27</v>
@@ -4423,7 +4424,9 @@
       <c r="E44" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="F44" s="29"/>
+      <c r="F44" s="29" t="s">
+        <v>235</v>
+      </c>
       <c r="G44" s="5" t="s">
         <v>27</v>
       </c>
@@ -4510,6 +4513,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D4:I50"/>
   <mergeCells count="7">
     <mergeCell ref="D35:D50"/>
     <mergeCell ref="D5:D12"/>

</xml_diff>

<commit_message>
[Doc]_Commit class design ( not done)
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ dự án_Coding, Design, TC, SRS.xlsx
@@ -1242,6 +1242,21 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1254,9 +1269,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1265,18 +1277,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1682,12 +1682,12 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1701,7 +1701,7 @@
       <c r="B7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="58" t="s">
         <v>118</v>
       </c>
       <c r="D7" s="24" t="s">
@@ -1737,7 +1737,7 @@
       <c r="B8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="61"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="24" t="s">
         <v>8</v>
       </c>
@@ -1768,12 +1768,12 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1787,7 +1787,7 @@
       <c r="B10" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="58" t="s">
         <v>121</v>
       </c>
       <c r="D10" s="24" t="s">
@@ -1825,7 +1825,7 @@
       <c r="B11" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="61"/>
+      <c r="C11" s="58"/>
       <c r="D11" s="24" t="s">
         <v>6</v>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="B12" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="61"/>
+      <c r="C12" s="58"/>
       <c r="D12" s="24" t="s">
         <v>123</v>
       </c>
@@ -1895,7 +1895,7 @@
       <c r="B13" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="61"/>
+      <c r="C13" s="58"/>
       <c r="D13" s="24" t="s">
         <v>125</v>
       </c>
@@ -1927,7 +1927,7 @@
       <c r="B14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="61"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="24" t="s">
         <v>126</v>
       </c>
@@ -1959,7 +1959,7 @@
       <c r="B15" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="58" t="s">
         <v>128</v>
       </c>
       <c r="D15" s="24" t="s">
@@ -1995,7 +1995,7 @@
       <c r="B16" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="61"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="25" t="s">
         <v>130</v>
       </c>
@@ -2027,7 +2027,7 @@
       <c r="B17" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="61"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="24" t="s">
         <v>132</v>
       </c>
@@ -2059,7 +2059,7 @@
       <c r="B18" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="61"/>
+      <c r="C18" s="58"/>
       <c r="D18" s="24" t="s">
         <v>134</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="B19" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="61"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="24" t="s">
         <v>48</v>
       </c>
@@ -2123,7 +2123,7 @@
       <c r="B20" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="61"/>
+      <c r="C20" s="58"/>
       <c r="D20" s="24" t="s">
         <v>9</v>
       </c>
@@ -2155,7 +2155,7 @@
       <c r="B21" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="61"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="24" t="s">
         <v>137</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="B22" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="61" t="s">
+      <c r="C22" s="58" t="s">
         <v>139</v>
       </c>
       <c r="D22" s="24" t="s">
@@ -2223,7 +2223,7 @@
       <c r="B23" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="61"/>
+      <c r="C23" s="58"/>
       <c r="D23" s="52" t="s">
         <v>142</v>
       </c>
@@ -2255,7 +2255,7 @@
       <c r="B24" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="61"/>
+      <c r="C24" s="58"/>
       <c r="D24" s="24" t="s">
         <v>144</v>
       </c>
@@ -2287,7 +2287,7 @@
       <c r="B25" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="61"/>
+      <c r="C25" s="58"/>
       <c r="D25" s="24" t="s">
         <v>10</v>
       </c>
@@ -2321,7 +2321,7 @@
       <c r="B26" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="61"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="24" t="s">
         <v>147</v>
       </c>
@@ -2355,7 +2355,7 @@
       <c r="B27" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="61"/>
+      <c r="C27" s="58"/>
       <c r="D27" s="24" t="s">
         <v>11</v>
       </c>
@@ -2387,7 +2387,7 @@
       <c r="B28" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="61"/>
+      <c r="C28" s="58"/>
       <c r="D28" s="25" t="s">
         <v>150</v>
       </c>
@@ -2419,7 +2419,7 @@
       <c r="B29" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="59" t="s">
         <v>152</v>
       </c>
       <c r="D29" s="24" t="s">
@@ -2455,7 +2455,7 @@
       <c r="B30" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="67"/>
+      <c r="C30" s="60"/>
       <c r="D30" s="24" t="s">
         <v>154</v>
       </c>
@@ -2491,7 +2491,7 @@
       <c r="B31" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="67"/>
+      <c r="C31" s="60"/>
       <c r="D31" s="24" t="s">
         <v>155</v>
       </c>
@@ -2523,7 +2523,7 @@
       <c r="B32" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="67"/>
+      <c r="C32" s="60"/>
       <c r="D32" s="24" t="s">
         <v>156</v>
       </c>
@@ -2559,7 +2559,7 @@
       <c r="B33" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="67"/>
+      <c r="C33" s="60"/>
       <c r="D33" s="24" t="s">
         <v>158</v>
       </c>
@@ -2593,7 +2593,7 @@
       <c r="B34" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="67"/>
+      <c r="C34" s="60"/>
       <c r="D34" s="24" t="s">
         <v>160</v>
       </c>
@@ -2629,7 +2629,7 @@
       <c r="B35" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="67"/>
+      <c r="C35" s="60"/>
       <c r="D35" s="24" t="s">
         <v>162</v>
       </c>
@@ -2665,7 +2665,7 @@
       <c r="B36" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="67"/>
+      <c r="C36" s="60"/>
       <c r="D36" s="25" t="s">
         <v>164</v>
       </c>
@@ -2697,7 +2697,7 @@
       <c r="B37" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="67"/>
+      <c r="C37" s="60"/>
       <c r="D37" s="25" t="s">
         <v>166</v>
       </c>
@@ -2727,7 +2727,7 @@
       <c r="B38" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="67"/>
+      <c r="C38" s="60"/>
       <c r="D38" s="25" t="s">
         <v>167</v>
       </c>
@@ -2759,7 +2759,7 @@
       <c r="B39" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="67"/>
+      <c r="C39" s="60"/>
       <c r="D39" s="25" t="s">
         <v>169</v>
       </c>
@@ -2791,7 +2791,7 @@
       <c r="B40" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="67"/>
+      <c r="C40" s="60"/>
       <c r="D40" s="25" t="s">
         <v>116</v>
       </c>
@@ -2821,7 +2821,7 @@
       <c r="B41" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="68"/>
+      <c r="C41" s="61"/>
       <c r="D41" s="25" t="s">
         <v>171</v>
       </c>
@@ -2851,7 +2851,7 @@
       <c r="B42" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="61" t="s">
+      <c r="C42" s="58" t="s">
         <v>172</v>
       </c>
       <c r="D42" s="24" t="s">
@@ -2889,7 +2889,7 @@
       <c r="B43" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="61"/>
+      <c r="C43" s="58"/>
       <c r="D43" s="24" t="s">
         <v>117</v>
       </c>
@@ -2921,7 +2921,7 @@
       <c r="B44" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="61"/>
+      <c r="C44" s="58"/>
       <c r="D44" s="24" t="s">
         <v>175</v>
       </c>
@@ -2953,7 +2953,7 @@
       <c r="B45" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="61"/>
+      <c r="C45" s="58"/>
       <c r="D45" s="25" t="s">
         <v>177</v>
       </c>
@@ -2985,7 +2985,7 @@
       <c r="B46" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="61"/>
+      <c r="C46" s="58"/>
       <c r="D46" s="24" t="s">
         <v>178</v>
       </c>
@@ -3014,12 +3014,12 @@
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="65" t="s">
+      <c r="B47" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="65"/>
-      <c r="D47" s="65"/>
-      <c r="E47" s="65"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -3033,7 +3033,7 @@
       <c r="B48" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="61" t="s">
+      <c r="C48" s="58" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="25" t="s">
@@ -3065,7 +3065,7 @@
       <c r="B49" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="61"/>
+      <c r="C49" s="58"/>
       <c r="D49" s="24" t="s">
         <v>17</v>
       </c>
@@ -3095,7 +3095,7 @@
       <c r="B50" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="61"/>
+      <c r="C50" s="58"/>
       <c r="D50" s="24" t="s">
         <v>18</v>
       </c>
@@ -3125,7 +3125,7 @@
       <c r="B51" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="61"/>
+      <c r="C51" s="58"/>
       <c r="D51" s="24" t="s">
         <v>182</v>
       </c>
@@ -3157,7 +3157,7 @@
       <c r="B52" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="61"/>
+      <c r="C52" s="58"/>
       <c r="D52" s="24" t="s">
         <v>183</v>
       </c>
@@ -3187,7 +3187,7 @@
       <c r="B53" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="61"/>
+      <c r="C53" s="58"/>
       <c r="D53" s="24" t="s">
         <v>184</v>
       </c>
@@ -3219,7 +3219,7 @@
       <c r="B54" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="61" t="s">
+      <c r="C54" s="58" t="s">
         <v>54</v>
       </c>
       <c r="D54" s="24" t="s">
@@ -3255,7 +3255,7 @@
       <c r="B55" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="61"/>
+      <c r="C55" s="58"/>
       <c r="D55" s="24" t="s">
         <v>44</v>
       </c>
@@ -3289,7 +3289,7 @@
       <c r="B56" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="61"/>
+      <c r="C56" s="58"/>
       <c r="D56" s="24" t="s">
         <v>187</v>
       </c>
@@ -3321,7 +3321,7 @@
       <c r="B57" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="61" t="s">
+      <c r="C57" s="58" t="s">
         <v>55</v>
       </c>
       <c r="D57" s="24" t="s">
@@ -3359,7 +3359,7 @@
       <c r="B58" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="61"/>
+      <c r="C58" s="58"/>
       <c r="D58" s="24" t="s">
         <v>190</v>
       </c>
@@ -3389,7 +3389,7 @@
       <c r="B59" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C59" s="61"/>
+      <c r="C59" s="58"/>
       <c r="D59" s="24" t="s">
         <v>192</v>
       </c>
@@ -3421,7 +3421,7 @@
       <c r="B60" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="61"/>
+      <c r="C60" s="58"/>
       <c r="D60" s="24" t="s">
         <v>19</v>
       </c>
@@ -3457,7 +3457,7 @@
       <c r="B61" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C61" s="61"/>
+      <c r="C61" s="58"/>
       <c r="D61" s="24" t="s">
         <v>195</v>
       </c>
@@ -3491,7 +3491,7 @@
       <c r="B62" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="61"/>
+      <c r="C62" s="58"/>
       <c r="D62" s="24" t="s">
         <v>196</v>
       </c>
@@ -3527,7 +3527,7 @@
       <c r="B63" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="C63" s="61" t="s">
+      <c r="C63" s="58" t="s">
         <v>57</v>
       </c>
       <c r="D63" s="24" t="s">
@@ -3565,7 +3565,7 @@
       <c r="B64" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="C64" s="61"/>
+      <c r="C64" s="58"/>
       <c r="D64" s="24" t="s">
         <v>200</v>
       </c>
@@ -3601,7 +3601,7 @@
       <c r="B65" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="C65" s="61"/>
+      <c r="C65" s="58"/>
       <c r="D65" s="24" t="s">
         <v>203</v>
       </c>
@@ -3633,7 +3633,7 @@
       <c r="B66" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="C66" s="61"/>
+      <c r="C66" s="58"/>
       <c r="D66" s="24" t="s">
         <v>206</v>
       </c>
@@ -3663,7 +3663,7 @@
       <c r="B67" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="C67" s="61" t="s">
+      <c r="C67" s="58" t="s">
         <v>58</v>
       </c>
       <c r="D67" s="24" t="s">
@@ -3701,7 +3701,7 @@
       <c r="B68" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="C68" s="61"/>
+      <c r="C68" s="58"/>
       <c r="D68" s="24" t="s">
         <v>211</v>
       </c>
@@ -3735,7 +3735,7 @@
       <c r="B69" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C69" s="61"/>
+      <c r="C69" s="58"/>
       <c r="D69" s="24" t="s">
         <v>214</v>
       </c>
@@ -3768,10 +3768,10 @@
       </c>
     </row>
     <row r="70" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B70" s="65" t="s">
+      <c r="B70" s="57" t="s">
         <v>215</v>
       </c>
-      <c r="C70" s="61" t="s">
+      <c r="C70" s="58" t="s">
         <v>59</v>
       </c>
       <c r="D70" s="24" t="s">
@@ -3780,96 +3780,83 @@
       <c r="E70" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="F70" s="62" t="s">
+      <c r="F70" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="G70" s="62"/>
-      <c r="H70" s="62"/>
-      <c r="I70" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="J70" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="K70" s="57" t="s">
+      <c r="G70" s="66"/>
+      <c r="H70" s="66"/>
+      <c r="I70" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="J70" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="K70" s="62" t="s">
         <v>28</v>
       </c>
       <c r="L70" s="48"/>
-      <c r="M70" s="60" t="s">
+      <c r="M70" s="65" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="71" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B71" s="65"/>
-      <c r="C71" s="61"/>
+      <c r="B71" s="57"/>
+      <c r="C71" s="58"/>
       <c r="D71" s="24" t="s">
         <v>218</v>
       </c>
       <c r="E71" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="F71" s="62"/>
-      <c r="G71" s="62"/>
-      <c r="H71" s="62"/>
-      <c r="I71" s="64"/>
-      <c r="J71" s="63"/>
-      <c r="K71" s="58"/>
+      <c r="F71" s="66"/>
+      <c r="G71" s="66"/>
+      <c r="H71" s="66"/>
+      <c r="I71" s="68"/>
+      <c r="J71" s="67"/>
+      <c r="K71" s="63"/>
       <c r="L71" s="49"/>
-      <c r="M71" s="60"/>
+      <c r="M71" s="65"/>
     </row>
     <row r="72" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B72" s="65"/>
-      <c r="C72" s="61"/>
+      <c r="B72" s="57"/>
+      <c r="C72" s="58"/>
       <c r="D72" s="24" t="s">
         <v>220</v>
       </c>
       <c r="E72" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="F72" s="62"/>
-      <c r="G72" s="62"/>
-      <c r="H72" s="62"/>
-      <c r="I72" s="64"/>
-      <c r="J72" s="63"/>
-      <c r="K72" s="58"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
+      <c r="H72" s="66"/>
+      <c r="I72" s="68"/>
+      <c r="J72" s="67"/>
+      <c r="K72" s="63"/>
       <c r="L72" s="49"/>
-      <c r="M72" s="60"/>
+      <c r="M72" s="65"/>
     </row>
     <row r="73" spans="2:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="B73" s="65"/>
-      <c r="C73" s="61"/>
+      <c r="B73" s="57"/>
+      <c r="C73" s="58"/>
       <c r="D73" s="24" t="s">
         <v>222</v>
       </c>
       <c r="E73" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="F73" s="62"/>
-      <c r="G73" s="62"/>
-      <c r="H73" s="62"/>
-      <c r="I73" s="64"/>
-      <c r="J73" s="63"/>
-      <c r="K73" s="59"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
+      <c r="H73" s="66"/>
+      <c r="I73" s="68"/>
+      <c r="J73" s="67"/>
+      <c r="K73" s="64"/>
       <c r="L73" s="50"/>
-      <c r="M73" s="60"/>
+      <c r="M73" s="65"/>
     </row>
   </sheetData>
   <autoFilter ref="F5:M73"/>
   <dataConsolidate/>
   <mergeCells count="23">
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C29:C41"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="C48:C53"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C57:C62"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="C15:C21"/>
     <mergeCell ref="K70:K73"/>
     <mergeCell ref="M70:M73"/>
     <mergeCell ref="C22:C28"/>
@@ -3880,6 +3867,19 @@
     <mergeCell ref="H70:H73"/>
     <mergeCell ref="I70:I73"/>
     <mergeCell ref="J70:J73"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="C15:C21"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C29:C41"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C62"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:J73 M7:M73 K7:L70">
@@ -3894,9 +3894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4444,8 +4442,8 @@
       <c r="F45" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="G45" s="5" t="s">
-        <v>27</v>
+      <c r="G45" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="I45" s="32" t="s">
         <v>27</v>
@@ -4459,8 +4457,8 @@
       <c r="F46" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="G46" s="5" t="s">
-        <v>27</v>
+      <c r="G46" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="I46" s="32" t="s">
         <v>28</v>
@@ -4590,7 +4588,7 @@
       </c>
       <c r="K5" s="42">
         <f>COUNTIF(DOC!G4:G49,"Done")</f>
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -4613,7 +4611,7 @@
       </c>
       <c r="K6" s="44">
         <f>COUNTIF(DOC!G4:G49,"In Progress")</f>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>